<commit_message>
Push to new version
</commit_message>
<xml_diff>
--- a/analyses/3_primary_production_analysis.xlsx
+++ b/analyses/3_primary_production_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22340" tabRatio="902" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="902" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="1" r:id="rId1"/>
@@ -5028,7 +5028,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="357">
+  <cellXfs count="356">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -5479,7 +5479,6 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="25" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="10" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5636,6 +5635,12 @@
     <xf numFmtId="2" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5696,12 +5701,6 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2680">
     <cellStyle name="Comma" xfId="2206" builtinId="3"/>
@@ -8385,7 +8384,27 @@
     <cellStyle name="Percent" xfId="731" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="2521"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FFCCFFCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCFFCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -12539,11 +12558,11 @@
       <c r="E4" s="234"/>
     </row>
     <row r="5" spans="2:6" ht="29" customHeight="1">
-      <c r="B5" s="339" t="s">
+      <c r="B5" s="342" t="s">
         <v>336</v>
       </c>
-      <c r="C5" s="340"/>
-      <c r="D5" s="340"/>
+      <c r="C5" s="343"/>
+      <c r="D5" s="343"/>
       <c r="E5" s="234"/>
     </row>
     <row r="6" spans="2:6" ht="16" thickBot="1">
@@ -12551,24 +12570,24 @@
       <c r="C6" s="9"/>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="317" t="s">
+      <c r="B7" s="316" t="s">
         <v>332</v>
       </c>
-      <c r="C7" s="318"/>
-      <c r="D7" s="319"/>
-      <c r="E7" s="318"/>
-      <c r="F7" s="320" t="s">
+      <c r="C7" s="317"/>
+      <c r="D7" s="318"/>
+      <c r="E7" s="317"/>
+      <c r="F7" s="319" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" customHeight="1">
       <c r="B8" s="58"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="299"/>
-      <c r="E8" s="321" t="s">
+      <c r="D8" s="298"/>
+      <c r="E8" s="320" t="s">
         <v>422</v>
       </c>
-      <c r="F8" s="324" t="s">
+      <c r="F8" s="323" t="s">
         <v>425</v>
       </c>
     </row>
@@ -12579,9 +12598,9 @@
       <c r="C9" s="235" t="s">
         <v>333</v>
       </c>
-      <c r="D9" s="325"/>
-      <c r="E9" s="322"/>
-      <c r="F9" s="323" t="s">
+      <c r="D9" s="324"/>
+      <c r="E9" s="321"/>
+      <c r="F9" s="322" t="s">
         <v>423</v>
       </c>
     </row>
@@ -12590,7 +12609,7 @@
         <v>337</v>
       </c>
       <c r="C10" s="109"/>
-      <c r="D10" s="300"/>
+      <c r="D10" s="299"/>
       <c r="E10" s="9"/>
       <c r="F10" s="59"/>
     </row>
@@ -12599,17 +12618,17 @@
       <c r="C11" s="204" t="s">
         <v>239</v>
       </c>
-      <c r="D11" s="299"/>
+      <c r="D11" s="298"/>
       <c r="E11" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="F11" s="316"/>
+      <c r="F11" s="315"/>
     </row>
     <row r="12" spans="2:6" ht="16" thickBot="1">
       <c r="B12" s="62"/>
       <c r="C12" s="63"/>
-      <c r="D12" s="301"/>
-      <c r="E12" s="315"/>
+      <c r="D12" s="300"/>
+      <c r="E12" s="314"/>
       <c r="F12" s="64"/>
     </row>
   </sheetData>
@@ -12659,12 +12678,12 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="342" t="s">
+      <c r="B5" s="345" t="s">
         <v>389</v>
       </c>
-      <c r="C5" s="343"/>
-      <c r="D5" s="343"/>
-      <c r="E5" s="344"/>
+      <c r="C5" s="346"/>
+      <c r="D5" s="346"/>
+      <c r="E5" s="347"/>
     </row>
     <row r="6" spans="2:5" ht="16" thickBot="1">
       <c r="B6" s="9"/>
@@ -12696,7 +12715,7 @@
       <c r="D9" s="228" t="s">
         <v>266</v>
       </c>
-      <c r="E9" s="284" t="s">
+      <c r="E9" s="283" t="s">
         <v>267</v>
       </c>
     </row>
@@ -12707,7 +12726,7 @@
       </c>
       <c r="C10" s="215"/>
       <c r="D10" s="223"/>
-      <c r="E10" s="285"/>
+      <c r="E10" s="284"/>
     </row>
     <row r="11" spans="2:5" ht="15" customHeight="1">
       <c r="B11" s="218"/>
@@ -12718,7 +12737,7 @@
         <f>IF(ISNUMBER(Dashboard!E17),Dashboard!E17,"-")</f>
         <v>-</v>
       </c>
-      <c r="E11" s="286"/>
+      <c r="E11" s="285"/>
     </row>
     <row r="12" spans="2:5" ht="15" customHeight="1">
       <c r="B12" s="218"/>
@@ -12729,7 +12748,7 @@
         <f>IF(ISNUMBER(Dashboard!E18),Dashboard!E18,"-")</f>
         <v>-</v>
       </c>
-      <c r="E12" s="286"/>
+      <c r="E12" s="285"/>
     </row>
     <row r="13" spans="2:5" ht="15" customHeight="1">
       <c r="B13" s="219"/>
@@ -12740,7 +12759,7 @@
         <f>IF(ISNUMBER(Dashboard!E19),Dashboard!E19,"-")</f>
         <v>-</v>
       </c>
-      <c r="E13" s="286"/>
+      <c r="E13" s="285"/>
     </row>
     <row r="14" spans="2:5" ht="15" customHeight="1">
       <c r="B14" s="202"/>
@@ -12751,7 +12770,7 @@
         <f>IF(ISNUMBER(Dashboard!E20),Dashboard!E20,"-")</f>
         <v>-</v>
       </c>
-      <c r="E14" s="286"/>
+      <c r="E14" s="285"/>
     </row>
     <row r="15" spans="2:5" ht="15" customHeight="1">
       <c r="B15" s="202"/>
@@ -12762,13 +12781,13 @@
         <f>IF(ISNUMBER(Dashboard!E21),Dashboard!E21,"-")</f>
         <v>-</v>
       </c>
-      <c r="E15" s="286"/>
+      <c r="E15" s="285"/>
     </row>
     <row r="16" spans="2:5" ht="15" customHeight="1">
       <c r="B16" s="114"/>
       <c r="C16" s="216"/>
-      <c r="D16" s="283"/>
-      <c r="E16" s="286"/>
+      <c r="D16" s="282"/>
+      <c r="E16" s="285"/>
     </row>
     <row r="17" spans="2:5" ht="15" customHeight="1">
       <c r="B17" s="114"/>
@@ -12779,7 +12798,7 @@
         <f>IF(ISNUMBER(Dashboard!E23),Dashboard!E23,"-")</f>
         <v>0</v>
       </c>
-      <c r="E17" s="287" t="str">
+      <c r="E17" s="286" t="str">
         <f>IF(ISNUMBER(Dashboard!E36),Dashboard!E36,"-")</f>
         <v>-</v>
       </c>
@@ -12793,7 +12812,7 @@
         <f>IF(ISNUMBER(Dashboard!E24),Dashboard!E24,"-")</f>
         <v>0</v>
       </c>
-      <c r="E18" s="287" t="str">
+      <c r="E18" s="286" t="str">
         <f>IF(ISNUMBER(Dashboard!E37),Dashboard!E37,"-")</f>
         <v>-</v>
       </c>
@@ -12807,7 +12826,7 @@
         <f>IF(ISNUMBER(Dashboard!E25),Dashboard!E25,"-")</f>
         <v>-</v>
       </c>
-      <c r="E19" s="287" t="str">
+      <c r="E19" s="286" t="str">
         <f>IF(ISNUMBER(Dashboard!E38),Dashboard!E38,"-")</f>
         <v>-</v>
       </c>
@@ -12821,7 +12840,7 @@
         <f>IF(ISNUMBER(Dashboard!E26),Dashboard!E26,"-")</f>
         <v>0</v>
       </c>
-      <c r="E20" s="287" t="str">
+      <c r="E20" s="286" t="str">
         <f>IF(ISNUMBER(Dashboard!E39),Dashboard!E39,"-")</f>
         <v>-</v>
       </c>
@@ -12835,7 +12854,7 @@
         <f>IF(ISNUMBER(Dashboard!E27),Dashboard!E27,"-")</f>
         <v>0</v>
       </c>
-      <c r="E21" s="287" t="str">
+      <c r="E21" s="286" t="str">
         <f>IF(ISNUMBER(Dashboard!E40),Dashboard!E40,"-")</f>
         <v>-</v>
       </c>
@@ -12849,7 +12868,7 @@
         <f>IF(ISNUMBER(Dashboard!E28),Dashboard!E28,"-")</f>
         <v>-</v>
       </c>
-      <c r="E22" s="287" t="str">
+      <c r="E22" s="286" t="str">
         <f>IF(ISNUMBER(Dashboard!E41),Dashboard!E41,"-")</f>
         <v>-</v>
       </c>
@@ -12863,7 +12882,7 @@
         <f>IF(ISNUMBER(Dashboard!E29),Dashboard!E29,"-")</f>
         <v>-</v>
       </c>
-      <c r="E23" s="287" t="str">
+      <c r="E23" s="286" t="str">
         <f>IF(ISNUMBER(Dashboard!E42),Dashboard!E42,"-")</f>
         <v>-</v>
       </c>
@@ -12877,7 +12896,7 @@
         <f>IF(ISNUMBER(Dashboard!E30),Dashboard!E30,"-")</f>
         <v>-</v>
       </c>
-      <c r="E24" s="287" t="str">
+      <c r="E24" s="286" t="str">
         <f>IF(ISNUMBER(Dashboard!E43),Dashboard!E43,"-")</f>
         <v>-</v>
       </c>
@@ -12891,7 +12910,7 @@
         <f>IF(ISNUMBER(Dashboard!E31),Dashboard!E31,"-")</f>
         <v>-</v>
       </c>
-      <c r="E25" s="287" t="str">
+      <c r="E25" s="286" t="str">
         <f>IF(ISNUMBER(Dashboard!E44),Dashboard!E44,"-")</f>
         <v>-</v>
       </c>
@@ -12905,7 +12924,7 @@
         <f>IF(ISNUMBER(Dashboard!E32),Dashboard!E32,"-")</f>
         <v>-</v>
       </c>
-      <c r="E26" s="287" t="str">
+      <c r="E26" s="286" t="str">
         <f>IF(ISNUMBER(Dashboard!E45),Dashboard!E45,"-")</f>
         <v>-</v>
       </c>
@@ -12919,7 +12938,7 @@
         <f>IF(ISNUMBER(Dashboard!E33),Dashboard!E33,"-")</f>
         <v>-</v>
       </c>
-      <c r="E27" s="287" t="str">
+      <c r="E27" s="286" t="str">
         <f>IF(ISNUMBER(Dashboard!E46),Dashboard!E46,"-")</f>
         <v>-</v>
       </c>
@@ -12928,7 +12947,7 @@
       <c r="B28" s="99"/>
       <c r="C28" s="200"/>
       <c r="D28" s="225"/>
-      <c r="E28" s="288"/>
+      <c r="E28" s="287"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12981,12 +13000,12 @@
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="345" t="s">
+      <c r="B5" s="348" t="s">
         <v>240</v>
       </c>
-      <c r="C5" s="346"/>
-      <c r="D5" s="346"/>
-      <c r="E5" s="347"/>
+      <c r="C5" s="349"/>
+      <c r="D5" s="349"/>
+      <c r="E5" s="350"/>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="2:7" ht="16" thickBot="1"/>
@@ -13185,11 +13204,11 @@
         <v>340</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="302" t="e">
+      <c r="D23" s="301" t="e">
         <f>D21+D22</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E23" s="303"/>
+      <c r="E23" s="302"/>
       <c r="F23" s="15"/>
       <c r="G23" s="59" t="s">
         <v>291</v>
@@ -13250,12 +13269,12 @@
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="2:7" ht="30" customHeight="1">
-      <c r="B5" s="339" t="s">
+      <c r="B5" s="342" t="s">
         <v>401</v>
       </c>
-      <c r="C5" s="348"/>
-      <c r="D5" s="348"/>
-      <c r="E5" s="349"/>
+      <c r="C5" s="351"/>
+      <c r="D5" s="351"/>
+      <c r="E5" s="352"/>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="2:7" ht="16" thickBot="1"/>
@@ -13408,15 +13427,15 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:15" ht="30" customHeight="1">
-      <c r="B5" s="350" t="s">
+      <c r="B5" s="353" t="s">
         <v>393</v>
       </c>
-      <c r="C5" s="351"/>
-      <c r="D5" s="351"/>
-      <c r="E5" s="351"/>
-      <c r="F5" s="351"/>
-      <c r="G5" s="351"/>
-      <c r="H5" s="352"/>
+      <c r="C5" s="354"/>
+      <c r="D5" s="354"/>
+      <c r="E5" s="354"/>
+      <c r="F5" s="354"/>
+      <c r="G5" s="354"/>
+      <c r="H5" s="355"/>
     </row>
     <row r="6" spans="2:15" ht="16" thickBot="1"/>
     <row r="7" spans="2:15">
@@ -13424,7 +13443,7 @@
         <v>376</v>
       </c>
       <c r="C7" s="56"/>
-      <c r="D7" s="263"/>
+      <c r="D7" s="262"/>
       <c r="E7" s="56"/>
       <c r="F7" s="66"/>
       <c r="G7" s="66"/>
@@ -13441,243 +13460,243 @@
       <c r="B8" s="58"/>
       <c r="C8" s="9"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="264"/>
-      <c r="F8" s="264"/>
-      <c r="G8" s="264"/>
-      <c r="H8" s="264"/>
-      <c r="I8" s="264"/>
-      <c r="J8" s="264"/>
-      <c r="K8" s="264"/>
-      <c r="L8" s="264"/>
-      <c r="M8" s="264"/>
-      <c r="N8" s="264"/>
-      <c r="O8" s="265"/>
+      <c r="E8" s="263"/>
+      <c r="F8" s="263"/>
+      <c r="G8" s="263"/>
+      <c r="H8" s="263"/>
+      <c r="I8" s="263"/>
+      <c r="J8" s="263"/>
+      <c r="K8" s="263"/>
+      <c r="L8" s="263"/>
+      <c r="M8" s="263"/>
+      <c r="N8" s="263"/>
+      <c r="O8" s="264"/>
     </row>
     <row r="9" spans="2:15" ht="30">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="265" t="s">
         <v>303</v>
       </c>
-      <c r="C9" s="267"/>
-      <c r="D9" s="268"/>
-      <c r="E9" s="269" t="s">
+      <c r="C9" s="266"/>
+      <c r="D9" s="267"/>
+      <c r="E9" s="268" t="s">
         <v>377</v>
       </c>
-      <c r="F9" s="269" t="s">
+      <c r="F9" s="268" t="s">
         <v>381</v>
       </c>
-      <c r="G9" s="269" t="s">
+      <c r="G9" s="268" t="s">
         <v>378</v>
       </c>
-      <c r="H9" s="269" t="s">
+      <c r="H9" s="268" t="s">
         <v>379</v>
       </c>
-      <c r="I9" s="269" t="s">
+      <c r="I9" s="268" t="s">
         <v>383</v>
       </c>
-      <c r="J9" s="269" t="s">
+      <c r="J9" s="268" t="s">
         <v>384</v>
       </c>
-      <c r="K9" s="269" t="s">
+      <c r="K9" s="268" t="s">
         <v>392</v>
       </c>
-      <c r="L9" s="269" t="s">
+      <c r="L9" s="268" t="s">
         <v>385</v>
       </c>
-      <c r="M9" s="269" t="s">
+      <c r="M9" s="268" t="s">
         <v>386</v>
       </c>
-      <c r="N9" s="269" t="s">
+      <c r="N9" s="268" t="s">
         <v>387</v>
       </c>
-      <c r="O9" s="270" t="s">
+      <c r="O9" s="269" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="10" spans="2:15">
-      <c r="B10" s="271"/>
-      <c r="C10" s="272"/>
-      <c r="D10" s="273"/>
-      <c r="E10" s="274"/>
-      <c r="F10" s="274"/>
-      <c r="G10" s="274"/>
-      <c r="H10" s="274"/>
-      <c r="I10" s="274"/>
-      <c r="J10" s="274"/>
-      <c r="K10" s="274"/>
-      <c r="L10" s="274"/>
-      <c r="M10" s="274"/>
-      <c r="N10" s="274"/>
-      <c r="O10" s="275"/>
+      <c r="B10" s="270"/>
+      <c r="C10" s="271"/>
+      <c r="D10" s="272"/>
+      <c r="E10" s="273"/>
+      <c r="F10" s="273"/>
+      <c r="G10" s="273"/>
+      <c r="H10" s="273"/>
+      <c r="I10" s="273"/>
+      <c r="J10" s="273"/>
+      <c r="K10" s="273"/>
+      <c r="L10" s="273"/>
+      <c r="M10" s="273"/>
+      <c r="N10" s="273"/>
+      <c r="O10" s="274"/>
     </row>
     <row r="11" spans="2:15">
-      <c r="B11" s="271" t="s">
+      <c r="B11" s="270" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="276"/>
-      <c r="D11" s="277"/>
-      <c r="E11" s="278">
+      <c r="C11" s="275"/>
+      <c r="D11" s="276"/>
+      <c r="E11" s="277">
         <f>SUM('Corrected energy balance step 2'!C9:H9,'Corrected energy balance step 2'!J9:N9,'Corrected energy balance step 2'!S9)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="278">
+      <c r="F11" s="277">
         <f>'Corrected energy balance step 2'!I9</f>
         <v>0</v>
       </c>
-      <c r="G11" s="278">
+      <c r="G11" s="277">
         <f>'Corrected energy balance step 2'!T9</f>
         <v>0</v>
       </c>
-      <c r="H11" s="278">
+      <c r="H11" s="277">
         <f>SUM('Corrected energy balance step 2'!U9:AQ9)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="278">
+      <c r="I11" s="277">
         <f>'Corrected energy balance step 2'!AS9</f>
         <v>0</v>
       </c>
-      <c r="J11" s="278">
+      <c r="J11" s="277">
         <f>SUM('Corrected energy balance step 2'!AR9,'Corrected energy balance step 2'!AT9)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="278">
+      <c r="K11" s="277">
         <f>'Corrected energy balance step 2'!AV9</f>
         <v>0</v>
       </c>
-      <c r="L11" s="278">
+      <c r="L11" s="277">
         <f>'Corrected energy balance step 2'!AW9</f>
         <v>0</v>
       </c>
-      <c r="M11" s="278">
+      <c r="M11" s="277">
         <f>'Corrected energy balance step 2'!AX9</f>
         <v>0</v>
       </c>
-      <c r="N11" s="278">
+      <c r="N11" s="277">
         <f>'Corrected energy balance step 2'!AU9+'Corrected energy balance step 2'!AZ9</f>
         <v>0</v>
       </c>
-      <c r="O11" s="279"/>
+      <c r="O11" s="278"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="B12" s="271"/>
-      <c r="C12" s="276"/>
-      <c r="D12" s="277"/>
-      <c r="E12" s="296"/>
-      <c r="F12" s="296"/>
-      <c r="G12" s="296"/>
-      <c r="H12" s="296"/>
-      <c r="I12" s="296"/>
-      <c r="J12" s="296"/>
-      <c r="K12" s="296"/>
-      <c r="L12" s="296"/>
-      <c r="M12" s="296"/>
-      <c r="N12" s="296"/>
-      <c r="O12" s="297"/>
+      <c r="B12" s="270"/>
+      <c r="C12" s="275"/>
+      <c r="D12" s="276"/>
+      <c r="E12" s="295"/>
+      <c r="F12" s="295"/>
+      <c r="G12" s="295"/>
+      <c r="H12" s="295"/>
+      <c r="I12" s="295"/>
+      <c r="J12" s="295"/>
+      <c r="K12" s="295"/>
+      <c r="L12" s="295"/>
+      <c r="M12" s="295"/>
+      <c r="N12" s="295"/>
+      <c r="O12" s="296"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="271" t="s">
+      <c r="B13" s="270" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="276"/>
-      <c r="D13" s="277"/>
-      <c r="E13" s="278"/>
-      <c r="F13" s="278"/>
-      <c r="G13" s="278"/>
-      <c r="H13" s="278"/>
-      <c r="I13" s="278"/>
-      <c r="J13" s="278"/>
-      <c r="K13" s="278">
+      <c r="C13" s="275"/>
+      <c r="D13" s="276"/>
+      <c r="E13" s="277"/>
+      <c r="F13" s="277"/>
+      <c r="G13" s="277"/>
+      <c r="H13" s="277"/>
+      <c r="I13" s="277"/>
+      <c r="J13" s="277"/>
+      <c r="K13" s="277">
         <f>'Corrected energy balance step 2'!AV15</f>
         <v>0</v>
       </c>
-      <c r="L13" s="278"/>
-      <c r="M13" s="278"/>
-      <c r="N13" s="278"/>
-      <c r="O13" s="279">
+      <c r="L13" s="277"/>
+      <c r="M13" s="277"/>
+      <c r="N13" s="277"/>
+      <c r="O13" s="278">
         <f>'Corrected energy balance step 2'!BD15</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="271"/>
-      <c r="C14" s="276"/>
-      <c r="D14" s="277"/>
-      <c r="E14" s="296"/>
-      <c r="F14" s="296"/>
-      <c r="G14" s="296"/>
-      <c r="H14" s="296"/>
-      <c r="I14" s="296"/>
-      <c r="J14" s="296"/>
-      <c r="K14" s="296"/>
-      <c r="L14" s="296"/>
-      <c r="M14" s="296"/>
-      <c r="N14" s="296"/>
-      <c r="O14" s="297"/>
+      <c r="B14" s="270"/>
+      <c r="C14" s="275"/>
+      <c r="D14" s="276"/>
+      <c r="E14" s="295"/>
+      <c r="F14" s="295"/>
+      <c r="G14" s="295"/>
+      <c r="H14" s="295"/>
+      <c r="I14" s="295"/>
+      <c r="J14" s="295"/>
+      <c r="K14" s="295"/>
+      <c r="L14" s="295"/>
+      <c r="M14" s="295"/>
+      <c r="N14" s="295"/>
+      <c r="O14" s="296"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="B15" s="271" t="s">
+      <c r="B15" s="270" t="s">
         <v>380</v>
       </c>
-      <c r="C15" s="276" t="s">
+      <c r="C15" s="275" t="s">
         <v>195</v>
       </c>
-      <c r="D15" s="277"/>
-      <c r="E15" s="278"/>
-      <c r="F15" s="278"/>
-      <c r="G15" s="278"/>
-      <c r="H15" s="278"/>
-      <c r="I15" s="278">
+      <c r="D15" s="276"/>
+      <c r="E15" s="277"/>
+      <c r="F15" s="277"/>
+      <c r="G15" s="277"/>
+      <c r="H15" s="277"/>
+      <c r="I15" s="277">
         <f>'Corrected energy balance step 2'!AS18</f>
         <v>0</v>
       </c>
-      <c r="J15" s="278">
+      <c r="J15" s="277">
         <f>SUM('Corrected energy balance step 2'!AR18,'Corrected energy balance step 2'!AT18)</f>
         <v>0</v>
       </c>
-      <c r="K15" s="278">
+      <c r="K15" s="277">
         <f>'Corrected energy balance step 2'!AV18</f>
         <v>0</v>
       </c>
-      <c r="L15" s="278"/>
-      <c r="M15" s="278"/>
-      <c r="N15" s="278"/>
-      <c r="O15" s="279"/>
+      <c r="L15" s="277"/>
+      <c r="M15" s="277"/>
+      <c r="N15" s="277"/>
+      <c r="O15" s="278"/>
     </row>
     <row r="16" spans="2:15">
       <c r="B16" s="87"/>
-      <c r="C16" s="276" t="s">
+      <c r="C16" s="275" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="277"/>
-      <c r="E16" s="278"/>
-      <c r="F16" s="278"/>
-      <c r="G16" s="278"/>
-      <c r="H16" s="278"/>
-      <c r="I16" s="278"/>
-      <c r="J16" s="278"/>
-      <c r="K16" s="278">
+      <c r="D16" s="276"/>
+      <c r="E16" s="277"/>
+      <c r="F16" s="277"/>
+      <c r="G16" s="277"/>
+      <c r="H16" s="277"/>
+      <c r="I16" s="277"/>
+      <c r="J16" s="277"/>
+      <c r="K16" s="277">
         <f>'Corrected energy balance step 2'!AV22</f>
         <v>0</v>
       </c>
-      <c r="L16" s="278"/>
-      <c r="M16" s="278"/>
-      <c r="N16" s="278"/>
-      <c r="O16" s="279"/>
+      <c r="L16" s="277"/>
+      <c r="M16" s="277"/>
+      <c r="N16" s="277"/>
+      <c r="O16" s="278"/>
     </row>
     <row r="17" spans="2:15" ht="16" thickBot="1">
-      <c r="B17" s="291"/>
-      <c r="C17" s="292"/>
-      <c r="D17" s="293"/>
-      <c r="E17" s="294"/>
-      <c r="F17" s="294"/>
-      <c r="G17" s="294"/>
-      <c r="H17" s="294"/>
-      <c r="I17" s="294"/>
-      <c r="J17" s="294"/>
-      <c r="K17" s="294"/>
-      <c r="L17" s="294"/>
-      <c r="M17" s="294"/>
-      <c r="N17" s="294"/>
-      <c r="O17" s="295"/>
+      <c r="B17" s="290"/>
+      <c r="C17" s="291"/>
+      <c r="D17" s="292"/>
+      <c r="E17" s="293"/>
+      <c r="F17" s="293"/>
+      <c r="G17" s="293"/>
+      <c r="H17" s="293"/>
+      <c r="I17" s="293"/>
+      <c r="J17" s="293"/>
+      <c r="K17" s="293"/>
+      <c r="L17" s="293"/>
+      <c r="M17" s="293"/>
+      <c r="N17" s="293"/>
+      <c r="O17" s="294"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -16932,129 +16951,129 @@
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="305">
+      <c r="B22" s="304">
         <v>41507</v>
       </c>
       <c r="C22" s="254" t="s">
         <v>406</v>
       </c>
-      <c r="D22" s="313">
+      <c r="D22" s="312">
         <v>1.07</v>
       </c>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="305">
+      <c r="B23" s="304">
         <v>41509</v>
       </c>
       <c r="C23" s="254" t="s">
         <v>407</v>
       </c>
-      <c r="D23" s="313">
+      <c r="D23" s="312">
         <v>1.08</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="30">
-      <c r="B24" s="305">
+      <c r="B24" s="304">
         <v>41514</v>
       </c>
       <c r="C24" s="254" t="s">
         <v>408</v>
       </c>
-      <c r="D24" s="313">
+      <c r="D24" s="312">
         <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30">
-      <c r="B25" s="305">
+      <c r="B25" s="304">
         <v>41519</v>
       </c>
       <c r="C25" s="254" t="s">
         <v>410</v>
       </c>
-      <c r="D25" s="313">
+      <c r="D25" s="312">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="305">
+      <c r="B26" s="304">
         <v>41520</v>
       </c>
       <c r="C26" s="254" t="s">
         <v>412</v>
       </c>
-      <c r="D26" s="313">
+      <c r="D26" s="312">
         <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="30">
-      <c r="B27" s="305">
+      <c r="B27" s="304">
         <v>41521</v>
       </c>
       <c r="C27" s="254" t="s">
         <v>414</v>
       </c>
-      <c r="D27" s="313">
+      <c r="D27" s="312">
         <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="305">
+      <c r="B28" s="304">
         <v>41521</v>
       </c>
       <c r="C28" s="254" t="s">
         <v>415</v>
       </c>
-      <c r="D28" s="313">
+      <c r="D28" s="312">
         <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="30">
-      <c r="B29" s="305">
+      <c r="B29" s="304">
         <v>41534</v>
       </c>
       <c r="C29" s="254" t="s">
         <v>426</v>
       </c>
-      <c r="D29" s="313" t="s">
+      <c r="D29" s="312" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="45">
-      <c r="B30" s="305">
+      <c r="B30" s="304">
         <v>41555</v>
       </c>
       <c r="C30" s="254" t="s">
         <v>429</v>
       </c>
-      <c r="D30" s="313" t="s">
+      <c r="D30" s="312" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" s="330" t="s">
+      <c r="B31" s="329" t="s">
         <v>430</v>
       </c>
-      <c r="C31" s="331" t="s">
+      <c r="C31" s="330" t="s">
         <v>431</v>
       </c>
-      <c r="D31" s="332">
+      <c r="D31" s="331">
         <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="32" spans="2:4">
-      <c r="B32" s="305"/>
+      <c r="B32" s="304"/>
       <c r="C32" s="254"/>
-      <c r="D32" s="313"/>
+      <c r="D32" s="312"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="305"/>
+      <c r="B33" s="304"/>
       <c r="C33" s="254"/>
-      <c r="D33" s="313"/>
+      <c r="D33" s="312"/>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="305"/>
+      <c r="B34" s="304"/>
       <c r="C34" s="254"/>
-      <c r="D34" s="313"/>
+      <c r="D34" s="312"/>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="248"/>
@@ -17064,7 +17083,7 @@
     <row r="36" spans="2:4">
       <c r="B36" s="250"/>
       <c r="C36" s="251"/>
-      <c r="D36" s="314"/>
+      <c r="D36" s="313"/>
     </row>
     <row r="37" spans="2:4">
       <c r="D37" s="233"/>
@@ -18670,10 +18689,10 @@
       </c>
     </row>
     <row r="19" spans="2:3" s="185" customFormat="1" ht="30" customHeight="1">
-      <c r="B19" s="289" t="s">
+      <c r="B19" s="288" t="s">
         <v>376</v>
       </c>
-      <c r="C19" s="290" t="s">
+      <c r="C19" s="289" t="s">
         <v>391</v>
       </c>
     </row>
@@ -18798,7 +18817,7 @@
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="2:4" ht="106" customHeight="1">
-      <c r="B6" s="280" t="s">
+      <c r="B6" s="279" t="s">
         <v>394</v>
       </c>
       <c r="C6" s="11"/>
@@ -18822,14 +18841,14 @@
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="2:4" ht="15" customHeight="1">
-      <c r="B10" s="281" t="s">
+      <c r="B10" s="280" t="s">
         <v>373</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
     </row>
     <row r="11" spans="2:4" ht="15" customHeight="1">
-      <c r="B11" s="282" t="s">
+      <c r="B11" s="281" t="s">
         <v>395</v>
       </c>
       <c r="C11" s="8"/>
@@ -18857,7 +18876,7 @@
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="2:4" ht="30" customHeight="1">
-      <c r="B15" s="298" t="s">
+      <c r="B15" s="297" t="s">
         <v>399</v>
       </c>
       <c r="C15" s="8"/>
@@ -19379,10 +19398,10 @@
     </row>
     <row r="5" spans="1:6" ht="79" customHeight="1">
       <c r="A5" s="101"/>
-      <c r="B5" s="333" t="s">
+      <c r="B5" s="336" t="s">
         <v>217</v>
       </c>
-      <c r="C5" s="334"/>
+      <c r="C5" s="337"/>
       <c r="D5" s="101"/>
     </row>
     <row r="6" spans="1:6" ht="16" thickBot="1">
@@ -19979,7 +19998,7 @@
     </row>
     <row r="89" spans="2:4">
       <c r="B89" s="119"/>
-      <c r="C89" s="304"/>
+      <c r="C89" s="303"/>
       <c r="D89" s="91"/>
     </row>
     <row r="90" spans="2:4">
@@ -20028,7 +20047,9 @@
   </sheetPr>
   <dimension ref="B2:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -20087,14 +20108,14 @@
       <c r="M4" s="8"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1">
-      <c r="B5" s="335" t="s">
+      <c r="B5" s="338" t="s">
         <v>325</v>
       </c>
-      <c r="C5" s="336"/>
-      <c r="D5" s="336"/>
-      <c r="E5" s="336"/>
-      <c r="F5" s="336"/>
-      <c r="G5" s="337"/>
+      <c r="C5" s="339"/>
+      <c r="D5" s="339"/>
+      <c r="E5" s="339"/>
+      <c r="F5" s="339"/>
+      <c r="G5" s="340"/>
       <c r="H5" s="166"/>
       <c r="I5" s="166"/>
       <c r="J5" s="101"/>
@@ -20103,12 +20124,12 @@
       <c r="M5" s="8"/>
     </row>
     <row r="6" spans="2:17">
-      <c r="B6" s="335"/>
-      <c r="C6" s="336"/>
-      <c r="D6" s="336"/>
-      <c r="E6" s="336"/>
-      <c r="F6" s="336"/>
-      <c r="G6" s="337"/>
+      <c r="B6" s="338"/>
+      <c r="C6" s="339"/>
+      <c r="D6" s="339"/>
+      <c r="E6" s="339"/>
+      <c r="F6" s="339"/>
+      <c r="G6" s="340"/>
       <c r="H6" s="166"/>
       <c r="I6" s="166"/>
       <c r="J6" s="101"/>
@@ -20117,12 +20138,12 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="2:17">
-      <c r="B7" s="333"/>
-      <c r="C7" s="338"/>
-      <c r="D7" s="338"/>
-      <c r="E7" s="338"/>
-      <c r="F7" s="338"/>
-      <c r="G7" s="334"/>
+      <c r="B7" s="336"/>
+      <c r="C7" s="341"/>
+      <c r="D7" s="341"/>
+      <c r="E7" s="341"/>
+      <c r="F7" s="341"/>
+      <c r="G7" s="337"/>
       <c r="H7" s="166"/>
       <c r="I7" s="166"/>
       <c r="J7" s="101"/>
@@ -20175,25 +20196,25 @@
       <c r="B11" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="309" t="s">
+      <c r="C11" s="308" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="309" t="s">
+      <c r="D11" s="308" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="353" t="s">
+      <c r="E11" s="332" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="353"/>
-      <c r="G11" s="353" t="s">
+      <c r="F11" s="332"/>
+      <c r="G11" s="332" t="s">
         <v>409</v>
       </c>
-      <c r="H11" s="353"/>
-      <c r="I11" s="353" t="s">
+      <c r="H11" s="332"/>
+      <c r="I11" s="332" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="309"/>
-      <c r="K11" s="310" t="s">
+      <c r="J11" s="308"/>
+      <c r="K11" s="309" t="s">
         <v>35</v>
       </c>
       <c r="L11" s="152" t="s">
@@ -20248,7 +20269,7 @@
       <c r="K13" s="155" t="s">
         <v>221</v>
       </c>
-      <c r="L13" s="326" t="b">
+      <c r="L13" s="325" t="b">
         <f>IF(COUNTIF(P:P,0)+COUNTIF(P:P,FALSE)=0,TRUE,FALSE)</f>
         <v>0</v>
       </c>
@@ -20280,7 +20301,7 @@
       <c r="K14" s="155" t="s">
         <v>203</v>
       </c>
-      <c r="L14" s="262" t="b">
+      <c r="L14" s="325" t="b">
         <f>IF(COUNTBLANK(C13:C51)-COUNTBLANK(E13:E51)=0,TRUE,FALSE)</f>
         <v>0</v>
       </c>
@@ -20300,13 +20321,13 @@
     </row>
     <row r="15" spans="2:17">
       <c r="B15" s="68"/>
-      <c r="C15" s="311"/>
-      <c r="D15" s="312"/>
-      <c r="E15" s="354"/>
-      <c r="F15" s="354"/>
-      <c r="G15" s="354"/>
-      <c r="H15" s="354"/>
-      <c r="I15" s="354"/>
+      <c r="C15" s="310"/>
+      <c r="D15" s="311"/>
+      <c r="E15" s="333"/>
+      <c r="F15" s="333"/>
+      <c r="G15" s="333"/>
+      <c r="H15" s="333"/>
+      <c r="I15" s="333"/>
       <c r="J15" s="150"/>
       <c r="K15" s="151"/>
       <c r="L15" s="179"/>
@@ -20345,7 +20366,7 @@
       <c r="D17" s="144" t="s">
         <v>252</v>
       </c>
-      <c r="E17" s="355" t="e">
+      <c r="E17" s="334" t="e">
         <f>VLOOKUP(base_year,Timecurves!B10:H50, 2)</f>
         <v>#N/A</v>
       </c>
@@ -20359,7 +20380,7 @@
       <c r="K17" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="L17" s="328" t="e">
+      <c r="L17" s="327" t="e">
         <f>IF(ABS((E17-'Fuel aggregation'!E11))&lt;=0.1*'Fuel aggregation'!E11,TRUE,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -20380,7 +20401,7 @@
       <c r="D18" s="144" t="s">
         <v>252</v>
       </c>
-      <c r="E18" s="355" t="e">
+      <c r="E18" s="334" t="e">
         <f>VLOOKUP(base_year,Timecurves!B10:H50, 3)</f>
         <v>#N/A</v>
       </c>
@@ -20394,7 +20415,7 @@
       <c r="K18" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="L18" s="328" t="e">
+      <c r="L18" s="327" t="e">
         <f>IF(ABS((E18-'Fuel aggregation'!F11))&lt;=0.1*'Fuel aggregation'!F11,TRUE,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -20415,7 +20436,7 @@
       <c r="D19" s="144" t="s">
         <v>252</v>
       </c>
-      <c r="E19" s="329" t="e">
+      <c r="E19" s="328" t="e">
         <f>VLOOKUP(base_year,Timecurves!B10:H50, 4)</f>
         <v>#N/A</v>
       </c>
@@ -20429,7 +20450,7 @@
       <c r="K19" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="L19" s="328" t="e">
+      <c r="L19" s="327" t="e">
         <f>IF(ABS((E19-'Fuel aggregation'!G11))&lt;=0.1*'Fuel aggregation'!G11,TRUE,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -20450,7 +20471,7 @@
       <c r="D20" s="144" t="s">
         <v>252</v>
       </c>
-      <c r="E20" s="329" t="e">
+      <c r="E20" s="328" t="e">
         <f>VLOOKUP(base_year,Timecurves!B10:H50, 5)</f>
         <v>#N/A</v>
       </c>
@@ -20464,7 +20485,7 @@
       <c r="K20" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="L20" s="328" t="e">
+      <c r="L20" s="327" t="e">
         <f>IF(ABS((E20-'Fuel aggregation'!H11))&lt;=0.1*'Fuel aggregation'!H11,TRUE,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -20485,7 +20506,7 @@
       <c r="D21" s="144" t="s">
         <v>252</v>
       </c>
-      <c r="E21" s="329" t="e">
+      <c r="E21" s="328" t="e">
         <f>VLOOKUP(base_year,Timecurves!B10:H50, 6)</f>
         <v>#N/A</v>
       </c>
@@ -20806,7 +20827,7 @@
       <c r="F34" s="178"/>
       <c r="G34" s="178"/>
       <c r="H34" s="178"/>
-      <c r="I34" s="354"/>
+      <c r="I34" s="333"/>
       <c r="J34" s="10"/>
       <c r="K34" s="16"/>
       <c r="L34" s="179"/>
@@ -21112,7 +21133,7 @@
       <c r="F47" s="178"/>
       <c r="G47" s="178"/>
       <c r="H47" s="178"/>
-      <c r="I47" s="354"/>
+      <c r="I47" s="333"/>
       <c r="J47" s="10"/>
       <c r="K47" s="16"/>
       <c r="L47" s="179"/>
@@ -21152,12 +21173,12 @@
       <c r="F49" s="170"/>
       <c r="G49" s="170"/>
       <c r="H49" s="170"/>
-      <c r="I49" s="356"/>
+      <c r="I49" s="335"/>
       <c r="J49" s="9"/>
       <c r="K49" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="L49" s="327">
+      <c r="L49" s="326">
         <f>IF(SUM(E49:E50)=1,TRUE,SUM(E49:E50))</f>
         <v>0</v>
       </c>
@@ -21239,23 +21260,23 @@
   <mergeCells count="1">
     <mergeCell ref="B5:G7"/>
   </mergeCells>
-  <conditionalFormatting sqref="L14">
-    <cfRule type="containsText" dxfId="5" priority="14" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",L14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:L20">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28228,13 +28249,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C9:BO101">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notBetween">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="notBetween">
       <formula>-999999999999999</formula>
       <formula>999999999999999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:BM91">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28287,15 +28308,15 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1">
-      <c r="B5" s="339" t="s">
+      <c r="B5" s="342" t="s">
         <v>326</v>
       </c>
-      <c r="C5" s="340"/>
-      <c r="D5" s="340"/>
-      <c r="E5" s="340"/>
-      <c r="F5" s="340"/>
-      <c r="G5" s="340"/>
-      <c r="H5" s="341"/>
+      <c r="C5" s="343"/>
+      <c r="D5" s="343"/>
+      <c r="E5" s="343"/>
+      <c r="F5" s="343"/>
+      <c r="G5" s="343"/>
+      <c r="H5" s="344"/>
     </row>
     <row r="6" spans="2:9" ht="16" thickBot="1"/>
     <row r="7" spans="2:9">
@@ -28345,454 +28366,454 @@
       <c r="B10" s="87">
         <v>2010</v>
       </c>
-      <c r="C10" s="306"/>
-      <c r="D10" s="307"/>
-      <c r="E10" s="307"/>
-      <c r="F10" s="307"/>
-      <c r="G10" s="307"/>
-      <c r="H10" s="308"/>
+      <c r="C10" s="305"/>
+      <c r="D10" s="306"/>
+      <c r="E10" s="306"/>
+      <c r="F10" s="306"/>
+      <c r="G10" s="306"/>
+      <c r="H10" s="307"/>
       <c r="I10"/>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" s="87">
         <v>2011</v>
       </c>
-      <c r="C11" s="306"/>
-      <c r="D11" s="307"/>
-      <c r="E11" s="307"/>
-      <c r="F11" s="307"/>
-      <c r="G11" s="307"/>
-      <c r="H11" s="308"/>
+      <c r="C11" s="305"/>
+      <c r="D11" s="306"/>
+      <c r="E11" s="306"/>
+      <c r="F11" s="306"/>
+      <c r="G11" s="306"/>
+      <c r="H11" s="307"/>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="87">
         <v>2012</v>
       </c>
-      <c r="C12" s="306"/>
-      <c r="D12" s="307"/>
-      <c r="E12" s="307"/>
-      <c r="F12" s="307"/>
-      <c r="G12" s="307"/>
-      <c r="H12" s="308"/>
+      <c r="C12" s="305"/>
+      <c r="D12" s="306"/>
+      <c r="E12" s="306"/>
+      <c r="F12" s="306"/>
+      <c r="G12" s="306"/>
+      <c r="H12" s="307"/>
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="87">
         <v>2013</v>
       </c>
-      <c r="C13" s="306"/>
-      <c r="D13" s="307"/>
-      <c r="E13" s="307"/>
-      <c r="F13" s="307"/>
-      <c r="G13" s="307"/>
-      <c r="H13" s="308"/>
+      <c r="C13" s="305"/>
+      <c r="D13" s="306"/>
+      <c r="E13" s="306"/>
+      <c r="F13" s="306"/>
+      <c r="G13" s="306"/>
+      <c r="H13" s="307"/>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="87">
         <v>2014</v>
       </c>
-      <c r="C14" s="306"/>
-      <c r="D14" s="307"/>
-      <c r="E14" s="307"/>
-      <c r="F14" s="307"/>
-      <c r="G14" s="307"/>
-      <c r="H14" s="308"/>
+      <c r="C14" s="305"/>
+      <c r="D14" s="306"/>
+      <c r="E14" s="306"/>
+      <c r="F14" s="306"/>
+      <c r="G14" s="306"/>
+      <c r="H14" s="307"/>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="87">
         <v>2015</v>
       </c>
-      <c r="C15" s="306"/>
-      <c r="D15" s="307"/>
-      <c r="E15" s="307"/>
-      <c r="F15" s="307"/>
-      <c r="G15" s="307"/>
-      <c r="H15" s="308"/>
+      <c r="C15" s="305"/>
+      <c r="D15" s="306"/>
+      <c r="E15" s="306"/>
+      <c r="F15" s="306"/>
+      <c r="G15" s="306"/>
+      <c r="H15" s="307"/>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="87">
         <v>2016</v>
       </c>
-      <c r="C16" s="306"/>
-      <c r="D16" s="307"/>
-      <c r="E16" s="307"/>
-      <c r="F16" s="307"/>
-      <c r="G16" s="307"/>
-      <c r="H16" s="308"/>
+      <c r="C16" s="305"/>
+      <c r="D16" s="306"/>
+      <c r="E16" s="306"/>
+      <c r="F16" s="306"/>
+      <c r="G16" s="306"/>
+      <c r="H16" s="307"/>
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="87">
         <v>2017</v>
       </c>
-      <c r="C17" s="306"/>
-      <c r="D17" s="307"/>
-      <c r="E17" s="307"/>
-      <c r="F17" s="307"/>
-      <c r="G17" s="307"/>
-      <c r="H17" s="308"/>
+      <c r="C17" s="305"/>
+      <c r="D17" s="306"/>
+      <c r="E17" s="306"/>
+      <c r="F17" s="306"/>
+      <c r="G17" s="306"/>
+      <c r="H17" s="307"/>
     </row>
     <row r="18" spans="1:8">
       <c r="B18" s="87">
         <v>2018</v>
       </c>
-      <c r="C18" s="306"/>
-      <c r="D18" s="307"/>
-      <c r="E18" s="307"/>
-      <c r="F18" s="307"/>
-      <c r="G18" s="307"/>
-      <c r="H18" s="308"/>
+      <c r="C18" s="305"/>
+      <c r="D18" s="306"/>
+      <c r="E18" s="306"/>
+      <c r="F18" s="306"/>
+      <c r="G18" s="306"/>
+      <c r="H18" s="307"/>
     </row>
     <row r="19" spans="1:8">
       <c r="B19" s="87">
         <v>2019</v>
       </c>
-      <c r="C19" s="306"/>
-      <c r="D19" s="307"/>
-      <c r="E19" s="307"/>
-      <c r="F19" s="307"/>
-      <c r="G19" s="307"/>
-      <c r="H19" s="308"/>
+      <c r="C19" s="305"/>
+      <c r="D19" s="306"/>
+      <c r="E19" s="306"/>
+      <c r="F19" s="306"/>
+      <c r="G19" s="306"/>
+      <c r="H19" s="307"/>
     </row>
     <row r="20" spans="1:8">
       <c r="B20" s="87">
         <v>2020</v>
       </c>
-      <c r="C20" s="306"/>
-      <c r="D20" s="307"/>
-      <c r="E20" s="307"/>
-      <c r="F20" s="307"/>
-      <c r="G20" s="307"/>
-      <c r="H20" s="308"/>
+      <c r="C20" s="305"/>
+      <c r="D20" s="306"/>
+      <c r="E20" s="306"/>
+      <c r="F20" s="306"/>
+      <c r="G20" s="306"/>
+      <c r="H20" s="307"/>
     </row>
     <row r="21" spans="1:8">
       <c r="B21" s="87">
         <v>2021</v>
       </c>
-      <c r="C21" s="306"/>
-      <c r="D21" s="307"/>
-      <c r="E21" s="307"/>
-      <c r="F21" s="307"/>
-      <c r="G21" s="307"/>
-      <c r="H21" s="308"/>
+      <c r="C21" s="305"/>
+      <c r="D21" s="306"/>
+      <c r="E21" s="306"/>
+      <c r="F21" s="306"/>
+      <c r="G21" s="306"/>
+      <c r="H21" s="307"/>
     </row>
     <row r="22" spans="1:8">
       <c r="B22" s="87">
         <v>2022</v>
       </c>
-      <c r="C22" s="306"/>
-      <c r="D22" s="307"/>
-      <c r="E22" s="307"/>
-      <c r="F22" s="307"/>
-      <c r="G22" s="307"/>
-      <c r="H22" s="308"/>
+      <c r="C22" s="305"/>
+      <c r="D22" s="306"/>
+      <c r="E22" s="306"/>
+      <c r="F22" s="306"/>
+      <c r="G22" s="306"/>
+      <c r="H22" s="307"/>
     </row>
     <row r="23" spans="1:8">
       <c r="B23" s="87">
         <v>2023</v>
       </c>
-      <c r="C23" s="306"/>
-      <c r="D23" s="307"/>
-      <c r="E23" s="307"/>
-      <c r="F23" s="307"/>
-      <c r="G23" s="307"/>
-      <c r="H23" s="308"/>
+      <c r="C23" s="305"/>
+      <c r="D23" s="306"/>
+      <c r="E23" s="306"/>
+      <c r="F23" s="306"/>
+      <c r="G23" s="306"/>
+      <c r="H23" s="307"/>
     </row>
     <row r="24" spans="1:8">
       <c r="B24" s="87">
         <v>2024</v>
       </c>
-      <c r="C24" s="306"/>
-      <c r="D24" s="307"/>
-      <c r="E24" s="307"/>
-      <c r="F24" s="307"/>
-      <c r="G24" s="307"/>
-      <c r="H24" s="308"/>
+      <c r="C24" s="305"/>
+      <c r="D24" s="306"/>
+      <c r="E24" s="306"/>
+      <c r="F24" s="306"/>
+      <c r="G24" s="306"/>
+      <c r="H24" s="307"/>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" s="87">
         <v>2025</v>
       </c>
-      <c r="C25" s="306"/>
-      <c r="D25" s="307"/>
-      <c r="E25" s="307"/>
-      <c r="F25" s="307"/>
-      <c r="G25" s="307"/>
-      <c r="H25" s="308"/>
+      <c r="C25" s="305"/>
+      <c r="D25" s="306"/>
+      <c r="E25" s="306"/>
+      <c r="F25" s="306"/>
+      <c r="G25" s="306"/>
+      <c r="H25" s="307"/>
     </row>
     <row r="26" spans="1:8">
       <c r="B26" s="87">
         <v>2026</v>
       </c>
-      <c r="C26" s="306"/>
-      <c r="D26" s="307"/>
-      <c r="E26" s="307"/>
-      <c r="F26" s="307"/>
-      <c r="G26" s="307"/>
-      <c r="H26" s="308"/>
+      <c r="C26" s="305"/>
+      <c r="D26" s="306"/>
+      <c r="E26" s="306"/>
+      <c r="F26" s="306"/>
+      <c r="G26" s="306"/>
+      <c r="H26" s="307"/>
     </row>
     <row r="27" spans="1:8">
       <c r="B27" s="87">
         <v>2027</v>
       </c>
-      <c r="C27" s="306"/>
-      <c r="D27" s="307"/>
-      <c r="E27" s="307"/>
-      <c r="F27" s="307"/>
-      <c r="G27" s="307"/>
-      <c r="H27" s="308"/>
+      <c r="C27" s="305"/>
+      <c r="D27" s="306"/>
+      <c r="E27" s="306"/>
+      <c r="F27" s="306"/>
+      <c r="G27" s="306"/>
+      <c r="H27" s="307"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="124"/>
       <c r="B28" s="87">
         <v>2028</v>
       </c>
-      <c r="C28" s="306"/>
-      <c r="D28" s="307"/>
-      <c r="E28" s="307"/>
-      <c r="F28" s="307"/>
-      <c r="G28" s="307"/>
-      <c r="H28" s="308"/>
+      <c r="C28" s="305"/>
+      <c r="D28" s="306"/>
+      <c r="E28" s="306"/>
+      <c r="F28" s="306"/>
+      <c r="G28" s="306"/>
+      <c r="H28" s="307"/>
     </row>
     <row r="29" spans="1:8">
       <c r="B29" s="87">
         <v>2029</v>
       </c>
-      <c r="C29" s="306"/>
-      <c r="D29" s="307"/>
-      <c r="E29" s="307"/>
-      <c r="F29" s="307"/>
-      <c r="G29" s="307"/>
-      <c r="H29" s="308"/>
+      <c r="C29" s="305"/>
+      <c r="D29" s="306"/>
+      <c r="E29" s="306"/>
+      <c r="F29" s="306"/>
+      <c r="G29" s="306"/>
+      <c r="H29" s="307"/>
     </row>
     <row r="30" spans="1:8">
       <c r="B30" s="87">
         <v>2030</v>
       </c>
-      <c r="C30" s="306"/>
-      <c r="D30" s="307"/>
-      <c r="E30" s="307"/>
-      <c r="F30" s="307"/>
-      <c r="G30" s="307"/>
-      <c r="H30" s="308"/>
+      <c r="C30" s="305"/>
+      <c r="D30" s="306"/>
+      <c r="E30" s="306"/>
+      <c r="F30" s="306"/>
+      <c r="G30" s="306"/>
+      <c r="H30" s="307"/>
     </row>
     <row r="31" spans="1:8">
       <c r="B31" s="87">
         <v>2031</v>
       </c>
-      <c r="C31" s="306"/>
-      <c r="D31" s="307"/>
-      <c r="E31" s="307"/>
-      <c r="F31" s="307"/>
-      <c r="G31" s="307"/>
-      <c r="H31" s="308"/>
+      <c r="C31" s="305"/>
+      <c r="D31" s="306"/>
+      <c r="E31" s="306"/>
+      <c r="F31" s="306"/>
+      <c r="G31" s="306"/>
+      <c r="H31" s="307"/>
     </row>
     <row r="32" spans="1:8">
       <c r="B32" s="87">
         <v>2032</v>
       </c>
-      <c r="C32" s="306"/>
-      <c r="D32" s="307"/>
-      <c r="E32" s="307"/>
-      <c r="F32" s="307"/>
-      <c r="G32" s="307"/>
-      <c r="H32" s="308"/>
+      <c r="C32" s="305"/>
+      <c r="D32" s="306"/>
+      <c r="E32" s="306"/>
+      <c r="F32" s="306"/>
+      <c r="G32" s="306"/>
+      <c r="H32" s="307"/>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="87">
         <v>2033</v>
       </c>
-      <c r="C33" s="306"/>
-      <c r="D33" s="307"/>
-      <c r="E33" s="307"/>
-      <c r="F33" s="307"/>
-      <c r="G33" s="307"/>
-      <c r="H33" s="308"/>
+      <c r="C33" s="305"/>
+      <c r="D33" s="306"/>
+      <c r="E33" s="306"/>
+      <c r="F33" s="306"/>
+      <c r="G33" s="306"/>
+      <c r="H33" s="307"/>
     </row>
     <row r="34" spans="2:8">
       <c r="B34" s="87">
         <v>2034</v>
       </c>
-      <c r="C34" s="306"/>
-      <c r="D34" s="307"/>
-      <c r="E34" s="307"/>
-      <c r="F34" s="307"/>
-      <c r="G34" s="307"/>
-      <c r="H34" s="308"/>
+      <c r="C34" s="305"/>
+      <c r="D34" s="306"/>
+      <c r="E34" s="306"/>
+      <c r="F34" s="306"/>
+      <c r="G34" s="306"/>
+      <c r="H34" s="307"/>
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="87">
         <v>2035</v>
       </c>
-      <c r="C35" s="306"/>
-      <c r="D35" s="307"/>
-      <c r="E35" s="307"/>
-      <c r="F35" s="307"/>
-      <c r="G35" s="307"/>
-      <c r="H35" s="308"/>
+      <c r="C35" s="305"/>
+      <c r="D35" s="306"/>
+      <c r="E35" s="306"/>
+      <c r="F35" s="306"/>
+      <c r="G35" s="306"/>
+      <c r="H35" s="307"/>
     </row>
     <row r="36" spans="2:8">
       <c r="B36" s="87">
         <v>2036</v>
       </c>
-      <c r="C36" s="306"/>
-      <c r="D36" s="307"/>
-      <c r="E36" s="307"/>
-      <c r="F36" s="307"/>
-      <c r="G36" s="307"/>
-      <c r="H36" s="308"/>
+      <c r="C36" s="305"/>
+      <c r="D36" s="306"/>
+      <c r="E36" s="306"/>
+      <c r="F36" s="306"/>
+      <c r="G36" s="306"/>
+      <c r="H36" s="307"/>
     </row>
     <row r="37" spans="2:8">
       <c r="B37" s="87">
         <v>2037</v>
       </c>
-      <c r="C37" s="306"/>
-      <c r="D37" s="307"/>
-      <c r="E37" s="307"/>
-      <c r="F37" s="307"/>
-      <c r="G37" s="307"/>
-      <c r="H37" s="308"/>
+      <c r="C37" s="305"/>
+      <c r="D37" s="306"/>
+      <c r="E37" s="306"/>
+      <c r="F37" s="306"/>
+      <c r="G37" s="306"/>
+      <c r="H37" s="307"/>
     </row>
     <row r="38" spans="2:8">
       <c r="B38" s="87">
         <v>2038</v>
       </c>
-      <c r="C38" s="306"/>
-      <c r="D38" s="307"/>
-      <c r="E38" s="307"/>
-      <c r="F38" s="307"/>
-      <c r="G38" s="307"/>
-      <c r="H38" s="308"/>
+      <c r="C38" s="305"/>
+      <c r="D38" s="306"/>
+      <c r="E38" s="306"/>
+      <c r="F38" s="306"/>
+      <c r="G38" s="306"/>
+      <c r="H38" s="307"/>
     </row>
     <row r="39" spans="2:8">
       <c r="B39" s="87">
         <v>2039</v>
       </c>
-      <c r="C39" s="306"/>
-      <c r="D39" s="307"/>
-      <c r="E39" s="307"/>
-      <c r="F39" s="307"/>
-      <c r="G39" s="307"/>
-      <c r="H39" s="308"/>
+      <c r="C39" s="305"/>
+      <c r="D39" s="306"/>
+      <c r="E39" s="306"/>
+      <c r="F39" s="306"/>
+      <c r="G39" s="306"/>
+      <c r="H39" s="307"/>
     </row>
     <row r="40" spans="2:8">
       <c r="B40" s="87">
         <v>2040</v>
       </c>
-      <c r="C40" s="306"/>
-      <c r="D40" s="307"/>
-      <c r="E40" s="307"/>
-      <c r="F40" s="307"/>
-      <c r="G40" s="307"/>
-      <c r="H40" s="308"/>
+      <c r="C40" s="305"/>
+      <c r="D40" s="306"/>
+      <c r="E40" s="306"/>
+      <c r="F40" s="306"/>
+      <c r="G40" s="306"/>
+      <c r="H40" s="307"/>
     </row>
     <row r="41" spans="2:8">
       <c r="B41" s="87">
         <v>2041</v>
       </c>
-      <c r="C41" s="306"/>
-      <c r="D41" s="307"/>
-      <c r="E41" s="307"/>
-      <c r="F41" s="307"/>
-      <c r="G41" s="307"/>
-      <c r="H41" s="308"/>
+      <c r="C41" s="305"/>
+      <c r="D41" s="306"/>
+      <c r="E41" s="306"/>
+      <c r="F41" s="306"/>
+      <c r="G41" s="306"/>
+      <c r="H41" s="307"/>
     </row>
     <row r="42" spans="2:8">
       <c r="B42" s="87">
         <v>2042</v>
       </c>
-      <c r="C42" s="306"/>
-      <c r="D42" s="307"/>
-      <c r="E42" s="307"/>
-      <c r="F42" s="307"/>
-      <c r="G42" s="307"/>
-      <c r="H42" s="308"/>
+      <c r="C42" s="305"/>
+      <c r="D42" s="306"/>
+      <c r="E42" s="306"/>
+      <c r="F42" s="306"/>
+      <c r="G42" s="306"/>
+      <c r="H42" s="307"/>
     </row>
     <row r="43" spans="2:8">
       <c r="B43" s="87">
         <v>2043</v>
       </c>
-      <c r="C43" s="306"/>
-      <c r="D43" s="307"/>
-      <c r="E43" s="307"/>
-      <c r="F43" s="307"/>
-      <c r="G43" s="307"/>
-      <c r="H43" s="308"/>
+      <c r="C43" s="305"/>
+      <c r="D43" s="306"/>
+      <c r="E43" s="306"/>
+      <c r="F43" s="306"/>
+      <c r="G43" s="306"/>
+      <c r="H43" s="307"/>
     </row>
     <row r="44" spans="2:8">
       <c r="B44" s="87">
         <v>2044</v>
       </c>
-      <c r="C44" s="306"/>
-      <c r="D44" s="307"/>
-      <c r="E44" s="307"/>
-      <c r="F44" s="307"/>
-      <c r="G44" s="307"/>
-      <c r="H44" s="308"/>
+      <c r="C44" s="305"/>
+      <c r="D44" s="306"/>
+      <c r="E44" s="306"/>
+      <c r="F44" s="306"/>
+      <c r="G44" s="306"/>
+      <c r="H44" s="307"/>
     </row>
     <row r="45" spans="2:8">
       <c r="B45" s="87">
         <v>2045</v>
       </c>
-      <c r="C45" s="306"/>
-      <c r="D45" s="307"/>
-      <c r="E45" s="307"/>
-      <c r="F45" s="307"/>
-      <c r="G45" s="307"/>
-      <c r="H45" s="308"/>
+      <c r="C45" s="305"/>
+      <c r="D45" s="306"/>
+      <c r="E45" s="306"/>
+      <c r="F45" s="306"/>
+      <c r="G45" s="306"/>
+      <c r="H45" s="307"/>
     </row>
     <row r="46" spans="2:8">
       <c r="B46" s="87">
         <v>2046</v>
       </c>
-      <c r="C46" s="306"/>
-      <c r="D46" s="307"/>
-      <c r="E46" s="307"/>
-      <c r="F46" s="307"/>
-      <c r="G46" s="307"/>
-      <c r="H46" s="308"/>
+      <c r="C46" s="305"/>
+      <c r="D46" s="306"/>
+      <c r="E46" s="306"/>
+      <c r="F46" s="306"/>
+      <c r="G46" s="306"/>
+      <c r="H46" s="307"/>
     </row>
     <row r="47" spans="2:8">
       <c r="B47" s="87">
         <v>2047</v>
       </c>
-      <c r="C47" s="306"/>
-      <c r="D47" s="307"/>
-      <c r="E47" s="307"/>
-      <c r="F47" s="307"/>
-      <c r="G47" s="307"/>
-      <c r="H47" s="308"/>
+      <c r="C47" s="305"/>
+      <c r="D47" s="306"/>
+      <c r="E47" s="306"/>
+      <c r="F47" s="306"/>
+      <c r="G47" s="306"/>
+      <c r="H47" s="307"/>
     </row>
     <row r="48" spans="2:8">
       <c r="B48" s="87">
         <v>2048</v>
       </c>
-      <c r="C48" s="306"/>
-      <c r="D48" s="307"/>
-      <c r="E48" s="307"/>
-      <c r="F48" s="307"/>
-      <c r="G48" s="307"/>
-      <c r="H48" s="308"/>
+      <c r="C48" s="305"/>
+      <c r="D48" s="306"/>
+      <c r="E48" s="306"/>
+      <c r="F48" s="306"/>
+      <c r="G48" s="306"/>
+      <c r="H48" s="307"/>
     </row>
     <row r="49" spans="2:8">
       <c r="B49" s="87">
         <v>2049</v>
       </c>
-      <c r="C49" s="306"/>
-      <c r="D49" s="307"/>
-      <c r="E49" s="307"/>
-      <c r="F49" s="307"/>
-      <c r="G49" s="307"/>
-      <c r="H49" s="308"/>
+      <c r="C49" s="305"/>
+      <c r="D49" s="306"/>
+      <c r="E49" s="306"/>
+      <c r="F49" s="306"/>
+      <c r="G49" s="306"/>
+      <c r="H49" s="307"/>
     </row>
     <row r="50" spans="2:8">
       <c r="B50" s="87">
         <v>2050</v>
       </c>
-      <c r="C50" s="306"/>
-      <c r="D50" s="307"/>
-      <c r="E50" s="307"/>
-      <c r="F50" s="307"/>
-      <c r="G50" s="307"/>
-      <c r="H50" s="308"/>
+      <c r="C50" s="305"/>
+      <c r="D50" s="306"/>
+      <c r="E50" s="306"/>
+      <c r="F50" s="306"/>
+      <c r="G50" s="306"/>
+      <c r="H50" s="307"/>
     </row>
     <row r="51" spans="2:8" ht="16" thickBot="1">
       <c r="B51" s="62"/>

</xml_diff>

<commit_message>
Added UK, PL, ES and FR datasets and updated analyses and documentation.
</commit_message>
<xml_diff>
--- a/analyses/3_primary_production_analysis.xlsx
+++ b/analyses/3_primary_production_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="902" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="902" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="1" r:id="rId1"/>
@@ -1085,9 +1085,6 @@
     <t>Bio-residues for firing</t>
   </si>
   <si>
-    <t>Bio-residues</t>
-  </si>
-  <si>
     <t>Total primary energy supply of biogas (from energy balance)</t>
   </si>
   <si>
@@ -1448,6 +1445,9 @@
 3. using assumptions on the Dashboard sheet
 4. based on the demand of these carriers. 
 The goal of this analysis is to combine data from different sources and determine the domestic production and extraction in the base year, which is reported in the primary production table. In addition, available timecurves are exported as csv files. The Primary production analysis includes also calculations related to the production of greengas and waste.</t>
+  </si>
+  <si>
+    <t>Woody biomass</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1467,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -12235,7 +12234,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D4" s="5"/>
       <c r="F4" s="18"/>
@@ -12521,7 +12520,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="20">
       <c r="B2" s="225" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C2" s="9"/>
     </row>
@@ -12535,7 +12534,7 @@
     </row>
     <row r="5" spans="2:6" ht="29" customHeight="1">
       <c r="B5" s="342" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C5" s="343"/>
       <c r="D5" s="343"/>
@@ -12547,13 +12546,13 @@
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="305" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C7" s="306"/>
       <c r="D7" s="307"/>
       <c r="E7" s="306"/>
       <c r="F7" s="308" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" customHeight="1">
@@ -12561,28 +12560,28 @@
       <c r="C8" s="9"/>
       <c r="D8" s="287"/>
       <c r="E8" s="309" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F8" s="312" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1">
       <c r="B9" s="71" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C9" s="228" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D9" s="313"/>
       <c r="E9" s="310"/>
       <c r="F9" s="311" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="111" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C10" s="107"/>
       <c r="D10" s="288"/>
@@ -12596,7 +12595,7 @@
       </c>
       <c r="D11" s="287"/>
       <c r="E11" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F11" s="304"/>
     </row>
@@ -12642,7 +12641,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="20">
       <c r="B2" s="22" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -12655,7 +12654,7 @@
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="345" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C5" s="346"/>
       <c r="D5" s="346"/>
@@ -13015,7 +13014,7 @@
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="58" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="229">
@@ -13028,7 +13027,7 @@
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="222" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C12" s="173" t="s">
         <v>289</v>
@@ -13087,7 +13086,7 @@
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="222" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="235">
@@ -13100,7 +13099,7 @@
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="58" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="231" t="e">
@@ -13147,7 +13146,7 @@
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="222" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="237" t="e">
@@ -13163,7 +13162,7 @@
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="58" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="290" t="e">
@@ -13218,7 +13217,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="20">
       <c r="B2" s="22" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -13232,7 +13231,7 @@
     </row>
     <row r="5" spans="2:7" ht="30" customHeight="1">
       <c r="B5" s="342" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C5" s="351"/>
       <c r="D5" s="351"/>
@@ -13284,7 +13283,7 @@
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="58" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="229">
@@ -13300,7 +13299,7 @@
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="58" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C12" s="141"/>
       <c r="D12" s="229">
@@ -13357,7 +13356,7 @@
   <sheetData>
     <row r="2" spans="2:15" ht="20">
       <c r="B2" s="225" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C2" s="225"/>
       <c r="D2" s="225"/>
@@ -13390,7 +13389,7 @@
     </row>
     <row r="5" spans="2:15" ht="30" customHeight="1">
       <c r="B5" s="353" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C5" s="354"/>
       <c r="D5" s="354"/>
@@ -13402,7 +13401,7 @@
     <row r="6" spans="2:15" ht="16" thickBot="1"/>
     <row r="7" spans="2:15">
       <c r="B7" s="55" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="255"/>
@@ -13441,37 +13440,37 @@
       <c r="C9" s="259"/>
       <c r="D9" s="260"/>
       <c r="E9" s="261" t="s">
+        <v>359</v>
+      </c>
+      <c r="F9" s="261" t="s">
+        <v>363</v>
+      </c>
+      <c r="G9" s="261" t="s">
         <v>360</v>
       </c>
-      <c r="F9" s="261" t="s">
-        <v>364</v>
-      </c>
-      <c r="G9" s="261" t="s">
+      <c r="H9" s="261" t="s">
         <v>361</v>
       </c>
-      <c r="H9" s="261" t="s">
-        <v>362</v>
-      </c>
       <c r="I9" s="261" t="s">
+        <v>365</v>
+      </c>
+      <c r="J9" s="261" t="s">
         <v>366</v>
       </c>
-      <c r="J9" s="261" t="s">
+      <c r="K9" s="261" t="s">
+        <v>374</v>
+      </c>
+      <c r="L9" s="261" t="s">
         <v>367</v>
       </c>
-      <c r="K9" s="261" t="s">
-        <v>375</v>
-      </c>
-      <c r="L9" s="261" t="s">
+      <c r="M9" s="261" t="s">
         <v>368</v>
       </c>
-      <c r="M9" s="261" t="s">
+      <c r="N9" s="261" t="s">
         <v>369</v>
       </c>
-      <c r="N9" s="261" t="s">
-        <v>370</v>
-      </c>
       <c r="O9" s="262" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="2:15">
@@ -13596,7 +13595,7 @@
     </row>
     <row r="15" spans="2:15">
       <c r="B15" s="263" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C15" s="268" t="s">
         <v>194</v>
@@ -13747,7 +13746,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="50" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B6" s="88" t="e">
         <f>'Greengas analysis'!D23</f>
@@ -14067,7 +14066,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -14728,7 +14727,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -15387,7 +15386,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -16046,7 +16045,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -16814,7 +16813,7 @@
         <v>41500</v>
       </c>
       <c r="C14" s="242" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D14" s="245">
         <v>0.9</v>
@@ -16825,7 +16824,7 @@
         <v>41500</v>
       </c>
       <c r="C15" s="240" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D15" s="245">
         <v>1</v>
@@ -16836,7 +16835,7 @@
         <v>41500</v>
       </c>
       <c r="C16" s="247" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D16" s="245">
         <v>1.01</v>
@@ -16847,7 +16846,7 @@
         <v>41501</v>
       </c>
       <c r="C17" s="240" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D17" s="245">
         <v>1.02</v>
@@ -16858,7 +16857,7 @@
         <v>41502</v>
       </c>
       <c r="C18" s="242" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D18" s="245">
         <v>1.03</v>
@@ -16869,7 +16868,7 @@
         <v>41505</v>
       </c>
       <c r="C19" s="240" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D19" s="245">
         <v>1.04</v>
@@ -16880,7 +16879,7 @@
         <v>41505</v>
       </c>
       <c r="C20" s="240" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D20" s="245">
         <v>1.05</v>
@@ -16891,7 +16890,7 @@
         <v>41506</v>
       </c>
       <c r="C21" s="242" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D21" s="245">
         <v>1.06</v>
@@ -16902,7 +16901,7 @@
         <v>41507</v>
       </c>
       <c r="C22" s="247" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D22" s="301">
         <v>1.07</v>
@@ -16913,7 +16912,7 @@
         <v>41509</v>
       </c>
       <c r="C23" s="247" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D23" s="301">
         <v>1.08</v>
@@ -16924,7 +16923,7 @@
         <v>41514</v>
       </c>
       <c r="C24" s="247" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D24" s="301">
         <v>1.0900000000000001</v>
@@ -16935,7 +16934,7 @@
         <v>41519</v>
       </c>
       <c r="C25" s="247" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D25" s="301">
         <v>1.1000000000000001</v>
@@ -16946,7 +16945,7 @@
         <v>41520</v>
       </c>
       <c r="C26" s="247" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D26" s="301">
         <v>1.1100000000000001</v>
@@ -16957,7 +16956,7 @@
         <v>41521</v>
       </c>
       <c r="C27" s="247" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D27" s="301">
         <v>1.1200000000000001</v>
@@ -16968,7 +16967,7 @@
         <v>41521</v>
       </c>
       <c r="C28" s="247" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D28" s="301">
         <v>1.1299999999999999</v>
@@ -16979,7 +16978,7 @@
         <v>41534</v>
       </c>
       <c r="C29" s="247" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D29" s="301" t="s">
         <v>289</v>
@@ -16990,7 +16989,7 @@
         <v>41555</v>
       </c>
       <c r="C30" s="247" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D30" s="301" t="s">
         <v>289</v>
@@ -16998,10 +16997,10 @@
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="318" t="s">
+        <v>408</v>
+      </c>
+      <c r="C31" s="319" t="s">
         <v>409</v>
-      </c>
-      <c r="C31" s="319" t="s">
-        <v>410</v>
       </c>
       <c r="D31" s="320">
         <v>1.1399999999999999</v>
@@ -17012,7 +17011,7 @@
         <v>41681</v>
       </c>
       <c r="C32" s="247" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D32" s="301">
         <v>1.1499999999999999</v>
@@ -17023,7 +17022,7 @@
         <v>41688</v>
       </c>
       <c r="C33" s="247" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D33" s="301">
         <v>1.1599999999999999</v>
@@ -17108,7 +17107,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -17767,7 +17766,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="99" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -18419,7 +18418,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -18441,7 +18440,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B4">
         <f>Dashboard!E48</f>
@@ -18473,7 +18472,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -18486,7 +18485,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B3">
         <f>'Waste analysis'!E12</f>
@@ -18495,7 +18494,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B4">
         <f>'Waste analysis'!E11</f>
@@ -18555,7 +18554,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="331" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18563,7 +18562,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="329" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18571,7 +18570,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="329" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18579,7 +18578,7 @@
         <v>208</v>
       </c>
       <c r="C9" s="329" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18587,7 +18586,7 @@
         <v>24</v>
       </c>
       <c r="C10" s="329" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18595,7 +18594,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="329" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18603,7 +18602,7 @@
         <v>302</v>
       </c>
       <c r="C12" s="329" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="13" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18611,20 +18610,20 @@
         <v>235</v>
       </c>
       <c r="C13" s="279" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="14" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B14" s="184" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C14" s="279" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B15" s="185" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C15" s="329" t="s">
         <v>269</v>
@@ -18635,23 +18634,23 @@
         <v>227</v>
       </c>
       <c r="C16" s="329" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="17" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B17" s="185" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C17" s="329" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="18" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B18" s="278" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C18" s="279" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="19" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18664,7 +18663,7 @@
     </row>
     <row r="20" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B20" s="186" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C20" s="329" t="s">
         <v>263</v>
@@ -18672,7 +18671,7 @@
     </row>
     <row r="21" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B21" s="186" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C21" s="329" t="s">
         <v>264</v>
@@ -18680,7 +18679,7 @@
     </row>
     <row r="22" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B22" s="186" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C22" s="329" t="s">
         <v>265</v>
@@ -18688,7 +18687,7 @@
     </row>
     <row r="23" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B23" s="186" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C23" s="329" t="s">
         <v>266</v>
@@ -18696,7 +18695,7 @@
     </row>
     <row r="24" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B24" s="186" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C24" s="329" t="s">
         <v>267</v>
@@ -18704,7 +18703,7 @@
     </row>
     <row r="25" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B25" s="186" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C25" s="330" t="s">
         <v>268</v>
@@ -18712,18 +18711,18 @@
     </row>
     <row r="26" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B26" s="186" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C26" s="330" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="27" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B27" s="186" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C27" s="330" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -18744,7 +18743,7 @@
   </sheetPr>
   <dimension ref="B2:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -18773,7 +18772,7 @@
     </row>
     <row r="6" spans="2:3" ht="150">
       <c r="B6" s="333" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C6" s="9"/>
     </row>
@@ -18797,49 +18796,49 @@
     </row>
     <row r="11" spans="2:3" ht="15" customHeight="1">
       <c r="B11" s="325" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C11" s="9"/>
     </row>
     <row r="12" spans="2:3" ht="15" customHeight="1">
       <c r="B12" s="325" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C12" s="9"/>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1">
       <c r="B13" s="325" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C13" s="9"/>
     </row>
     <row r="14" spans="2:3" ht="15" customHeight="1">
       <c r="B14" s="325" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C14" s="9"/>
     </row>
     <row r="15" spans="2:3" ht="15" customHeight="1">
       <c r="B15" s="325" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C15" s="9"/>
     </row>
     <row r="16" spans="2:3" ht="30" customHeight="1">
       <c r="B16" s="333" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C16" s="9"/>
     </row>
     <row r="17" spans="2:3" ht="15" customHeight="1">
       <c r="B17" s="325" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C17" s="9"/>
     </row>
     <row r="18" spans="2:3" ht="15" customHeight="1">
       <c r="B18" s="325" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C18" s="9"/>
     </row>
@@ -18852,7 +18851,7 @@
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="187" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -18860,7 +18859,7 @@
     </row>
     <row r="23" spans="2:3" ht="90">
       <c r="B23" s="327" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="24" spans="2:3">
@@ -19432,7 +19431,7 @@
     <row r="15" spans="1:6" ht="30">
       <c r="B15" s="70"/>
       <c r="C15" s="114" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D15" s="188"/>
       <c r="F15" s="89"/>
@@ -19496,7 +19495,7 @@
     <row r="24" spans="2:4">
       <c r="B24" s="112"/>
       <c r="C24" s="114" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D24" s="188"/>
     </row>
@@ -19517,14 +19516,14 @@
     <row r="27" spans="2:4">
       <c r="B27" s="202"/>
       <c r="C27" s="197" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D27" s="188"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="202"/>
       <c r="C28" s="197" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D28" s="188"/>
     </row>
@@ -19687,7 +19686,7 @@
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="111" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C52" s="74" t="s">
         <v>42</v>
@@ -19997,9 +19996,7 @@
   </sheetPr>
   <dimension ref="B2:Q59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -20059,7 +20056,7 @@
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1">
       <c r="B5" s="338" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C5" s="339"/>
       <c r="D5" s="339"/>
@@ -20157,7 +20154,7 @@
       </c>
       <c r="F11" s="321"/>
       <c r="G11" s="321" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H11" s="321"/>
       <c r="I11" s="321" t="s">
@@ -20328,7 +20325,7 @@
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L17" s="316" t="e">
         <f>IF(ABS((E17-'Fuel aggregation'!E11))&lt;=0.1*'Fuel aggregation'!E11,TRUE,FALSE)</f>
@@ -20363,7 +20360,7 @@
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L18" s="316" t="e">
         <f>IF(ABS((E18-'Fuel aggregation'!F11))&lt;=0.1*'Fuel aggregation'!F11,TRUE,FALSE)</f>
@@ -20398,7 +20395,7 @@
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L19" s="316" t="e">
         <f>IF(ABS((E19-'Fuel aggregation'!G11))&lt;=0.1*'Fuel aggregation'!G11,TRUE,FALSE)</f>
@@ -20433,7 +20430,7 @@
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L20" s="316" t="e">
         <f>IF(ABS((E20-'Fuel aggregation'!H11))&lt;=0.1*'Fuel aggregation'!H11,TRUE,FALSE)</f>
@@ -20509,7 +20506,7 @@
       <c r="G23" s="161"/>
       <c r="H23" s="161"/>
       <c r="I23" s="107" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="15"/>
@@ -20536,7 +20533,7 @@
       <c r="G24" s="161"/>
       <c r="H24" s="161"/>
       <c r="I24" s="107" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="15"/>
@@ -20587,7 +20584,7 @@
       <c r="G26" s="161"/>
       <c r="H26" s="161"/>
       <c r="I26" s="107" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="15"/>
@@ -20614,7 +20611,7 @@
       <c r="G27" s="161"/>
       <c r="H27" s="161"/>
       <c r="I27" s="107" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="15"/>
@@ -20740,7 +20737,7 @@
       <c r="M32" s="59"/>
       <c r="N32" s="9"/>
       <c r="O32" s="135" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="P32" s="132"/>
       <c r="Q32" s="9"/>
@@ -20875,7 +20872,7 @@
       <c r="M38" s="59"/>
       <c r="N38" s="9"/>
       <c r="O38" s="135" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="P38" s="132"/>
       <c r="Q38" s="9"/>
@@ -20899,7 +20896,7 @@
       <c r="M39" s="59"/>
       <c r="N39" s="9"/>
       <c r="O39" s="135" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P39" s="132"/>
       <c r="Q39" s="9"/>
@@ -28178,7 +28175,9 @@
   </sheetPr>
   <dimension ref="A2:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -28209,7 +28208,7 @@
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1">
       <c r="B5" s="342" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C5" s="343"/>
       <c r="D5" s="343"/>
@@ -28221,7 +28220,7 @@
     <row r="6" spans="2:9" ht="16" thickBot="1"/>
     <row r="7" spans="2:9">
       <c r="B7" s="55" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C7" s="66"/>
       <c r="D7" s="66"/>
@@ -28259,7 +28258,7 @@
         <v>234</v>
       </c>
       <c r="H9" s="118" t="s">
-        <v>313</v>
+        <v>432</v>
       </c>
     </row>
     <row r="10" spans="2:9">

</xml_diff>

<commit_message>
Published state of ETDataset on 31 October 2014.
</commit_message>
<xml_diff>
--- a/analyses/3_primary_production_analysis.xlsx
+++ b/analyses/3_primary_production_analysis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="902" activeTab="6"/>
@@ -27,7 +27,7 @@
     <sheet name="csv_natural_gas_time_curve" sheetId="61" r:id="rId18"/>
     <sheet name="csv_crude_oil_time_curve" sheetId="63" r:id="rId19"/>
     <sheet name="csv_uranium_oxide_time_curve" sheetId="62" r:id="rId20"/>
-    <sheet name="csv_bio_residues_time_curve" sheetId="64" r:id="rId21"/>
+    <sheet name="csv_woody_biomass_time_curve" sheetId="64" r:id="rId21"/>
     <sheet name="csv_energy_distribution_wood_pa" sheetId="68" r:id="rId22"/>
     <sheet name="csv_energy_distribution_waste_m" sheetId="70" r:id="rId23"/>
   </sheets>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="431">
   <si>
     <t>Changelog</t>
   </si>
@@ -869,9 +869,6 @@
     <t>Wood</t>
   </si>
   <si>
-    <t>Bio residues for firing</t>
-  </si>
-  <si>
     <t>Bio-oil</t>
   </si>
   <si>
@@ -899,9 +896,6 @@
     <t>energy_production_bio_oil</t>
   </si>
   <si>
-    <t>energy_production_bio_residues_for_firing</t>
-  </si>
-  <si>
     <t>energy_production_wood_pellets</t>
   </si>
   <si>
@@ -950,9 +944,6 @@
     <t>Output data from this analysis. The timecurve for domestic uranium oxide extraction</t>
   </si>
   <si>
-    <t>Output data from this analysis. The timecurve for the maximum domestic production of bio residues</t>
-  </si>
-  <si>
     <t>An aggregation of the production values in the IEA energy balance with a comparison against the assumptions made on the dashboard</t>
   </si>
   <si>
@@ -962,9 +953,6 @@
     <t>For the domestic extraction of coal, lignite, natural gas, crude oi and uranium oxide, the user is asked to collect and paste timecurves for their country in PJ annual extraction up to 2050</t>
   </si>
   <si>
-    <t>For the maximum domestic production of bio residues, the user is asked to collect and paste a timecurve for their country in PJ annual production up to 2050</t>
-  </si>
-  <si>
     <t>Currently these timecurves are available for some countries in the InputExcel</t>
   </si>
   <si>
@@ -1082,9 +1070,6 @@
     <t>For the other carriers, the domestic production in the base year must be estimated by the user on the dashboard.</t>
   </si>
   <si>
-    <t>Bio-residues for firing</t>
-  </si>
-  <si>
     <t>Total primary energy supply of biogas (from energy balance)</t>
   </si>
   <si>
@@ -1208,9 +1193,6 @@
     <t>csv_uranium_oxide_time_curve</t>
   </si>
   <si>
-    <t>csv_bio_residues_time_curve</t>
-  </si>
-  <si>
     <t>Review by RD</t>
   </si>
   <si>
@@ -1343,9 +1325,6 @@
     <t>energy_extraction_uranium_oxide_time_curve</t>
   </si>
   <si>
-    <t>energy_distribution_bio_residues_for_firing_time_curve</t>
-  </si>
-  <si>
     <t>converter key</t>
   </si>
   <si>
@@ -1424,9 +1403,6 @@
     <t>Corrected energy balance step 2 for your country and year.</t>
   </si>
   <si>
-    <t>Timecurves for domestic extraction of coal, lignite, natural gas, crude oil, uranium oxide and bio residues. The timecurves need to be created using a country-specific source analysis</t>
-  </si>
-  <si>
     <t>Calculation of the shares of biogenic and non-biogenic waste in the waste mix</t>
   </si>
   <si>
@@ -1434,9 +1410,6 @@
   </si>
   <si>
     <t>On this page the country specific assumptions must be entered, with the source of the data when applicable. Besides the corrected energy balance and the timecurves, this is the only manual input that is needed from data analysts. The checks on the right show immediately if there are any inconsistensies between the data and assumptions. A green check means that everything is fine. A red check means that there is a critical issue that must be addressed before the analysis can be used. If a check fails, please read behind the check what you can do to solve it.</t>
-  </si>
-  <si>
-    <t>Please paste (as values) the timescurves of fossil fuels and bio-residues in this page. They should be generated using a country-specific source analysis.</t>
   </si>
   <si>
     <t>The goal of the Primary production analysis is to define the (maximum) production and extraction of energy carriers in the ETM. These values are required in the ETM to determine the domestic potential of certain carriers and to calculate the import and export of carriers. The (maximum) production and extraction of energy carriers can be defined:
@@ -1448,6 +1421,27 @@
   </si>
   <si>
     <t>Woody biomass</t>
+  </si>
+  <si>
+    <t>energy_distribution_woody_biomass_time_curve</t>
+  </si>
+  <si>
+    <t>Please paste (as values) the timescurves of fossil fuels and woody biomass in this page. They should be generated using a country-specific source analysis.</t>
+  </si>
+  <si>
+    <t>energy_production_woody_biomass</t>
+  </si>
+  <si>
+    <t>Timecurves for domestic extraction of coal, lignite, natural gas, crude oil, uranium oxide and woody biomass. The timecurves need to be created using a country-specific source analysis</t>
+  </si>
+  <si>
+    <t>csv_woody_biomass_time_curve</t>
+  </si>
+  <si>
+    <t>Output data from this analysis. The timecurve for the maximum domestic production of woody biomass</t>
+  </si>
+  <si>
+    <t>For the maximum domestic production of woody biomass, the user is asked to collect and paste a timecurve for their country in PJ annual production up to 2050</t>
   </si>
 </sst>
 </file>
@@ -12234,7 +12228,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D4" s="5"/>
       <c r="F4" s="18"/>
@@ -12366,7 +12360,7 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="20" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>214</v>
@@ -12520,7 +12514,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="20">
       <c r="B2" s="225" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C2" s="9"/>
     </row>
@@ -12534,7 +12528,7 @@
     </row>
     <row r="5" spans="2:6" ht="29" customHeight="1">
       <c r="B5" s="342" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C5" s="343"/>
       <c r="D5" s="343"/>
@@ -12546,13 +12540,13 @@
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="305" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C7" s="306"/>
       <c r="D7" s="307"/>
       <c r="E7" s="306"/>
       <c r="F7" s="308" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" customHeight="1">
@@ -12560,28 +12554,28 @@
       <c r="C8" s="9"/>
       <c r="D8" s="287"/>
       <c r="E8" s="309" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="F8" s="312" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1">
       <c r="B9" s="71" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C9" s="228" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D9" s="313"/>
       <c r="E9" s="310"/>
       <c r="F9" s="311" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="111" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C10" s="107"/>
       <c r="D10" s="288"/>
@@ -12595,7 +12589,7 @@
       </c>
       <c r="D11" s="287"/>
       <c r="E11" s="9" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="F11" s="304"/>
     </row>
@@ -12628,7 +12622,7 @@
   <dimension ref="B2:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12641,7 +12635,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="20">
       <c r="B2" s="22" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -12654,7 +12648,7 @@
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="345" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C5" s="346"/>
       <c r="D5" s="346"/>
@@ -12688,10 +12682,10 @@
         <v>40</v>
       </c>
       <c r="D9" s="221" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E9" s="273" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -12795,7 +12789,7 @@
     <row r="19" spans="2:5" ht="15" customHeight="1">
       <c r="B19" s="112"/>
       <c r="C19" s="163" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D19" s="217" t="str">
         <f>IF(ISNUMBER(Dashboard!E25),Dashboard!E25,"-")</f>
@@ -12851,7 +12845,7 @@
     <row r="23" spans="2:5" ht="15" customHeight="1">
       <c r="B23" s="112"/>
       <c r="C23" s="163" t="s">
-        <v>241</v>
+        <v>423</v>
       </c>
       <c r="D23" s="217" t="str">
         <f>IF(ISNUMBER(Dashboard!E29),Dashboard!E29,"-")</f>
@@ -13014,7 +13008,7 @@
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="58" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="229">
@@ -13027,10 +13021,10 @@
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="222" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C12" s="173" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D12" s="233">
         <f>-'Fuel aggregation'!K16</f>
@@ -13052,7 +13046,7 @@
       <c r="E13" s="214"/>
       <c r="F13" s="213"/>
       <c r="G13" s="59" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="2:7">
@@ -13086,7 +13080,7 @@
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="222" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="235">
@@ -13099,7 +13093,7 @@
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="58" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="231" t="e">
@@ -13109,7 +13103,7 @@
       <c r="E18" s="9"/>
       <c r="F18" s="15"/>
       <c r="G18" s="59" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="2:7">
@@ -13146,7 +13140,7 @@
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="222" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="237" t="e">
@@ -13162,7 +13156,7 @@
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="58" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="290" t="e">
@@ -13172,7 +13166,7 @@
       <c r="E23" s="291"/>
       <c r="F23" s="15"/>
       <c r="G23" s="59" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="16" thickBot="1">
@@ -13217,7 +13211,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="20">
       <c r="B2" s="22" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -13231,7 +13225,7 @@
     </row>
     <row r="5" spans="2:7" ht="30" customHeight="1">
       <c r="B5" s="342" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C5" s="351"/>
       <c r="D5" s="351"/>
@@ -13283,7 +13277,7 @@
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="58" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="229">
@@ -13299,7 +13293,7 @@
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="58" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C12" s="141"/>
       <c r="D12" s="229">
@@ -13356,7 +13350,7 @@
   <sheetData>
     <row r="2" spans="2:15" ht="20">
       <c r="B2" s="225" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C2" s="225"/>
       <c r="D2" s="225"/>
@@ -13389,7 +13383,7 @@
     </row>
     <row r="5" spans="2:15" ht="30" customHeight="1">
       <c r="B5" s="353" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C5" s="354"/>
       <c r="D5" s="354"/>
@@ -13401,7 +13395,7 @@
     <row r="6" spans="2:15" ht="16" thickBot="1"/>
     <row r="7" spans="2:15">
       <c r="B7" s="55" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="255"/>
@@ -13435,42 +13429,42 @@
     </row>
     <row r="9" spans="2:15" ht="30">
       <c r="B9" s="258" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C9" s="259"/>
       <c r="D9" s="260"/>
       <c r="E9" s="261" t="s">
+        <v>353</v>
+      </c>
+      <c r="F9" s="261" t="s">
+        <v>357</v>
+      </c>
+      <c r="G9" s="261" t="s">
+        <v>354</v>
+      </c>
+      <c r="H9" s="261" t="s">
+        <v>355</v>
+      </c>
+      <c r="I9" s="261" t="s">
         <v>359</v>
       </c>
-      <c r="F9" s="261" t="s">
+      <c r="J9" s="261" t="s">
+        <v>360</v>
+      </c>
+      <c r="K9" s="261" t="s">
+        <v>368</v>
+      </c>
+      <c r="L9" s="261" t="s">
+        <v>361</v>
+      </c>
+      <c r="M9" s="261" t="s">
+        <v>362</v>
+      </c>
+      <c r="N9" s="261" t="s">
         <v>363</v>
       </c>
-      <c r="G9" s="261" t="s">
-        <v>360</v>
-      </c>
-      <c r="H9" s="261" t="s">
-        <v>361</v>
-      </c>
-      <c r="I9" s="261" t="s">
-        <v>365</v>
-      </c>
-      <c r="J9" s="261" t="s">
-        <v>366</v>
-      </c>
-      <c r="K9" s="261" t="s">
-        <v>374</v>
-      </c>
-      <c r="L9" s="261" t="s">
-        <v>367</v>
-      </c>
-      <c r="M9" s="261" t="s">
-        <v>368</v>
-      </c>
-      <c r="N9" s="261" t="s">
-        <v>369</v>
-      </c>
       <c r="O9" s="262" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
     </row>
     <row r="10" spans="2:15">
@@ -13595,7 +13589,7 @@
     </row>
     <row r="15" spans="2:15">
       <c r="B15" s="263" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C15" s="268" t="s">
         <v>194</v>
@@ -13681,7 +13675,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13691,7 +13685,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -13702,12 +13696,12 @@
         <v>197</v>
       </c>
       <c r="C2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B3" s="88">
         <f>IF(ISNUMBER('Production analysis'!D17),'Production analysis'!D17,"")</f>
@@ -13720,7 +13714,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="50" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4" s="88">
         <f>IF(ISNUMBER('Production analysis'!D18),'Production analysis'!D18,"")</f>
@@ -13733,7 +13727,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="50" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B5" s="88" t="str">
         <f>IF(ISNUMBER('Production analysis'!D19),'Production analysis'!D19,"")</f>
@@ -13746,7 +13740,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="50" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="B6" s="88" t="e">
         <f>'Greengas analysis'!D23</f>
@@ -13755,7 +13749,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="50" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B7" s="88">
         <f>IF(ISNUMBER('Production analysis'!D20),'Production analysis'!D20,"")</f>
@@ -13768,7 +13762,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B8" s="88">
         <f>IF(ISNUMBER('Production analysis'!D21),'Production analysis'!D21,"")</f>
@@ -13781,7 +13775,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="50" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B9" s="88" t="str">
         <f>IF(ISNUMBER('Production analysis'!D22),'Production analysis'!D22,"")</f>
@@ -13794,7 +13788,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="50" t="s">
-        <v>251</v>
+        <v>426</v>
       </c>
       <c r="B10" s="88" t="str">
         <f>IF(ISNUMBER('Production analysis'!D23),'Production analysis'!D23,"")</f>
@@ -13807,7 +13801,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="50" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B11" s="88" t="str">
         <f>IF(ISNUMBER('Production analysis'!D24),'Production analysis'!D24,"")</f>
@@ -13820,7 +13814,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="50" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B12" s="88" t="str">
         <f>IF(ISNUMBER('Production analysis'!D25),'Production analysis'!D25,"")</f>
@@ -13833,7 +13827,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="50" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B13" s="88" t="str">
         <f>IF(ISNUMBER('Production analysis'!D26),'Production analysis'!D26,"")</f>
@@ -14066,7 +14060,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -14074,7 +14068,7 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -14727,7 +14721,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -14735,7 +14729,7 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -15386,7 +15380,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -15394,7 +15388,7 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -16045,7 +16039,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -16053,7 +16047,7 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -16736,7 +16730,7 @@
         <v>41488</v>
       </c>
       <c r="C7" s="240" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D7" s="245">
         <v>0.2</v>
@@ -16747,7 +16741,7 @@
         <v>41491</v>
       </c>
       <c r="C8" s="240" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D8" s="245">
         <v>0.3</v>
@@ -16758,7 +16752,7 @@
         <v>41492</v>
       </c>
       <c r="C9" s="240" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D9" s="245">
         <v>0.4</v>
@@ -16769,7 +16763,7 @@
         <v>41494</v>
       </c>
       <c r="C10" s="240" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D10" s="245">
         <v>0.5</v>
@@ -16780,7 +16774,7 @@
         <v>41498</v>
       </c>
       <c r="C11" s="240" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D11" s="245">
         <v>0.6</v>
@@ -16791,7 +16785,7 @@
         <v>41499</v>
       </c>
       <c r="C12" s="240" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D12" s="245">
         <v>0.7</v>
@@ -16802,7 +16796,7 @@
         <v>41500</v>
       </c>
       <c r="C13" s="240" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D13" s="245">
         <v>0.8</v>
@@ -16813,7 +16807,7 @@
         <v>41500</v>
       </c>
       <c r="C14" s="242" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D14" s="245">
         <v>0.9</v>
@@ -16824,7 +16818,7 @@
         <v>41500</v>
       </c>
       <c r="C15" s="240" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D15" s="245">
         <v>1</v>
@@ -16835,7 +16829,7 @@
         <v>41500</v>
       </c>
       <c r="C16" s="247" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D16" s="245">
         <v>1.01</v>
@@ -16846,7 +16840,7 @@
         <v>41501</v>
       </c>
       <c r="C17" s="240" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D17" s="245">
         <v>1.02</v>
@@ -16857,7 +16851,7 @@
         <v>41502</v>
       </c>
       <c r="C18" s="242" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D18" s="245">
         <v>1.03</v>
@@ -16868,7 +16862,7 @@
         <v>41505</v>
       </c>
       <c r="C19" s="240" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="D19" s="245">
         <v>1.04</v>
@@ -16879,7 +16873,7 @@
         <v>41505</v>
       </c>
       <c r="C20" s="240" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D20" s="245">
         <v>1.05</v>
@@ -16890,7 +16884,7 @@
         <v>41506</v>
       </c>
       <c r="C21" s="242" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="D21" s="245">
         <v>1.06</v>
@@ -16901,7 +16895,7 @@
         <v>41507</v>
       </c>
       <c r="C22" s="247" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="D22" s="301">
         <v>1.07</v>
@@ -16912,7 +16906,7 @@
         <v>41509</v>
       </c>
       <c r="C23" s="247" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="D23" s="301">
         <v>1.08</v>
@@ -16923,7 +16917,7 @@
         <v>41514</v>
       </c>
       <c r="C24" s="247" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="D24" s="301">
         <v>1.0900000000000001</v>
@@ -16934,7 +16928,7 @@
         <v>41519</v>
       </c>
       <c r="C25" s="247" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="D25" s="301">
         <v>1.1000000000000001</v>
@@ -16945,7 +16939,7 @@
         <v>41520</v>
       </c>
       <c r="C26" s="247" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D26" s="301">
         <v>1.1100000000000001</v>
@@ -16956,7 +16950,7 @@
         <v>41521</v>
       </c>
       <c r="C27" s="247" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="D27" s="301">
         <v>1.1200000000000001</v>
@@ -16967,7 +16961,7 @@
         <v>41521</v>
       </c>
       <c r="C28" s="247" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="D28" s="301">
         <v>1.1299999999999999</v>
@@ -16978,10 +16972,10 @@
         <v>41534</v>
       </c>
       <c r="C29" s="247" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="D29" s="301" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="45">
@@ -16989,18 +16983,18 @@
         <v>41555</v>
       </c>
       <c r="C30" s="247" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="D30" s="301" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="318" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="C31" s="319" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="D31" s="320">
         <v>1.1399999999999999</v>
@@ -17011,7 +17005,7 @@
         <v>41681</v>
       </c>
       <c r="C32" s="247" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="D32" s="301">
         <v>1.1499999999999999</v>
@@ -17022,7 +17016,7 @@
         <v>41688</v>
       </c>
       <c r="C33" s="247" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="D33" s="301">
         <v>1.1599999999999999</v>
@@ -17107,7 +17101,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -17115,7 +17109,7 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -17766,7 +17760,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="99" t="s">
-        <v>399</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -17774,7 +17768,7 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -18418,7 +18412,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -18431,7 +18425,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B3">
         <f>Dashboard!E47</f>
@@ -18440,7 +18434,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B4">
         <f>Dashboard!E48</f>
@@ -18472,7 +18466,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -18485,7 +18479,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B3">
         <f>'Waste analysis'!E12</f>
@@ -18494,7 +18488,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B4">
         <f>'Waste analysis'!E11</f>
@@ -18518,7 +18512,9 @@
   </sheetPr>
   <dimension ref="B2:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -18554,7 +18550,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="331" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18562,7 +18558,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="329" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18570,7 +18566,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="329" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18578,7 +18574,7 @@
         <v>208</v>
       </c>
       <c r="C9" s="329" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18586,7 +18582,7 @@
         <v>24</v>
       </c>
       <c r="C10" s="329" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18594,15 +18590,15 @@
         <v>29</v>
       </c>
       <c r="C11" s="329" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B12" s="184" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C12" s="329" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
     </row>
     <row r="13" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18610,23 +18606,23 @@
         <v>235</v>
       </c>
       <c r="C13" s="279" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="14" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B14" s="184" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C14" s="279" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B15" s="185" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C15" s="329" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
@@ -18634,95 +18630,95 @@
         <v>227</v>
       </c>
       <c r="C16" s="329" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="17" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B17" s="185" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C17" s="329" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="18" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B18" s="278" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C18" s="279" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B19" s="186" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C19" s="329" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B20" s="186" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C20" s="329" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B21" s="186" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C21" s="329" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B22" s="186" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C22" s="329" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B23" s="186" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C23" s="329" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B24" s="186" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C24" s="329" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B25" s="186" t="s">
-        <v>354</v>
+        <v>428</v>
       </c>
       <c r="C25" s="330" t="s">
-        <v>268</v>
+        <v>429</v>
       </c>
     </row>
     <row r="26" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B26" s="186" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C26" s="330" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="27" spans="2:3" s="181" customFormat="1" ht="30" customHeight="1">
       <c r="B27" s="186" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C27" s="330" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -18772,7 +18768,7 @@
     </row>
     <row r="6" spans="2:3" ht="150">
       <c r="B6" s="333" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="C6" s="9"/>
     </row>
@@ -18796,49 +18792,49 @@
     </row>
     <row r="11" spans="2:3" ht="15" customHeight="1">
       <c r="B11" s="325" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="C11" s="9"/>
     </row>
     <row r="12" spans="2:3" ht="15" customHeight="1">
       <c r="B12" s="325" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C12" s="9"/>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1">
       <c r="B13" s="325" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C13" s="9"/>
     </row>
     <row r="14" spans="2:3" ht="15" customHeight="1">
       <c r="B14" s="325" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C14" s="9"/>
     </row>
     <row r="15" spans="2:3" ht="15" customHeight="1">
       <c r="B15" s="325" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C15" s="9"/>
     </row>
     <row r="16" spans="2:3" ht="30" customHeight="1">
       <c r="B16" s="333" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C16" s="9"/>
     </row>
     <row r="17" spans="2:3" ht="15" customHeight="1">
       <c r="B17" s="325" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="C17" s="9"/>
     </row>
     <row r="18" spans="2:3" ht="15" customHeight="1">
       <c r="B18" s="325" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="C18" s="9"/>
     </row>
@@ -18851,7 +18847,7 @@
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="187" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -18859,7 +18855,7 @@
     </row>
     <row r="23" spans="2:3" ht="90">
       <c r="B23" s="327" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="24" spans="2:3">
@@ -18894,7 +18890,7 @@
   <sheetData>
     <row r="2" spans="2:78" ht="21" customHeight="1">
       <c r="B2" s="82" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C2" s="77"/>
       <c r="D2" s="77"/>
@@ -19315,7 +19311,9 @@
   </sheetPr>
   <dimension ref="A2:F93"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -19398,32 +19396,32 @@
       <c r="A11" s="100"/>
       <c r="B11" s="112"/>
       <c r="C11" s="114" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D11" s="113"/>
     </row>
     <row r="12" spans="1:6" ht="31" customHeight="1">
       <c r="B12" s="112"/>
       <c r="C12" s="65" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D12" s="204" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="31" customHeight="1">
       <c r="B13" s="70"/>
       <c r="C13" s="114" t="s">
-        <v>272</v>
+        <v>430</v>
       </c>
       <c r="D13" s="204" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30">
       <c r="B14" s="70"/>
       <c r="C14" s="114" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D14" s="188"/>
       <c r="F14" s="89"/>
@@ -19431,7 +19429,7 @@
     <row r="15" spans="1:6" ht="30">
       <c r="B15" s="70"/>
       <c r="C15" s="114" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="D15" s="188"/>
       <c r="F15" s="89"/>
@@ -19474,28 +19472,28 @@
         <v>233</v>
       </c>
       <c r="C21" s="196" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D21" s="110"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="111"/>
       <c r="C22" s="197" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D22" s="74"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="112"/>
       <c r="C23" s="114" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D23" s="198"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="112"/>
       <c r="C24" s="114" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="D24" s="188"/>
     </row>
@@ -19506,24 +19504,24 @@
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="202" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C26" s="196" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D26" s="203"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="202"/>
       <c r="C27" s="197" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D27" s="188"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="202"/>
       <c r="C28" s="197" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D28" s="188"/>
     </row>
@@ -19534,17 +19532,17 @@
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="202" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C30" s="197" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D30" s="198"/>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="112"/>
       <c r="C31" s="197" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D31" s="198"/>
     </row>
@@ -19572,10 +19570,10 @@
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="108" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C36" s="116" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D36" s="90"/>
     </row>
@@ -19686,7 +19684,7 @@
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="111" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C52" s="74" t="s">
         <v>42</v>
@@ -20024,7 +20022,7 @@
         <v>29</v>
       </c>
       <c r="K2" s="126" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="L2" s="13"/>
       <c r="M2" s="5"/>
@@ -20056,7 +20054,7 @@
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1">
       <c r="B5" s="338" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="C5" s="339"/>
       <c r="D5" s="339"/>
@@ -20154,7 +20152,7 @@
       </c>
       <c r="F11" s="321"/>
       <c r="G11" s="321" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H11" s="321"/>
       <c r="I11" s="321" t="s">
@@ -20172,10 +20170,10 @@
       </c>
       <c r="N11" s="18"/>
       <c r="O11" s="136" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="P11" s="137" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="Q11" s="9"/>
     </row>
@@ -20208,7 +20206,7 @@
       <c r="E13" s="107"/>
       <c r="F13" s="107"/>
       <c r="G13" s="196" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="H13" s="107"/>
       <c r="I13" s="109"/>
@@ -20226,7 +20224,7 @@
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="135" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="P13" s="132"/>
       <c r="Q13" s="9"/>
@@ -20234,13 +20232,13 @@
     <row r="14" spans="2:17">
       <c r="B14" s="61"/>
       <c r="C14" s="151" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D14" s="153"/>
       <c r="E14" s="107"/>
       <c r="F14" s="107"/>
       <c r="G14" s="196" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="H14" s="107"/>
       <c r="I14" s="107"/>
@@ -20258,7 +20256,7 @@
       </c>
       <c r="N14" s="9"/>
       <c r="O14" s="135" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="P14" s="254" t="b">
         <f>L14</f>
@@ -20311,7 +20309,7 @@
         <v>41</v>
       </c>
       <c r="D17" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E17" s="323" t="e">
         <f>VLOOKUP(base_year,Timecurves!B10:H50, 2)</f>
@@ -20325,7 +20323,7 @@
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="15" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="L17" s="316" t="e">
         <f>IF(ABS((E17-'Fuel aggregation'!E11))&lt;=0.1*'Fuel aggregation'!E11,TRUE,FALSE)</f>
@@ -20346,7 +20344,7 @@
         <v>137</v>
       </c>
       <c r="D18" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E18" s="323" t="e">
         <f>VLOOKUP(base_year,Timecurves!B10:H50, 3)</f>
@@ -20360,7 +20358,7 @@
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="15" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="L18" s="316" t="e">
         <f>IF(ABS((E18-'Fuel aggregation'!F11))&lt;=0.1*'Fuel aggregation'!F11,TRUE,FALSE)</f>
@@ -20381,7 +20379,7 @@
         <v>42</v>
       </c>
       <c r="D19" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E19" s="317" t="e">
         <f>VLOOKUP(base_year,Timecurves!B10:H50, 4)</f>
@@ -20395,7 +20393,7 @@
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="15" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="L19" s="316" t="e">
         <f>IF(ABS((E19-'Fuel aggregation'!G11))&lt;=0.1*'Fuel aggregation'!G11,TRUE,FALSE)</f>
@@ -20416,7 +20414,7 @@
         <v>150</v>
       </c>
       <c r="D20" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E20" s="317" t="e">
         <f>VLOOKUP(base_year,Timecurves!B10:H50, 5)</f>
@@ -20430,7 +20428,7 @@
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="15" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="L20" s="316" t="e">
         <f>IF(ABS((E20-'Fuel aggregation'!H11))&lt;=0.1*'Fuel aggregation'!H11,TRUE,FALSE)</f>
@@ -20451,7 +20449,7 @@
         <v>234</v>
       </c>
       <c r="D21" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E21" s="317" t="e">
         <f>VLOOKUP(base_year,Timecurves!B10:H50, 6)</f>
@@ -20496,7 +20494,7 @@
         <v>236</v>
       </c>
       <c r="D23" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E23" s="177">
         <f>'Fuel aggregation'!L11</f>
@@ -20506,7 +20504,7 @@
       <c r="G23" s="161"/>
       <c r="H23" s="161"/>
       <c r="I23" s="107" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="15"/>
@@ -20523,7 +20521,7 @@
         <v>237</v>
       </c>
       <c r="D24" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E24" s="177">
         <f>'Fuel aggregation'!M11</f>
@@ -20533,7 +20531,7 @@
       <c r="G24" s="161"/>
       <c r="H24" s="161"/>
       <c r="I24" s="107" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="15"/>
@@ -20547,10 +20545,10 @@
     <row r="25" spans="2:17" ht="16" thickBot="1">
       <c r="B25" s="58"/>
       <c r="C25" s="155" t="s">
+        <v>241</v>
+      </c>
+      <c r="D25" s="141" t="s">
         <v>242</v>
-      </c>
-      <c r="D25" s="141" t="s">
-        <v>243</v>
       </c>
       <c r="E25" s="162"/>
       <c r="F25" s="161"/>
@@ -20563,7 +20561,7 @@
       <c r="M25" s="59"/>
       <c r="N25" s="9"/>
       <c r="O25" s="135" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="P25" s="132"/>
       <c r="Q25" s="9"/>
@@ -20574,7 +20572,7 @@
         <v>202</v>
       </c>
       <c r="D26" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E26" s="177">
         <f>'Fuel aggregation'!I11</f>
@@ -20584,7 +20582,7 @@
       <c r="G26" s="161"/>
       <c r="H26" s="161"/>
       <c r="I26" s="107" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="15"/>
@@ -20601,7 +20599,7 @@
         <v>219</v>
       </c>
       <c r="D27" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E27" s="177">
         <f>'Fuel aggregation'!J11</f>
@@ -20611,7 +20609,7 @@
       <c r="G27" s="161"/>
       <c r="H27" s="161"/>
       <c r="I27" s="107" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="15"/>
@@ -20628,10 +20626,10 @@
         <v>196</v>
       </c>
       <c r="D28" s="164" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E28" s="165" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F28" s="161"/>
       <c r="G28" s="161"/>
@@ -20649,13 +20647,13 @@
     <row r="29" spans="2:17">
       <c r="B29" s="58"/>
       <c r="C29" s="163" t="s">
-        <v>312</v>
+        <v>423</v>
       </c>
       <c r="D29" s="164" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E29" s="165" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F29" s="161"/>
       <c r="G29" s="161"/>
@@ -20676,10 +20674,10 @@
         <v>239</v>
       </c>
       <c r="D30" s="164" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E30" s="156" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F30" s="159"/>
       <c r="G30" s="159"/>
@@ -20700,10 +20698,10 @@
         <v>238</v>
       </c>
       <c r="D31" s="164" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E31" s="165" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F31" s="161"/>
       <c r="G31" s="161"/>
@@ -20724,7 +20722,7 @@
         <v>240</v>
       </c>
       <c r="D32" s="164" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E32" s="162"/>
       <c r="F32" s="161"/>
@@ -20737,7 +20735,7 @@
       <c r="M32" s="59"/>
       <c r="N32" s="9"/>
       <c r="O32" s="135" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="P32" s="132"/>
       <c r="Q32" s="9"/>
@@ -20787,10 +20785,10 @@
         <v>236</v>
       </c>
       <c r="D35" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E35" s="165" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F35" s="161"/>
       <c r="G35" s="161"/>
@@ -20811,10 +20809,10 @@
         <v>237</v>
       </c>
       <c r="D36" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E36" s="165" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F36" s="161"/>
       <c r="G36" s="161"/>
@@ -20832,13 +20830,13 @@
     <row r="37" spans="2:17" ht="16" thickBot="1">
       <c r="B37" s="61"/>
       <c r="C37" s="155" t="s">
+        <v>241</v>
+      </c>
+      <c r="D37" s="141" t="s">
         <v>242</v>
       </c>
-      <c r="D37" s="141" t="s">
-        <v>243</v>
-      </c>
       <c r="E37" s="165" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F37" s="161"/>
       <c r="G37" s="161"/>
@@ -20859,7 +20857,7 @@
         <v>202</v>
       </c>
       <c r="D38" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E38" s="251"/>
       <c r="F38" s="161"/>
@@ -20872,7 +20870,7 @@
       <c r="M38" s="59"/>
       <c r="N38" s="9"/>
       <c r="O38" s="135" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="P38" s="132"/>
       <c r="Q38" s="9"/>
@@ -20883,7 +20881,7 @@
         <v>219</v>
       </c>
       <c r="D39" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E39" s="252"/>
       <c r="F39" s="161"/>
@@ -20896,7 +20894,7 @@
       <c r="M39" s="59"/>
       <c r="N39" s="9"/>
       <c r="O39" s="135" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="P39" s="132"/>
       <c r="Q39" s="9"/>
@@ -20907,10 +20905,10 @@
         <v>196</v>
       </c>
       <c r="D40" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E40" s="165" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F40" s="161"/>
       <c r="G40" s="161"/>
@@ -20928,10 +20926,10 @@
     <row r="41" spans="2:17">
       <c r="B41" s="61"/>
       <c r="C41" s="163" t="s">
-        <v>312</v>
+        <v>423</v>
       </c>
       <c r="D41" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E41" s="177" t="e">
         <f>VLOOKUP(base_year,Timecurves!B10:H50, 7)</f>
@@ -20958,10 +20956,10 @@
         <v>239</v>
       </c>
       <c r="D42" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E42" s="156" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F42" s="159"/>
       <c r="G42" s="159"/>
@@ -20982,10 +20980,10 @@
         <v>238</v>
       </c>
       <c r="D43" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E43" s="165" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F43" s="161"/>
       <c r="G43" s="161"/>
@@ -21006,10 +21004,10 @@
         <v>240</v>
       </c>
       <c r="D44" s="141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E44" s="165" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F44" s="161"/>
       <c r="G44" s="161"/>
@@ -21044,7 +21042,7 @@
     </row>
     <row r="46" spans="2:17" ht="16" thickBot="1">
       <c r="B46" s="73" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="141"/>
@@ -21065,7 +21063,7 @@
     <row r="47" spans="2:17" ht="16" thickBot="1">
       <c r="B47" s="61"/>
       <c r="C47" s="9" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D47" s="141"/>
       <c r="E47" s="168"/>
@@ -21075,7 +21073,7 @@
       <c r="I47" s="324"/>
       <c r="J47" s="9"/>
       <c r="K47" s="15" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="L47" s="315">
         <f>IF(SUM(E47:E48)=1,TRUE,SUM(E47:E48))</f>
@@ -21087,7 +21085,7 @@
       </c>
       <c r="N47" s="9"/>
       <c r="O47" s="135" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="P47" s="132">
         <f>IF(L47=TRUE,1,0)</f>
@@ -21098,7 +21096,7 @@
     <row r="48" spans="2:17" ht="16" thickBot="1">
       <c r="B48" s="61"/>
       <c r="C48" s="9" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D48" s="141"/>
       <c r="E48" s="169"/>
@@ -21112,7 +21110,7 @@
       <c r="M48" s="59"/>
       <c r="N48" s="9"/>
       <c r="O48" s="135" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="P48" s="132"/>
       <c r="Q48" s="9"/>
@@ -21303,7 +21301,7 @@
   <sheetData>
     <row r="2" spans="2:67" ht="20">
       <c r="B2" s="22" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C2" s="100"/>
       <c r="D2" s="100"/>
@@ -21354,7 +21352,7 @@
     </row>
     <row r="5" spans="2:67" ht="30">
       <c r="B5" s="179" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="W5" s="144"/>
       <c r="X5" s="144"/>
@@ -28176,7 +28174,7 @@
   <dimension ref="A2:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B5" sqref="B5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -28189,7 +28187,7 @@
   <sheetData>
     <row r="2" spans="2:9" ht="20">
       <c r="B2" s="22" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="2:9">
@@ -28208,7 +28206,7 @@
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1">
       <c r="B5" s="342" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="C5" s="343"/>
       <c r="D5" s="343"/>
@@ -28220,7 +28218,7 @@
     <row r="6" spans="2:9" ht="16" thickBot="1"/>
     <row r="7" spans="2:9">
       <c r="B7" s="55" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="C7" s="66"/>
       <c r="D7" s="66"/>
@@ -28240,7 +28238,7 @@
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="119" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C9" s="148" t="s">
         <v>41</v>
@@ -28258,7 +28256,7 @@
         <v>234</v>
       </c>
       <c r="H9" s="118" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
     </row>
     <row r="10" spans="2:9">

</xml_diff>

<commit_message>
Published state of ETDataset on 23 October 2015
</commit_message>
<xml_diff>
--- a/analyses/3_primary_production_analysis.xlsx
+++ b/analyses/3_primary_production_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="902" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="902" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="1" r:id="rId1"/>
@@ -13199,7 +13199,7 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q46" sqref="Q46"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13301,8 +13301,8 @@
         <v>0</v>
       </c>
       <c r="E12" s="238">
-        <f>IF(SUM($D$11:$D$12)=0,0,D12/SUM($D$11:$D$12))</f>
-        <v>0</v>
+        <f>IF(SUM($D$11:$D$12)=0,1,D12/SUM($D$11:$D$12))</f>
+        <v>1</v>
       </c>
       <c r="F12" s="224"/>
       <c r="G12" s="59"/>
@@ -18459,7 +18459,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18483,7 +18483,7 @@
       </c>
       <c r="B3">
         <f>'Waste analysis'!E12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
Published state of ETDataset on 12 April 2018
</commit_message>
<xml_diff>
--- a/analyses/3_primary_production_analysis.xlsx
+++ b/analyses/3_primary_production_analysis.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10319"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/analyses/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EC8C7B-2912-074D-96E0-D97841255533}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="902" firstSheet="20" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="46120" windowHeight="25780" tabRatio="902" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="1" r:id="rId1"/>
@@ -19,129 +25,124 @@
     <sheet name="technical_specs" sheetId="67" r:id="rId10"/>
     <sheet name="Production analysis" sheetId="49" r:id="rId11"/>
     <sheet name="Network_gas_analysis" sheetId="73" r:id="rId12"/>
-    <sheet name="Hydrogen_production_analysis" sheetId="78" r:id="rId13"/>
-    <sheet name="Waste analysis" sheetId="69" r:id="rId14"/>
-    <sheet name="Fuel aggregation" sheetId="72" r:id="rId15"/>
-    <sheet name="csv_carrier_domestic_production" sheetId="24" r:id="rId16"/>
-    <sheet name="csv_coal_time_curve" sheetId="57" r:id="rId17"/>
-    <sheet name="csv_lignite_time_curve" sheetId="60" r:id="rId18"/>
-    <sheet name="csv_natural_gas_time_curve" sheetId="61" r:id="rId19"/>
-    <sheet name="csv_crude_oil_time_curve" sheetId="63" r:id="rId20"/>
-    <sheet name="csv_uranium_oxide_time_curve" sheetId="62" r:id="rId21"/>
-    <sheet name="csv_woody_biomass_time_curve" sheetId="64" r:id="rId22"/>
-    <sheet name="csv_energy_distribution_wood_pa" sheetId="68" r:id="rId23"/>
-    <sheet name="csv_energy_distribution_waste_m" sheetId="70" r:id="rId24"/>
-    <sheet name="csv_green_gas_grid_child_share" sheetId="75" r:id="rId25"/>
-    <sheet name="csv_natural_gas_grid_child_shar" sheetId="74" r:id="rId26"/>
-    <sheet name="csv_hydrogen_distribution_share" sheetId="76" r:id="rId27"/>
-    <sheet name="csv_hydrogen_compressor_share" sheetId="77" r:id="rId28"/>
+    <sheet name="Waste analysis" sheetId="69" r:id="rId13"/>
+    <sheet name="Fuel aggregation" sheetId="72" r:id="rId14"/>
+    <sheet name="csv_carrier_domestic_production" sheetId="24" r:id="rId15"/>
+    <sheet name="csv_coal_time_curve" sheetId="57" r:id="rId16"/>
+    <sheet name="csv_lignite_time_curve" sheetId="60" r:id="rId17"/>
+    <sheet name="csv_natural_gas_time_curve" sheetId="61" r:id="rId18"/>
+    <sheet name="csv_crude_oil_time_curve" sheetId="63" r:id="rId19"/>
+    <sheet name="csv_uranium_oxide_time_curve" sheetId="62" r:id="rId20"/>
+    <sheet name="csv_woody_biomass_time_curve" sheetId="64" r:id="rId21"/>
+    <sheet name="csv_energy_distribution_wood_pa" sheetId="68" r:id="rId22"/>
+    <sheet name="csv_energy_distribution_waste_m" sheetId="70" r:id="rId23"/>
+    <sheet name="csv_green_gas_grid_child_share" sheetId="75" r:id="rId24"/>
+    <sheet name="csv_natural_gas_grid_child_shar" sheetId="74" r:id="rId25"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId26"/>
+    <externalReference r:id="rId27"/>
+    <externalReference r:id="rId28"/>
     <externalReference r:id="rId29"/>
-    <externalReference r:id="rId30"/>
-    <externalReference r:id="rId31"/>
-    <externalReference r:id="rId32"/>
   </externalReferences>
   <definedNames>
+    <definedName name="ap_subfuel_allo" localSheetId="16">#REF!</definedName>
     <definedName name="ap_subfuel_allo" localSheetId="17">#REF!</definedName>
-    <definedName name="ap_subfuel_allo" localSheetId="18">#REF!</definedName>
     <definedName name="ap_subfuel_allo" localSheetId="4">'[1]CEB allocation'!$F$12:$BC$12</definedName>
-    <definedName name="base_year" localSheetId="14">[2]Dashboard!$E$14</definedName>
+    <definedName name="base_year" localSheetId="13">[2]Dashboard!$E$14</definedName>
     <definedName name="base_year" localSheetId="9">[3]Dashboard!$E$12</definedName>
     <definedName name="base_year">Dashboard!$E$14</definedName>
-    <definedName name="country" localSheetId="14">[2]Dashboard!$E$13</definedName>
+    <definedName name="country" localSheetId="13">[2]Dashboard!$E$13</definedName>
     <definedName name="country" localSheetId="9">[3]Dashboard!$E$11</definedName>
     <definedName name="country">Dashboard!$E$13</definedName>
-    <definedName name="Eff_Airco" localSheetId="14">'[4]Technological specifications'!$F$25</definedName>
-    <definedName name="Eff_Biomass_Heater" localSheetId="14">'[4]Technological specifications'!$F$19</definedName>
-    <definedName name="Eff_Centralized_Heater" localSheetId="14">'[4]Technological specifications'!#REF!</definedName>
-    <definedName name="Eff_Coal_Heater" localSheetId="14">'[4]Technological specifications'!$F$17</definedName>
-    <definedName name="Eff_Distr_Heater" localSheetId="14">'[4]Technological specifications'!$F$20</definedName>
-    <definedName name="Eff_Elec_Cold_Pump" localSheetId="14">'[4]Technological specifications'!$F$24</definedName>
-    <definedName name="Eff_Elec_Heat_Pump" localSheetId="14">'[4]Technological specifications'!$F$14</definedName>
-    <definedName name="Eff_Elec_Heater" localSheetId="14">'[4]Technological specifications'!$F$15</definedName>
-    <definedName name="Eff_Fluo_Lamp" localSheetId="14">'[4]Technological specifications'!$F$29</definedName>
-    <definedName name="Eff_Fluo_Tube" localSheetId="14">'[4]Technological specifications'!$F$30</definedName>
-    <definedName name="Eff_Gas_Cold_Pump" localSheetId="14">'[4]Technological specifications'!$F$23</definedName>
-    <definedName name="Eff_Gas_Heat_Pump" localSheetId="14">'[4]Technological specifications'!$F$13</definedName>
-    <definedName name="Eff_Gas_Heater" localSheetId="14">'[4]Technological specifications'!$F$12</definedName>
-    <definedName name="Eff_Geothermal_Heater" localSheetId="14">'[4]Technological specifications'!#REF!</definedName>
-    <definedName name="Eff_Incan_Lamp" localSheetId="14">'[4]Technological specifications'!$F$28</definedName>
-    <definedName name="Eff_LED_Lamp" localSheetId="14">'[4]Technological specifications'!$F$31</definedName>
-    <definedName name="Eff_Oil_Heater" localSheetId="14">'[4]Technological specifications'!$F$18</definedName>
-    <definedName name="Eff_Solar_Heater" localSheetId="14">'[4]Technological specifications'!$F$16</definedName>
+    <definedName name="Eff_Airco" localSheetId="13">'[4]Technological specifications'!$F$25</definedName>
+    <definedName name="Eff_Biomass_Heater" localSheetId="13">'[4]Technological specifications'!$F$19</definedName>
+    <definedName name="Eff_Centralized_Heater" localSheetId="13">'[4]Technological specifications'!#REF!</definedName>
+    <definedName name="Eff_Coal_Heater" localSheetId="13">'[4]Technological specifications'!$F$17</definedName>
+    <definedName name="Eff_Distr_Heater" localSheetId="13">'[4]Technological specifications'!$F$20</definedName>
+    <definedName name="Eff_Elec_Cold_Pump" localSheetId="13">'[4]Technological specifications'!$F$24</definedName>
+    <definedName name="Eff_Elec_Heat_Pump" localSheetId="13">'[4]Technological specifications'!$F$14</definedName>
+    <definedName name="Eff_Elec_Heater" localSheetId="13">'[4]Technological specifications'!$F$15</definedName>
+    <definedName name="Eff_Fluo_Lamp" localSheetId="13">'[4]Technological specifications'!$F$29</definedName>
+    <definedName name="Eff_Fluo_Tube" localSheetId="13">'[4]Technological specifications'!$F$30</definedName>
+    <definedName name="Eff_Gas_Cold_Pump" localSheetId="13">'[4]Technological specifications'!$F$23</definedName>
+    <definedName name="Eff_Gas_Heat_Pump" localSheetId="13">'[4]Technological specifications'!$F$13</definedName>
+    <definedName name="Eff_Gas_Heater" localSheetId="13">'[4]Technological specifications'!$F$12</definedName>
+    <definedName name="Eff_Geothermal_Heater" localSheetId="13">'[4]Technological specifications'!#REF!</definedName>
+    <definedName name="Eff_Incan_Lamp" localSheetId="13">'[4]Technological specifications'!$F$28</definedName>
+    <definedName name="Eff_LED_Lamp" localSheetId="13">'[4]Technological specifications'!$F$31</definedName>
+    <definedName name="Eff_Oil_Heater" localSheetId="13">'[4]Technological specifications'!$F$18</definedName>
+    <definedName name="Eff_Solar_Heater" localSheetId="13">'[4]Technological specifications'!$F$16</definedName>
+    <definedName name="ei_subsector_allo" localSheetId="16">#REF!</definedName>
     <definedName name="ei_subsector_allo" localSheetId="17">#REF!</definedName>
-    <definedName name="ei_subsector_allo" localSheetId="18">#REF!</definedName>
     <definedName name="ei_subsector_allo" localSheetId="4">'[1]CEB allocation'!$D$17:$D$33</definedName>
-    <definedName name="ei_subsector_allo" localSheetId="12">#REF!</definedName>
     <definedName name="ei_subsector_allo" localSheetId="10">#REF!</definedName>
     <definedName name="export_csv">"Button 2"</definedName>
-    <definedName name="Final_Demand_Comm_and_Publ_Services" localSheetId="14">'[4]Corrected energy balance'!$BN$84</definedName>
-    <definedName name="Final_Demand_Electrical_Appliances" localSheetId="14">'[4]Final demand per energy carrier'!$F$41</definedName>
-    <definedName name="Final_Demand_Lighting" localSheetId="14">[4]Dashboard!$D$26</definedName>
-    <definedName name="Final_Demand_Other_Appliances" localSheetId="14">[4]Dashboard!$D$29</definedName>
-    <definedName name="Final_Demand_Space_Cooling" localSheetId="14">[4]Dashboard!$D$25</definedName>
-    <definedName name="Final_demand_Space_Heating" localSheetId="14">[4]Dashboard!$D$24</definedName>
-    <definedName name="GWh_to_TJ" localSheetId="14">[4]Assumptions!$C$131</definedName>
-    <definedName name="Heat_eff_Biogas_CHP" localSheetId="14">'[4]Technological specifications'!#REF!</definedName>
-    <definedName name="Heat_Eff_Biomass_CHP" localSheetId="14">'[4]Technological specifications'!#REF!</definedName>
-    <definedName name="Heat_Eff_Gas_CHP" localSheetId="14">'[4]Technological specifications'!#REF!</definedName>
+    <definedName name="Final_Demand_Comm_and_Publ_Services" localSheetId="13">'[4]Corrected energy balance'!$BN$84</definedName>
+    <definedName name="Final_Demand_Electrical_Appliances" localSheetId="13">'[4]Final demand per energy carrier'!$F$41</definedName>
+    <definedName name="Final_Demand_Lighting" localSheetId="13">[4]Dashboard!$D$26</definedName>
+    <definedName name="Final_Demand_Other_Appliances" localSheetId="13">[4]Dashboard!$D$29</definedName>
+    <definedName name="Final_Demand_Space_Cooling" localSheetId="13">[4]Dashboard!$D$25</definedName>
+    <definedName name="Final_demand_Space_Heating" localSheetId="13">[4]Dashboard!$D$24</definedName>
+    <definedName name="GWh_to_TJ" localSheetId="13">[4]Assumptions!$C$131</definedName>
+    <definedName name="Heat_eff_Biogas_CHP" localSheetId="13">'[4]Technological specifications'!#REF!</definedName>
+    <definedName name="Heat_Eff_Biomass_CHP" localSheetId="13">'[4]Technological specifications'!#REF!</definedName>
+    <definedName name="Heat_Eff_Gas_CHP" localSheetId="13">'[4]Technological specifications'!#REF!</definedName>
+    <definedName name="i_subsector_allo" localSheetId="16">#REF!</definedName>
     <definedName name="i_subsector_allo" localSheetId="17">#REF!</definedName>
-    <definedName name="i_subsector_allo" localSheetId="18">#REF!</definedName>
     <definedName name="i_subsector_allo" localSheetId="4">'[1]CEB allocation'!$D$37:$D$49</definedName>
-    <definedName name="i_subsector_allo" localSheetId="12">#REF!</definedName>
     <definedName name="i_subsector_allo" localSheetId="10">#REF!</definedName>
     <definedName name="import_ceb2">"Button 1"</definedName>
     <definedName name="kWh_MJ_conversion" localSheetId="4">[1]Assumptions!$C$176</definedName>
+    <definedName name="ma_subfuel_allo" localSheetId="16">#REF!</definedName>
     <definedName name="ma_subfuel_allo" localSheetId="17">#REF!</definedName>
-    <definedName name="ma_subfuel_allo" localSheetId="18">#REF!</definedName>
+    <definedName name="net_gross_conv" localSheetId="16">#REF!</definedName>
     <definedName name="net_gross_conv" localSheetId="17">#REF!</definedName>
-    <definedName name="net_gross_conv" localSheetId="18">#REF!</definedName>
     <definedName name="net_gross_conv" localSheetId="4">'[1]AP net-gross conversion'!$D$12</definedName>
-    <definedName name="Perc_Final_Demand_Lighting_Fluo_Lamps" localSheetId="14">'[4]Technology split of final deman'!$G$31</definedName>
-    <definedName name="Perc_Final_Demand_Lighting_Fluo_Tubes" localSheetId="14">'[4]Technology split of final deman'!$G$32</definedName>
-    <definedName name="Perc_Final_Demand_Lighting_Incan_Lamps" localSheetId="14">'[4]Technology split of final deman'!$G$30</definedName>
-    <definedName name="Perc_Final_Demand_Lighting_LED_Lamps" localSheetId="14">'[4]Technology split of final deman'!$G$33</definedName>
-    <definedName name="Perc_Final_Demand_Space_Cooling_Airco" localSheetId="14">'[4]Technology split of final deman'!$G$25</definedName>
-    <definedName name="Perc_Final_Demand_Space_Cooling_Elec_Heat_Pump" localSheetId="14">'[4]Technology split of final deman'!$G$24</definedName>
-    <definedName name="Perc_Final_Demand_Space_Cooling_Gas_Heat_Pump" localSheetId="14">'[4]Technology split of final deman'!$G$23</definedName>
-    <definedName name="Perc_Final_Demand_Space_Heating_Biomass_Heater" localSheetId="14">'[4]Technology split of final deman'!$G$17</definedName>
-    <definedName name="Perc_Final_Demand_Space_Heating_Coal_Heater" localSheetId="14">'[4]Technology split of final deman'!$G$13</definedName>
-    <definedName name="Perc_Final_Demand_Space_Heating_District_Heating" localSheetId="14">'[4]Technology split of final deman'!$G$16</definedName>
-    <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heat_Pump" localSheetId="14">'[4]Technology split of final deman'!$G$11</definedName>
-    <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heater" localSheetId="14">'[4]Technology split of final deman'!$G$12</definedName>
-    <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heat_Pump" localSheetId="14">'[4]Technology split of final deman'!$G$10</definedName>
-    <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heater" localSheetId="14">'[4]Technology split of final deman'!$G$9</definedName>
-    <definedName name="Perc_Final_Demand_Space_Heating_Oil_Heater" localSheetId="14">'[4]Technology split of final deman'!$G$14</definedName>
-    <definedName name="Perc_Final_Demand_Space_Heating_Solar_Heater" localSheetId="14">'[4]Technology split of final deman'!$G$18</definedName>
-    <definedName name="Perc_Heat_Delivered_Biomass_Heater" localSheetId="14">'[4]Tech split of useful demand'!$G$17</definedName>
-    <definedName name="Perc_Heat_Delivered_District_Heat" localSheetId="14">'[4]Tech split of useful demand'!$G$16</definedName>
-    <definedName name="Perc_Heat_Delivered_Solar_Thermal" localSheetId="14">'[4]Tech split of useful demand'!$G$18</definedName>
-    <definedName name="Perc_Roof_for_PV" localSheetId="14">'[4]PV solar area and production'!$E$22</definedName>
-    <definedName name="Share_Lighting_Fluorescent_Lamp" localSheetId="14">'[4]Shares per tech per carrier'!$E$22</definedName>
-    <definedName name="Share_Lighting_Fluorescent_Tube" localSheetId="14">'[4]Shares per tech per carrier'!$E$23</definedName>
-    <definedName name="Share_Lighting_Incandescent_Lamp" localSheetId="14">'[4]Shares per tech per carrier'!$E$21</definedName>
-    <definedName name="Share_Lighting_LED" localSheetId="14">'[4]Shares per tech per carrier'!$E$24</definedName>
-    <definedName name="Share_Space_Cooling_Electric_Airco" localSheetId="14">'[4]Shares per tech per carrier'!$E$18</definedName>
-    <definedName name="Share_Space_Cooling_Electric_Heat_Pump" localSheetId="14">'[4]Shares per tech per carrier'!$E$17</definedName>
-    <definedName name="Share_Space_Heating_Electric_Heat_Pump" localSheetId="14">'[4]Shares per tech per carrier'!$E$13</definedName>
-    <definedName name="Share_Space_Heating_Electric_Heater" localSheetId="14">'[4]Shares per tech per carrier'!$E$14</definedName>
-    <definedName name="Share_Space_Heating_Network_Gas_Heat_Pump" localSheetId="14">'[4]Shares per tech per carrier'!$E$10</definedName>
-    <definedName name="Share_Space_Heating_Network_Gas_Heater" localSheetId="14">'[4]Shares per tech per carrier'!$E$9</definedName>
-    <definedName name="Solar_PV_Roof_CaPS" localSheetId="14">'[4]PV solar area and production'!$E$13</definedName>
-    <definedName name="Solar_PV_Roof_Residential" localSheetId="14">'[4]IEA autoproducer prod.'!$AO$10</definedName>
-    <definedName name="Solar_PV_Roof_Total" localSheetId="14">'[4]Corrected energy balance'!$BG$95</definedName>
+    <definedName name="Perc_Final_Demand_Lighting_Fluo_Lamps" localSheetId="13">'[4]Technology split of final deman'!$G$31</definedName>
+    <definedName name="Perc_Final_Demand_Lighting_Fluo_Tubes" localSheetId="13">'[4]Technology split of final deman'!$G$32</definedName>
+    <definedName name="Perc_Final_Demand_Lighting_Incan_Lamps" localSheetId="13">'[4]Technology split of final deman'!$G$30</definedName>
+    <definedName name="Perc_Final_Demand_Lighting_LED_Lamps" localSheetId="13">'[4]Technology split of final deman'!$G$33</definedName>
+    <definedName name="Perc_Final_Demand_Space_Cooling_Airco" localSheetId="13">'[4]Technology split of final deman'!$G$25</definedName>
+    <definedName name="Perc_Final_Demand_Space_Cooling_Elec_Heat_Pump" localSheetId="13">'[4]Technology split of final deman'!$G$24</definedName>
+    <definedName name="Perc_Final_Demand_Space_Cooling_Gas_Heat_Pump" localSheetId="13">'[4]Technology split of final deman'!$G$23</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Biomass_Heater" localSheetId="13">'[4]Technology split of final deman'!$G$17</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Coal_Heater" localSheetId="13">'[4]Technology split of final deman'!$G$13</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_District_Heating" localSheetId="13">'[4]Technology split of final deman'!$G$16</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heat_Pump" localSheetId="13">'[4]Technology split of final deman'!$G$11</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heater" localSheetId="13">'[4]Technology split of final deman'!$G$12</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heat_Pump" localSheetId="13">'[4]Technology split of final deman'!$G$10</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heater" localSheetId="13">'[4]Technology split of final deman'!$G$9</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Oil_Heater" localSheetId="13">'[4]Technology split of final deman'!$G$14</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Solar_Heater" localSheetId="13">'[4]Technology split of final deman'!$G$18</definedName>
+    <definedName name="Perc_Heat_Delivered_Biomass_Heater" localSheetId="13">'[4]Tech split of useful demand'!$G$17</definedName>
+    <definedName name="Perc_Heat_Delivered_District_Heat" localSheetId="13">'[4]Tech split of useful demand'!$G$16</definedName>
+    <definedName name="Perc_Heat_Delivered_Solar_Thermal" localSheetId="13">'[4]Tech split of useful demand'!$G$18</definedName>
+    <definedName name="Perc_Roof_for_PV" localSheetId="13">'[4]PV solar area and production'!$E$22</definedName>
+    <definedName name="Share_Lighting_Fluorescent_Lamp" localSheetId="13">'[4]Shares per tech per carrier'!$E$22</definedName>
+    <definedName name="Share_Lighting_Fluorescent_Tube" localSheetId="13">'[4]Shares per tech per carrier'!$E$23</definedName>
+    <definedName name="Share_Lighting_Incandescent_Lamp" localSheetId="13">'[4]Shares per tech per carrier'!$E$21</definedName>
+    <definedName name="Share_Lighting_LED" localSheetId="13">'[4]Shares per tech per carrier'!$E$24</definedName>
+    <definedName name="Share_Space_Cooling_Electric_Airco" localSheetId="13">'[4]Shares per tech per carrier'!$E$18</definedName>
+    <definedName name="Share_Space_Cooling_Electric_Heat_Pump" localSheetId="13">'[4]Shares per tech per carrier'!$E$17</definedName>
+    <definedName name="Share_Space_Heating_Electric_Heat_Pump" localSheetId="13">'[4]Shares per tech per carrier'!$E$13</definedName>
+    <definedName name="Share_Space_Heating_Electric_Heater" localSheetId="13">'[4]Shares per tech per carrier'!$E$14</definedName>
+    <definedName name="Share_Space_Heating_Network_Gas_Heat_Pump" localSheetId="13">'[4]Shares per tech per carrier'!$E$10</definedName>
+    <definedName name="Share_Space_Heating_Network_Gas_Heater" localSheetId="13">'[4]Shares per tech per carrier'!$E$9</definedName>
+    <definedName name="Solar_PV_Roof_CaPS" localSheetId="13">'[4]PV solar area and production'!$E$13</definedName>
+    <definedName name="Solar_PV_Roof_Residential" localSheetId="13">'[4]IEA autoproducer prod.'!$AO$10</definedName>
+    <definedName name="Solar_PV_Roof_Total" localSheetId="13">'[4]Corrected energy balance'!$BG$95</definedName>
+    <definedName name="switch_decc" localSheetId="16">#REF!</definedName>
     <definedName name="switch_decc" localSheetId="17">#REF!</definedName>
-    <definedName name="switch_decc" localSheetId="18">#REF!</definedName>
     <definedName name="switch_decc" localSheetId="4">'[1]Fuel allocation'!$C$133</definedName>
+    <definedName name="switch_iea" localSheetId="16">#REF!</definedName>
     <definedName name="switch_iea" localSheetId="17">#REF!</definedName>
-    <definedName name="switch_iea" localSheetId="18">#REF!</definedName>
     <definedName name="switch_iea" localSheetId="4">'[1]Fuel allocation'!$C$91</definedName>
+    <definedName name="switch_protermo" localSheetId="16">#REF!</definedName>
     <definedName name="switch_protermo" localSheetId="17">#REF!</definedName>
-    <definedName name="switch_protermo" localSheetId="18">#REF!</definedName>
     <definedName name="switch_protermo" localSheetId="4">'[1]Fuel allocation'!$C$49</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentManualCount="2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -151,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="469">
   <si>
     <t>Changelog</t>
   </si>
@@ -1541,42 +1542,6 @@
     <t>regasified_bio_lng</t>
   </si>
   <si>
-    <t>energy_local_electrolysis_hydrogen</t>
-  </si>
-  <si>
-    <t>energy_distribution_hydrogen</t>
-  </si>
-  <si>
-    <t>energy_distribution_hydrogen_child_share</t>
-  </si>
-  <si>
-    <t>energy_steam_methane_reformer_ccs_hydrogen</t>
-  </si>
-  <si>
-    <t>energy_steam_methane_reformer_hydrogen</t>
-  </si>
-  <si>
-    <t>energy_biomass_gasification_ccs_hydrogen</t>
-  </si>
-  <si>
-    <t>energy_biomass_gasification_hydrogen</t>
-  </si>
-  <si>
-    <t>Hydrogen production for transport</t>
-  </si>
-  <si>
-    <t>Total hydrogen produced for transport</t>
-  </si>
-  <si>
-    <t>percentage_steam_methane_reforming</t>
-  </si>
-  <si>
-    <t>percentage_steam_methane_reforming_ccs</t>
-  </si>
-  <si>
-    <t>percentage_local_electrolysis</t>
-  </si>
-  <si>
     <t>January 19, 2016</t>
   </si>
   <si>
@@ -1599,63 +1564,12 @@
   </si>
   <si>
     <t>Child shares of local hydrogen production</t>
-  </si>
-  <si>
-    <t>On this page the hydrogen production shares are collected from the Dashboard, and divided into local and central production.</t>
-  </si>
-  <si>
-    <t>Production process</t>
-  </si>
-  <si>
-    <t>Share of total production</t>
-  </si>
-  <si>
-    <t>Steam methane reforming</t>
-  </si>
-  <si>
-    <t>Steam methane reforming CCS</t>
-  </si>
-  <si>
-    <t>Local electrolysis</t>
-  </si>
-  <si>
-    <t>Biomass gasification</t>
-  </si>
-  <si>
-    <t>Biomass gasification CCS</t>
-  </si>
-  <si>
-    <t>Share of central production</t>
-  </si>
-  <si>
-    <t>Local production</t>
-  </si>
-  <si>
-    <t>Central production</t>
-  </si>
-  <si>
-    <t>Local vs central production share</t>
-  </si>
-  <si>
-    <t>Hydrogen produced through steam methane reforming CCS percentage of total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydrogen produced through steam methane reforming percentage of total </t>
-  </si>
-  <si>
-    <t>Hydrogen produced through (local) electrolysis percentage of total</t>
-  </si>
-  <si>
-    <t>Hydrogen flow is currently statistically irrelevant</t>
-  </si>
-  <si>
-    <t>energy_locally_available_hydrogen_before_p2g_child_share</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1663,7 +1577,7 @@
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="31">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1713,6 +1627,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1736,17 +1651,20 @@
       <sz val="16"/>
       <color theme="3"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1760,6 +1678,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1773,6 +1692,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1780,12 +1700,14 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1793,12 +1715,14 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1811,29 +1735,34 @@
       <b/>
       <sz val="16"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1841,6 +1770,7 @@
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1848,16 +1778,19 @@
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1865,6 +1798,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -5479,7 +5413,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="377">
+  <cellXfs count="367">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -6091,10 +6025,6 @@
     <xf numFmtId="10" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="10" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -6107,30 +6037,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="25" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -9114,9 +9020,9 @@
     <cellStyle name="Hyperlink" xfId="2920" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="731" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="2521"/>
+    <cellStyle name="Percent 2" xfId="2521" xr:uid="{00000000-0005-0000-0000-0000690B0000}"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -9197,21 +9103,14 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCFFCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -9246,7 +9145,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="L-Shape 1"/>
+        <xdr:cNvPr id="2" name="L-Shape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9311,7 +9216,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9374,7 +9285,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle 3"/>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9439,7 +9356,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4"/>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9502,7 +9425,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9564,7 +9493,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9625,7 +9560,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 7"/>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9686,7 +9627,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 8"/>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9747,7 +9694,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="Straight Connector 9"/>
+        <xdr:cNvPr id="10" name="Straight Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -9797,7 +9750,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 10"/>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9866,7 +9825,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Straight Connector 11"/>
+        <xdr:cNvPr id="12" name="Straight Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -9916,7 +9881,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Rectangle 12"/>
+        <xdr:cNvPr id="13" name="Rectangle 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9972,7 +9943,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Rectangle 13"/>
+        <xdr:cNvPr id="14" name="Rectangle 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10028,7 +10005,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Straight Connector 14"/>
+        <xdr:cNvPr id="15" name="Straight Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -10078,7 +10061,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Rectangle 15"/>
+        <xdr:cNvPr id="16" name="Rectangle 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10134,7 +10123,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Rectangle 16"/>
+        <xdr:cNvPr id="17" name="Rectangle 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10195,7 +10190,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="Straight Arrow Connector 136"/>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 136">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="16" idx="3"/>
           <a:endCxn id="21" idx="1"/>
@@ -10245,7 +10246,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="Straight Arrow Connector 136"/>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 136">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="17" idx="3"/>
           <a:endCxn id="14" idx="1"/>
@@ -10295,7 +10302,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="Elbow Connector 70"/>
+        <xdr:cNvPr id="20" name="Elbow Connector 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="13" idx="3"/>
           <a:endCxn id="9" idx="1"/>
@@ -10345,7 +10358,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Rectangle 20"/>
+        <xdr:cNvPr id="21" name="Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10401,7 +10420,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Rectangle 21"/>
+        <xdr:cNvPr id="22" name="Rectangle 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10464,7 +10489,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Rectangle 22"/>
+        <xdr:cNvPr id="23" name="Rectangle 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10525,7 +10556,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="TextBox 24"/>
+        <xdr:cNvPr id="25" name="TextBox 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000019000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10588,7 +10625,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="TextBox 25"/>
+        <xdr:cNvPr id="26" name="TextBox 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10651,7 +10694,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="27" name="Straight Arrow Connector 136"/>
+        <xdr:cNvPr id="27" name="Straight Arrow Connector 136">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="3" idx="2"/>
         </xdr:cNvCxnSpPr>
@@ -10700,7 +10749,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="Rectangle 27"/>
+        <xdr:cNvPr id="28" name="Rectangle 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10756,7 +10811,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="Elbow Connector 28"/>
+        <xdr:cNvPr id="29" name="Elbow Connector 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="28" idx="3"/>
           <a:endCxn id="23" idx="1"/>
@@ -10808,7 +10869,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="Elbow Connector 29"/>
+        <xdr:cNvPr id="30" name="Elbow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="28" idx="3"/>
           <a:endCxn id="11" idx="1"/>
@@ -10860,7 +10927,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="Rectangle 30"/>
+        <xdr:cNvPr id="31" name="Rectangle 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10921,7 +10994,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="35" name="Elbow Connector 34"/>
+        <xdr:cNvPr id="35" name="Elbow Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="11" idx="3"/>
           <a:endCxn id="17" idx="2"/>
@@ -10971,7 +11050,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="36" name="Elbow Connector 35"/>
+        <xdr:cNvPr id="36" name="Elbow Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000024000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="23" idx="3"/>
           <a:endCxn id="17" idx="2"/>
@@ -11021,7 +11106,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="37" name="Rectangle 36"/>
+        <xdr:cNvPr id="37" name="Rectangle 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000025000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11082,7 +11173,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="Rectangle 37"/>
+        <xdr:cNvPr id="38" name="Rectangle 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000026000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11143,7 +11240,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="39" name="Straight Arrow Connector 136"/>
+        <xdr:cNvPr id="39" name="Straight Arrow Connector 136">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="37" idx="3"/>
           <a:endCxn id="38" idx="1"/>
@@ -11193,7 +11296,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="24" name="Elbow Connector 23"/>
+        <xdr:cNvPr id="24" name="Elbow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="13" idx="3"/>
           <a:endCxn id="17" idx="1"/>
@@ -11245,7 +11354,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="32" name="Elbow Connector 31"/>
+        <xdr:cNvPr id="32" name="Elbow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="31" idx="3"/>
           <a:endCxn id="16" idx="1"/>
@@ -11295,7 +11410,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="Elbow Connector 23"/>
+        <xdr:cNvPr id="33" name="Elbow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="41" idx="3"/>
           <a:endCxn id="16" idx="1"/>
@@ -11347,7 +11468,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="40" name="Elbow Connector 39"/>
+        <xdr:cNvPr id="40" name="Elbow Connector 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="8" idx="3"/>
           <a:endCxn id="41" idx="1"/>
@@ -11397,7 +11524,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name="Rectangle 40"/>
+        <xdr:cNvPr id="41" name="Rectangle 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11453,7 +11586,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="57" name="Elbow Connector 23"/>
+        <xdr:cNvPr id="57" name="Elbow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000039000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="41" idx="3"/>
           <a:endCxn id="17" idx="1"/>
@@ -11505,7 +11644,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="60" name="Elbow Connector 39"/>
+        <xdr:cNvPr id="60" name="Elbow Connector 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="41" idx="3"/>
           <a:endCxn id="37" idx="1"/>
@@ -11567,11 +11712,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2049"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000001080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -11579,6 +11727,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
@@ -11592,9 +11746,8 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Lucida Grande"/>
-                  <a:ea typeface="Lucida Grande"/>
-                  <a:cs typeface="Lucida Grande"/>
+                  <a:latin typeface="Lucida Grande" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Lucida Grande" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>import data</a:t>
               </a:r>
@@ -11628,11 +11781,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2050"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -11640,6 +11796,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
@@ -11653,9 +11815,8 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Lucida Grande"/>
-                  <a:ea typeface="Lucida Grande"/>
-                  <a:cs typeface="Lucida Grande"/>
+                  <a:latin typeface="Lucida Grande" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Lucida Grande" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>export to 'data/…/ouput' folder</a:t>
               </a:r>
@@ -11689,11 +11850,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2055"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000007080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -11701,6 +11865,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
@@ -11714,9 +11884,8 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Lucida Grande"/>
-                  <a:ea typeface="Lucida Grande"/>
-                  <a:cs typeface="Lucida Grande"/>
+                  <a:latin typeface="Lucida Grande" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Lucida Grande" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>optional: load different Dashboard values</a:t>
               </a:r>
@@ -11732,7 +11901,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover sheet"/>
@@ -12132,7 +12301,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover Sheet"/>
@@ -12212,7 +12381,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover Sheet"/>
@@ -12296,7 +12465,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover Sheet"/>
@@ -12973,15 +13142,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="13.33203125" style="2" customWidth="1"/>
@@ -12990,7 +13159,7 @@
     <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="20">
+    <row r="2" spans="2:8" ht="21">
       <c r="B2" s="22" t="s">
         <v>204</v>
       </c>
@@ -13104,14 +13273,14 @@
       </c>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="2:8" ht="16" thickBot="1">
+    <row r="15" spans="2:8" ht="17" thickBot="1">
       <c r="B15" s="20"/>
       <c r="C15" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="2:8" ht="16" thickBot="1">
+    <row r="16" spans="2:8" ht="17" thickBot="1">
       <c r="B16" s="20"/>
       <c r="C16" s="19" t="s">
         <v>13</v>
@@ -13265,15 +13434,15 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="21.6640625" style="2" customWidth="1"/>
@@ -13284,7 +13453,7 @@
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="20">
+    <row r="2" spans="2:6" ht="21">
       <c r="B2" s="220" t="s">
         <v>308</v>
       </c>
@@ -13299,14 +13468,14 @@
       <c r="E4" s="222"/>
     </row>
     <row r="5" spans="2:6" ht="29" customHeight="1">
-      <c r="B5" s="363" t="s">
+      <c r="B5" s="353" t="s">
         <v>313</v>
       </c>
-      <c r="C5" s="364"/>
-      <c r="D5" s="364"/>
+      <c r="C5" s="354"/>
+      <c r="D5" s="354"/>
       <c r="E5" s="222"/>
     </row>
-    <row r="6" spans="2:6" ht="16" thickBot="1">
+    <row r="6" spans="2:6" ht="17" thickBot="1">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
     </row>
@@ -13365,7 +13534,7 @@
       </c>
       <c r="F11" s="299"/>
     </row>
-    <row r="12" spans="2:6" ht="16" thickBot="1">
+    <row r="12" spans="2:6" ht="17" thickBot="1">
       <c r="B12" s="62"/>
       <c r="C12" s="63"/>
       <c r="D12" s="284"/>
@@ -13387,8 +13556,8 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B2:E27"/>
@@ -13397,7 +13566,7 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="24.83203125" style="2" bestFit="1" customWidth="1"/>
@@ -13405,7 +13574,7 @@
     <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="20">
+    <row r="2" spans="2:5" ht="21">
       <c r="B2" s="22" t="s">
         <v>319</v>
       </c>
@@ -13419,14 +13588,14 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="366" t="s">
+      <c r="B5" s="356" t="s">
         <v>363</v>
       </c>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="368"/>
-    </row>
-    <row r="6" spans="2:5" ht="16" thickBot="1">
+      <c r="C5" s="357"/>
+      <c r="D5" s="357"/>
+      <c r="E5" s="358"/>
+    </row>
+    <row r="6" spans="2:5" ht="17" thickBot="1">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -13670,7 +13839,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="16" thickBot="1">
+    <row r="27" spans="2:5" ht="17" thickBot="1">
       <c r="B27" s="98"/>
       <c r="C27" s="188"/>
       <c r="D27" s="213"/>
@@ -13691,8 +13860,8 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B2:G45"/>
@@ -13701,7 +13870,7 @@
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="62.5" style="2" bestFit="1" customWidth="1"/>
@@ -13712,7 +13881,7 @@
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="20">
+    <row r="2" spans="2:7" ht="21">
       <c r="B2" s="22" t="s">
         <v>431</v>
       </c>
@@ -13727,15 +13896,15 @@
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="369" t="s">
+      <c r="B5" s="359" t="s">
         <v>442</v>
       </c>
-      <c r="C5" s="370"/>
-      <c r="D5" s="370"/>
-      <c r="E5" s="371"/>
+      <c r="C5" s="360"/>
+      <c r="D5" s="360"/>
+      <c r="E5" s="361"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="2:7" ht="16" thickBot="1"/>
+    <row r="6" spans="2:7" ht="17" thickBot="1"/>
     <row r="7" spans="2:7">
       <c r="B7" s="55" t="s">
         <v>227</v>
@@ -13941,7 +14110,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="16" thickBot="1">
+    <row r="24" spans="2:7" ht="17" thickBot="1">
       <c r="B24" s="62"/>
       <c r="C24" s="63"/>
       <c r="D24" s="229"/>
@@ -13958,14 +14127,14 @@
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="369" t="s">
+      <c r="B28" s="359" t="s">
         <v>443</v>
       </c>
-      <c r="C28" s="370"/>
-      <c r="D28" s="370"/>
-      <c r="E28" s="371"/>
-    </row>
-    <row r="29" spans="2:7" ht="16" thickBot="1"/>
+      <c r="C28" s="360"/>
+      <c r="D28" s="360"/>
+      <c r="E28" s="361"/>
+    </row>
+    <row r="29" spans="2:7" ht="17" thickBot="1"/>
     <row r="30" spans="2:7">
       <c r="B30" s="55" t="s">
         <v>227</v>
@@ -14170,7 +14339,7 @@
       <c r="F44" s="15"/>
       <c r="G44" s="59"/>
     </row>
-    <row r="45" spans="2:7" ht="16" thickBot="1">
+    <row r="45" spans="2:7" ht="17" thickBot="1">
       <c r="B45" s="62"/>
       <c r="C45" s="63"/>
       <c r="D45" s="229"/>
@@ -14194,240 +14363,8 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="8" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="B2:F26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" ht="20">
-      <c r="B2" s="22" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="366" t="s">
-        <v>481</v>
-      </c>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="368"/>
-    </row>
-    <row r="6" spans="2:6" ht="16" thickBot="1">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="94" t="s">
-        <v>199</v>
-      </c>
-      <c r="C7" s="205"/>
-      <c r="D7" s="210"/>
-      <c r="E7" s="95"/>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="96"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="97"/>
-    </row>
-    <row r="9" spans="2:6" ht="31" customHeight="1">
-      <c r="B9" s="214" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="215" t="s">
-        <v>482</v>
-      </c>
-      <c r="D9" s="216" t="s">
-        <v>483</v>
-      </c>
-      <c r="E9" s="268" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="197" t="str">
-        <f>"Hydrogen production in "&amp;base_year</f>
-        <v xml:space="preserve">Hydrogen production in </v>
-      </c>
-      <c r="C10" s="203"/>
-      <c r="D10" s="211"/>
-      <c r="E10" s="262"/>
-    </row>
-    <row r="11" spans="2:6" ht="15" customHeight="1">
-      <c r="B11" s="206"/>
-      <c r="C11" s="107" t="s">
-        <v>486</v>
-      </c>
-      <c r="D11" s="349">
-        <f>Dashboard!E61</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="350"/>
-    </row>
-    <row r="12" spans="2:6" ht="15" customHeight="1">
-      <c r="B12" s="206"/>
-      <c r="C12" s="107" t="s">
-        <v>484</v>
-      </c>
-      <c r="D12" s="349">
-        <f>Dashboard!E59</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="350">
-        <f>IF(SUM($D$12:$D$15)=0,1,D12/SUM($D$12:$D$15))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="15" customHeight="1">
-      <c r="B13" s="207"/>
-      <c r="C13" s="107" t="s">
-        <v>485</v>
-      </c>
-      <c r="D13" s="349">
-        <f>Dashboard!E60</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="350">
-        <f>IF(SUM($D$12:$D$15)=0,0,D13/SUM($D$12:$D$15))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="15" customHeight="1">
-      <c r="B14" s="190"/>
-      <c r="C14" s="107" t="s">
-        <v>487</v>
-      </c>
-      <c r="D14" s="349">
-        <v>0</v>
-      </c>
-      <c r="E14" s="350">
-        <f>IF(SUM($D$12:$D$15)=0,0,D14/SUM($D$12:$D$15))</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="338"/>
-    </row>
-    <row r="15" spans="2:6" ht="15" customHeight="1">
-      <c r="B15" s="190"/>
-      <c r="C15" s="107" t="s">
-        <v>488</v>
-      </c>
-      <c r="D15" s="349">
-        <v>0</v>
-      </c>
-      <c r="E15" s="350">
-        <f>IF(SUM($D$12:$D$15)=0,0,D15/SUM($D$12:$D$15))</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="338"/>
-    </row>
-    <row r="16" spans="2:6" ht="15" customHeight="1">
-      <c r="B16" s="194"/>
-      <c r="C16" s="352"/>
-      <c r="D16" s="353"/>
-      <c r="E16" s="354"/>
-    </row>
-    <row r="17" spans="2:5" ht="15" customHeight="1">
-      <c r="B17" s="197" t="str">
-        <f>"Hydrogen production type in "&amp;base_year</f>
-        <v xml:space="preserve">Hydrogen production type in </v>
-      </c>
-      <c r="C17" s="107"/>
-      <c r="D17" s="267"/>
-      <c r="E17" s="351"/>
-    </row>
-    <row r="18" spans="2:5" ht="15" customHeight="1">
-      <c r="B18" s="112"/>
-      <c r="C18" s="204"/>
-      <c r="D18" s="267"/>
-      <c r="E18" s="355"/>
-    </row>
-    <row r="19" spans="2:5" ht="15" customHeight="1">
-      <c r="B19" s="112"/>
-      <c r="C19" s="204"/>
-      <c r="D19" s="356" t="s">
-        <v>492</v>
-      </c>
-      <c r="E19" s="355"/>
-    </row>
-    <row r="20" spans="2:5" ht="15" customHeight="1">
-      <c r="B20" s="190"/>
-      <c r="C20" s="107" t="s">
-        <v>490</v>
-      </c>
-      <c r="D20" s="349">
-        <f>IF(SUM($D$11:$D$15)=0,0, D11)</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="355"/>
-    </row>
-    <row r="21" spans="2:5" ht="15" customHeight="1">
-      <c r="B21" s="190"/>
-      <c r="C21" s="107" t="s">
-        <v>491</v>
-      </c>
-      <c r="D21" s="349">
-        <f>IF(SUM($D$11:$D$15)=0,1, SUM(D12:D15))</f>
-        <v>1</v>
-      </c>
-      <c r="E21" s="355"/>
-    </row>
-    <row r="22" spans="2:5" ht="15" customHeight="1">
-      <c r="B22" s="112"/>
-      <c r="C22" s="204"/>
-      <c r="D22" s="267"/>
-      <c r="E22" s="351"/>
-    </row>
-    <row r="23" spans="2:5" ht="15" customHeight="1" thickBot="1">
-      <c r="B23" s="98"/>
-      <c r="C23" s="188"/>
-      <c r="D23" s="213"/>
-      <c r="E23" s="272"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" customHeight="1"/>
-    <row r="25" spans="2:5" ht="15" customHeight="1"/>
-    <row r="26" spans="2:5" ht="15" customHeight="1"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:E5"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B2:G13"/>
@@ -14436,14 +14373,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="5" width="10.83203125" style="2"/>
     <col min="6" max="6" width="3.5" style="2" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="20">
+    <row r="2" spans="2:7" ht="21">
       <c r="B2" s="22" t="s">
         <v>327</v>
       </c>
@@ -14458,15 +14395,15 @@
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="2:7" ht="30" customHeight="1">
-      <c r="B5" s="363" t="s">
+      <c r="B5" s="353" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="372"/>
-      <c r="D5" s="372"/>
-      <c r="E5" s="373"/>
+      <c r="C5" s="362"/>
+      <c r="D5" s="362"/>
+      <c r="E5" s="363"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="2:7" ht="16" thickBot="1"/>
+    <row r="6" spans="2:7" ht="17" thickBot="1"/>
     <row r="7" spans="2:7">
       <c r="B7" s="55" t="s">
         <v>227</v>
@@ -14541,7 +14478,7 @@
       <c r="F12" s="219"/>
       <c r="G12" s="59"/>
     </row>
-    <row r="13" spans="2:7" ht="16" thickBot="1">
+    <row r="13" spans="2:7" ht="17" thickBot="1">
       <c r="B13" s="62"/>
       <c r="C13" s="63"/>
       <c r="D13" s="229"/>
@@ -14562,9 +14499,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="B2:O17"/>
@@ -14573,7 +14510,7 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="100"/>
     <col min="2" max="3" width="30.5" style="100" customWidth="1"/>
@@ -14582,7 +14519,7 @@
     <col min="16" max="16384" width="10.83203125" style="100"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="20">
+    <row r="2" spans="2:15" ht="21">
       <c r="B2" s="220" t="s">
         <v>349</v>
       </c>
@@ -14616,17 +14553,17 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:15" ht="30" customHeight="1">
-      <c r="B5" s="374" t="s">
+      <c r="B5" s="364" t="s">
         <v>367</v>
       </c>
-      <c r="C5" s="375"/>
-      <c r="D5" s="375"/>
-      <c r="E5" s="375"/>
-      <c r="F5" s="375"/>
-      <c r="G5" s="375"/>
-      <c r="H5" s="376"/>
-    </row>
-    <row r="6" spans="2:15" ht="16" thickBot="1"/>
+      <c r="C5" s="365"/>
+      <c r="D5" s="365"/>
+      <c r="E5" s="365"/>
+      <c r="F5" s="365"/>
+      <c r="G5" s="365"/>
+      <c r="H5" s="366"/>
+    </row>
+    <row r="6" spans="2:15" ht="17" thickBot="1"/>
     <row r="7" spans="2:15">
       <c r="B7" s="55" t="s">
         <v>350</v>
@@ -14661,7 +14598,7 @@
       <c r="N8" s="251"/>
       <c r="O8" s="252"/>
     </row>
-    <row r="9" spans="2:15" ht="30">
+    <row r="9" spans="2:15" ht="32">
       <c r="B9" s="253" t="s">
         <v>284</v>
       </c>
@@ -14874,7 +14811,7 @@
       <c r="N16" s="265"/>
       <c r="O16" s="266"/>
     </row>
-    <row r="17" spans="2:15" ht="16" thickBot="1">
+    <row r="17" spans="2:15" ht="17" thickBot="1">
       <c r="B17" s="275"/>
       <c r="C17" s="276"/>
       <c r="D17" s="277"/>
@@ -14904,9 +14841,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:C60"/>
@@ -14915,7 +14852,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="51.5" customWidth="1"/>
   </cols>
@@ -15273,9 +15210,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:G43"/>
@@ -15284,7 +15221,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
@@ -15934,9 +15871,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:G43"/>
@@ -15945,7 +15882,7 @@
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
@@ -16595,16 +16532,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -17254,431 +17191,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="2"/>
-  </sheetPr>
-  <dimension ref="B2:D45"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.5" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" ht="20">
-      <c r="B2" s="22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="6"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="125">
-        <v>41487</v>
-      </c>
-      <c r="C6" s="235" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="240">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="236">
-        <v>41488</v>
-      </c>
-      <c r="C7" s="235" t="s">
-        <v>298</v>
-      </c>
-      <c r="D7" s="240">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="236">
-        <v>41491</v>
-      </c>
-      <c r="C8" s="235" t="s">
-        <v>268</v>
-      </c>
-      <c r="D8" s="240">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="236">
-        <v>41492</v>
-      </c>
-      <c r="C9" s="235" t="s">
-        <v>278</v>
-      </c>
-      <c r="D9" s="240">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="236">
-        <v>41494</v>
-      </c>
-      <c r="C10" s="235" t="s">
-        <v>279</v>
-      </c>
-      <c r="D10" s="240">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="236">
-        <v>41498</v>
-      </c>
-      <c r="C11" s="235" t="s">
-        <v>299</v>
-      </c>
-      <c r="D11" s="240">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="236">
-        <v>41499</v>
-      </c>
-      <c r="C12" s="235" t="s">
-        <v>295</v>
-      </c>
-      <c r="D12" s="240">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="236">
-        <v>41500</v>
-      </c>
-      <c r="C13" s="235" t="s">
-        <v>297</v>
-      </c>
-      <c r="D13" s="240">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="45">
-      <c r="B14" s="236">
-        <v>41500</v>
-      </c>
-      <c r="C14" s="237" t="s">
-        <v>318</v>
-      </c>
-      <c r="D14" s="240">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="236">
-        <v>41500</v>
-      </c>
-      <c r="C15" s="235" t="s">
-        <v>325</v>
-      </c>
-      <c r="D15" s="240">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="241">
-        <v>41500</v>
-      </c>
-      <c r="C16" s="242" t="s">
-        <v>326</v>
-      </c>
-      <c r="D16" s="240">
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="236">
-        <v>41501</v>
-      </c>
-      <c r="C17" s="235" t="s">
-        <v>340</v>
-      </c>
-      <c r="D17" s="240">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="30">
-      <c r="B18" s="236">
-        <v>41502</v>
-      </c>
-      <c r="C18" s="237" t="s">
-        <v>341</v>
-      </c>
-      <c r="D18" s="240">
-        <v>1.03</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="236">
-        <v>41505</v>
-      </c>
-      <c r="C19" s="235" t="s">
-        <v>347</v>
-      </c>
-      <c r="D19" s="240">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="236">
-        <v>41505</v>
-      </c>
-      <c r="C20" s="235" t="s">
-        <v>364</v>
-      </c>
-      <c r="D20" s="240">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="30">
-      <c r="B21" s="236">
-        <v>41506</v>
-      </c>
-      <c r="C21" s="237" t="s">
-        <v>375</v>
-      </c>
-      <c r="D21" s="240">
-        <v>1.06</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="288">
-        <v>41507</v>
-      </c>
-      <c r="C22" s="242" t="s">
-        <v>376</v>
-      </c>
-      <c r="D22" s="296">
-        <v>1.07</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="288">
-        <v>41509</v>
-      </c>
-      <c r="C23" s="242" t="s">
-        <v>377</v>
-      </c>
-      <c r="D23" s="296">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="30">
-      <c r="B24" s="288">
-        <v>41514</v>
-      </c>
-      <c r="C24" s="242" t="s">
-        <v>378</v>
-      </c>
-      <c r="D24" s="296">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="30">
-      <c r="B25" s="288">
-        <v>41519</v>
-      </c>
-      <c r="C25" s="242" t="s">
-        <v>380</v>
-      </c>
-      <c r="D25" s="296">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="288">
-        <v>41520</v>
-      </c>
-      <c r="C26" s="242" t="s">
-        <v>382</v>
-      </c>
-      <c r="D26" s="296">
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="30">
-      <c r="B27" s="288">
-        <v>41521</v>
-      </c>
-      <c r="C27" s="242" t="s">
-        <v>384</v>
-      </c>
-      <c r="D27" s="296">
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="288">
-        <v>41521</v>
-      </c>
-      <c r="C28" s="242" t="s">
-        <v>385</v>
-      </c>
-      <c r="D28" s="296">
-        <v>1.1299999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="30">
-      <c r="B29" s="288">
-        <v>41534</v>
-      </c>
-      <c r="C29" s="242" t="s">
-        <v>395</v>
-      </c>
-      <c r="D29" s="296" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" ht="45">
-      <c r="B30" s="288">
-        <v>41555</v>
-      </c>
-      <c r="C30" s="242" t="s">
-        <v>398</v>
-      </c>
-      <c r="D30" s="296" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="313" t="s">
-        <v>399</v>
-      </c>
-      <c r="C31" s="314" t="s">
-        <v>400</v>
-      </c>
-      <c r="D31" s="315">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" ht="30">
-      <c r="B32" s="288">
-        <v>41681</v>
-      </c>
-      <c r="C32" s="242" t="s">
-        <v>402</v>
-      </c>
-      <c r="D32" s="296">
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="288">
-        <v>41688</v>
-      </c>
-      <c r="C33" s="242" t="s">
-        <v>409</v>
-      </c>
-      <c r="D33" s="296">
-        <v>1.1599999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="288">
-        <v>42300</v>
-      </c>
-      <c r="C34" s="242" t="s">
-        <v>428</v>
-      </c>
-      <c r="D34" s="296">
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4">
-      <c r="B35" s="288" t="s">
-        <v>473</v>
-      </c>
-      <c r="C35" s="242" t="s">
-        <v>474</v>
-      </c>
-      <c r="D35" s="296">
-        <v>1.18</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36" s="236"/>
-      <c r="C36" s="235"/>
-      <c r="D36" s="240"/>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37" s="238"/>
-      <c r="C37" s="239"/>
-      <c r="D37" s="297"/>
-    </row>
-    <row r="38" spans="2:4">
-      <c r="D38" s="221"/>
-    </row>
-    <row r="39" spans="2:4">
-      <c r="D39" s="221"/>
-    </row>
-    <row r="40" spans="2:4">
-      <c r="D40" s="221"/>
-    </row>
-    <row r="41" spans="2:4">
-      <c r="D41" s="221"/>
-    </row>
-    <row r="42" spans="2:4">
-      <c r="D42" s="221"/>
-    </row>
-    <row r="43" spans="2:4">
-      <c r="D43" s="221"/>
-    </row>
-    <row r="44" spans="2:4">
-      <c r="D44" s="221"/>
-    </row>
-    <row r="45" spans="2:4">
-      <c r="D45" s="221"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
@@ -18328,9 +17850,424 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
+  <dimension ref="B2:D45"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.5" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="21">
+      <c r="B2" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="6"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="125">
+        <v>41487</v>
+      </c>
+      <c r="C6" s="235" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="240">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="236">
+        <v>41488</v>
+      </c>
+      <c r="C7" s="235" t="s">
+        <v>298</v>
+      </c>
+      <c r="D7" s="240">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="236">
+        <v>41491</v>
+      </c>
+      <c r="C8" s="235" t="s">
+        <v>268</v>
+      </c>
+      <c r="D8" s="240">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="236">
+        <v>41492</v>
+      </c>
+      <c r="C9" s="235" t="s">
+        <v>278</v>
+      </c>
+      <c r="D9" s="240">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="236">
+        <v>41494</v>
+      </c>
+      <c r="C10" s="235" t="s">
+        <v>279</v>
+      </c>
+      <c r="D10" s="240">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="236">
+        <v>41498</v>
+      </c>
+      <c r="C11" s="235" t="s">
+        <v>299</v>
+      </c>
+      <c r="D11" s="240">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="236">
+        <v>41499</v>
+      </c>
+      <c r="C12" s="235" t="s">
+        <v>295</v>
+      </c>
+      <c r="D12" s="240">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="236">
+        <v>41500</v>
+      </c>
+      <c r="C13" s="235" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" s="240">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="48">
+      <c r="B14" s="236">
+        <v>41500</v>
+      </c>
+      <c r="C14" s="237" t="s">
+        <v>318</v>
+      </c>
+      <c r="D14" s="240">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="236">
+        <v>41500</v>
+      </c>
+      <c r="C15" s="235" t="s">
+        <v>325</v>
+      </c>
+      <c r="D15" s="240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="241">
+        <v>41500</v>
+      </c>
+      <c r="C16" s="242" t="s">
+        <v>326</v>
+      </c>
+      <c r="D16" s="240">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="236">
+        <v>41501</v>
+      </c>
+      <c r="C17" s="235" t="s">
+        <v>340</v>
+      </c>
+      <c r="D17" s="240">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="32">
+      <c r="B18" s="236">
+        <v>41502</v>
+      </c>
+      <c r="C18" s="237" t="s">
+        <v>341</v>
+      </c>
+      <c r="D18" s="240">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="236">
+        <v>41505</v>
+      </c>
+      <c r="C19" s="235" t="s">
+        <v>347</v>
+      </c>
+      <c r="D19" s="240">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="236">
+        <v>41505</v>
+      </c>
+      <c r="C20" s="235" t="s">
+        <v>364</v>
+      </c>
+      <c r="D20" s="240">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="32">
+      <c r="B21" s="236">
+        <v>41506</v>
+      </c>
+      <c r="C21" s="237" t="s">
+        <v>375</v>
+      </c>
+      <c r="D21" s="240">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="288">
+        <v>41507</v>
+      </c>
+      <c r="C22" s="242" t="s">
+        <v>376</v>
+      </c>
+      <c r="D22" s="296">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="288">
+        <v>41509</v>
+      </c>
+      <c r="C23" s="242" t="s">
+        <v>377</v>
+      </c>
+      <c r="D23" s="296">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="32">
+      <c r="B24" s="288">
+        <v>41514</v>
+      </c>
+      <c r="C24" s="242" t="s">
+        <v>378</v>
+      </c>
+      <c r="D24" s="296">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="32">
+      <c r="B25" s="288">
+        <v>41519</v>
+      </c>
+      <c r="C25" s="242" t="s">
+        <v>380</v>
+      </c>
+      <c r="D25" s="296">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="288">
+        <v>41520</v>
+      </c>
+      <c r="C26" s="242" t="s">
+        <v>382</v>
+      </c>
+      <c r="D26" s="296">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="32">
+      <c r="B27" s="288">
+        <v>41521</v>
+      </c>
+      <c r="C27" s="242" t="s">
+        <v>384</v>
+      </c>
+      <c r="D27" s="296">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="288">
+        <v>41521</v>
+      </c>
+      <c r="C28" s="242" t="s">
+        <v>385</v>
+      </c>
+      <c r="D28" s="296">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="32">
+      <c r="B29" s="288">
+        <v>41534</v>
+      </c>
+      <c r="C29" s="242" t="s">
+        <v>395</v>
+      </c>
+      <c r="D29" s="296" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="48">
+      <c r="B30" s="288">
+        <v>41555</v>
+      </c>
+      <c r="C30" s="242" t="s">
+        <v>398</v>
+      </c>
+      <c r="D30" s="296" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="313" t="s">
+        <v>399</v>
+      </c>
+      <c r="C31" s="314" t="s">
+        <v>400</v>
+      </c>
+      <c r="D31" s="315">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="32">
+      <c r="B32" s="288">
+        <v>41681</v>
+      </c>
+      <c r="C32" s="242" t="s">
+        <v>402</v>
+      </c>
+      <c r="D32" s="296">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="288">
+        <v>41688</v>
+      </c>
+      <c r="C33" s="242" t="s">
+        <v>409</v>
+      </c>
+      <c r="D33" s="296">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="288">
+        <v>42300</v>
+      </c>
+      <c r="C34" s="242" t="s">
+        <v>428</v>
+      </c>
+      <c r="D34" s="296">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="288" t="s">
+        <v>461</v>
+      </c>
+      <c r="C35" s="242" t="s">
+        <v>462</v>
+      </c>
+      <c r="D35" s="296">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="236"/>
+      <c r="C36" s="235"/>
+      <c r="D36" s="240"/>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="238"/>
+      <c r="C37" s="239"/>
+      <c r="D37" s="297"/>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="D38" s="221"/>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="D39" s="221"/>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="D40" s="221"/>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="D41" s="221"/>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="D42" s="221"/>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="D43" s="221"/>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="D44" s="221"/>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="D45" s="221"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:G43"/>
@@ -18339,7 +18276,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
@@ -18989,9 +18926,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:G43"/>
@@ -19000,7 +18937,7 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="47.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
@@ -19650,9 +19587,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
@@ -19661,7 +19598,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -19691,6 +19628,60 @@
       </c>
       <c r="B4">
         <f>Dashboard!E48</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B3">
+        <f>'Waste analysis'!E12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4">
+        <f>'Waste analysis'!E11</f>
         <v>0</v>
       </c>
     </row>
@@ -19705,62 +19696,8 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>331</v>
-      </c>
-      <c r="B3">
-        <f>'Waste analysis'!E12</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>332</v>
-      </c>
-      <c r="B4">
-        <f>'Waste analysis'!E11</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
@@ -19769,7 +19706,7 @@
       <selection activeCell="C1" sqref="C1:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="51.5" customWidth="1"/>
   </cols>
@@ -19816,9 +19753,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
@@ -19827,7 +19764,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="51.5" customWidth="1"/>
   </cols>
@@ -19860,143 +19797,6 @@
       </c>
       <c r="B4" s="88">
         <f>Network_gas_analysis!E35</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="51.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="50" t="s">
-        <v>465</v>
-      </c>
-      <c r="B3" s="88">
-        <f>Hydrogen_production_analysis!E12</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="50" t="s">
-        <v>464</v>
-      </c>
-      <c r="B4" s="88">
-        <f>Hydrogen_production_analysis!E13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>467</v>
-      </c>
-      <c r="B5" s="88">
-        <f>Hydrogen_production_analysis!E14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>466</v>
-      </c>
-      <c r="B6" s="88">
-        <f>Hydrogen_production_analysis!E15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="50"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="51.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="50" t="s">
-        <v>461</v>
-      </c>
-      <c r="B3" s="88">
-        <f>Hydrogen_production_analysis!D20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="50" t="s">
-        <v>462</v>
-      </c>
-      <c r="B4" s="88">
-        <f>Hydrogen_production_analysis!D21</f>
         <v>1</v>
       </c>
     </row>
@@ -20012,8 +19812,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:C32"/>
@@ -20022,7 +19822,7 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="35.83203125" style="2" customWidth="1"/>
@@ -20030,7 +19830,7 @@
     <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="20">
+    <row r="2" spans="2:3" ht="21">
       <c r="B2" s="22" t="s">
         <v>22</v>
       </c>
@@ -20149,10 +19949,10 @@
     </row>
     <row r="18" spans="2:3" s="176" customFormat="1" ht="30" customHeight="1">
       <c r="B18" s="180" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="C18" s="324" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
     </row>
     <row r="19" spans="2:3" s="176" customFormat="1" ht="30" customHeight="1">
@@ -20253,18 +20053,18 @@
     </row>
     <row r="31" spans="2:3" ht="33" customHeight="1">
       <c r="B31" s="181" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="C31" s="325" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="31" customHeight="1">
       <c r="B32" s="181" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="C32" s="325" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -20279,8 +20079,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:C33"/>
@@ -20289,7 +20089,7 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="140.83203125" style="2" customWidth="1"/>
@@ -20297,7 +20097,7 @@
     <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="20">
+    <row r="2" spans="2:3" ht="21">
       <c r="B2" s="22" t="s">
         <v>20</v>
       </c>
@@ -20312,7 +20112,7 @@
       <c r="B5" s="327"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="2:3" ht="150">
+    <row r="6" spans="2:3" ht="160">
       <c r="B6" s="328" t="s">
         <v>419</v>
       </c>
@@ -20399,7 +20199,7 @@
     <row r="22" spans="2:3">
       <c r="B22" s="321"/>
     </row>
-    <row r="23" spans="2:3" ht="90">
+    <row r="23" spans="2:3" ht="96">
       <c r="B23" s="322" t="s">
         <v>408</v>
       </c>
@@ -20421,14 +20221,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:BZ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Z54" sqref="Z54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="8.1640625" style="2" customWidth="1"/>
     <col min="2" max="16384" width="2.83203125" style="2"/>
@@ -20851,8 +20651,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="A2:F93"/>
@@ -20861,7 +20661,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="25.83203125" style="2" customWidth="1"/>
@@ -20869,7 +20669,7 @@
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="20">
+    <row r="2" spans="1:6" ht="21">
       <c r="B2" s="22" t="s">
         <v>24</v>
       </c>
@@ -20891,13 +20691,13 @@
     </row>
     <row r="5" spans="1:6" ht="79" customHeight="1">
       <c r="A5" s="100"/>
-      <c r="B5" s="357" t="s">
+      <c r="B5" s="347" t="s">
         <v>213</v>
       </c>
-      <c r="C5" s="358"/>
+      <c r="C5" s="348"/>
       <c r="D5" s="100"/>
     </row>
-    <row r="6" spans="1:6" ht="16" thickBot="1">
+    <row r="6" spans="1:6" ht="17" thickBot="1">
       <c r="A6" s="100"/>
       <c r="B6" s="100"/>
       <c r="C6" s="100"/>
@@ -20964,7 +20764,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30">
+    <row r="14" spans="1:6" ht="32">
       <c r="B14" s="70"/>
       <c r="C14" s="114" t="s">
         <v>305</v>
@@ -20972,7 +20772,7 @@
       <c r="D14" s="183"/>
       <c r="F14" s="89"/>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="32">
       <c r="B15" s="70"/>
       <c r="C15" s="114" t="s">
         <v>397</v>
@@ -20980,12 +20780,12 @@
       <c r="D15" s="183"/>
       <c r="F15" s="89"/>
     </row>
-    <row r="16" spans="1:6" ht="16" thickBot="1">
+    <row r="16" spans="1:6" ht="17" thickBot="1">
       <c r="B16" s="93"/>
       <c r="C16" s="185"/>
       <c r="D16" s="186"/>
     </row>
-    <row r="17" spans="2:4" ht="16" thickBot="1">
+    <row r="17" spans="2:4" ht="17" thickBot="1">
       <c r="B17" s="100"/>
       <c r="C17" s="100"/>
       <c r="D17" s="100"/>
@@ -21092,12 +20892,12 @@
       </c>
       <c r="D31" s="193"/>
     </row>
-    <row r="32" spans="2:4" ht="16" thickBot="1">
+    <row r="32" spans="2:4" ht="17" thickBot="1">
       <c r="B32" s="98"/>
       <c r="C32" s="188"/>
       <c r="D32" s="189"/>
     </row>
-    <row r="33" spans="2:4" ht="16" thickBot="1">
+    <row r="33" spans="2:4" ht="17" thickBot="1">
       <c r="B33" s="100"/>
       <c r="C33" s="100"/>
       <c r="D33" s="100"/>
@@ -21503,7 +21303,7 @@
       </c>
       <c r="D90" s="90"/>
     </row>
-    <row r="91" spans="2:4" ht="16" thickBot="1">
+    <row r="91" spans="2:4" ht="17" thickBot="1">
       <c r="B91" s="98"/>
       <c r="C91" s="189"/>
       <c r="D91" s="90"/>
@@ -21534,17 +21334,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:Q63"/>
+  <dimension ref="A2:Q57"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" style="2" bestFit="1" customWidth="1"/>
@@ -21565,7 +21365,7 @@
     <col min="17" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="20">
+    <row r="2" spans="2:17" ht="21">
       <c r="B2" s="22" t="s">
         <v>29</v>
       </c>
@@ -21601,14 +21401,14 @@
       <c r="M4" s="8"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1">
-      <c r="B5" s="359" t="s">
+      <c r="B5" s="349" t="s">
         <v>418</v>
       </c>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
-      <c r="G5" s="361"/>
+      <c r="C5" s="350"/>
+      <c r="D5" s="350"/>
+      <c r="E5" s="350"/>
+      <c r="F5" s="350"/>
+      <c r="G5" s="351"/>
       <c r="H5" s="159"/>
       <c r="I5" s="159"/>
       <c r="J5" s="100"/>
@@ -21617,12 +21417,12 @@
       <c r="M5" s="8"/>
     </row>
     <row r="6" spans="2:17">
-      <c r="B6" s="359"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="361"/>
+      <c r="B6" s="349"/>
+      <c r="C6" s="350"/>
+      <c r="D6" s="350"/>
+      <c r="E6" s="350"/>
+      <c r="F6" s="350"/>
+      <c r="G6" s="351"/>
       <c r="H6" s="159"/>
       <c r="I6" s="159"/>
       <c r="J6" s="100"/>
@@ -21631,12 +21431,12 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="2:17">
-      <c r="B7" s="357"/>
-      <c r="C7" s="362"/>
-      <c r="D7" s="362"/>
-      <c r="E7" s="362"/>
-      <c r="F7" s="362"/>
-      <c r="G7" s="358"/>
+      <c r="B7" s="347"/>
+      <c r="C7" s="352"/>
+      <c r="D7" s="352"/>
+      <c r="E7" s="352"/>
+      <c r="F7" s="352"/>
+      <c r="G7" s="348"/>
       <c r="H7" s="159"/>
       <c r="I7" s="159"/>
       <c r="J7" s="100"/>
@@ -22063,7 +21863,7 @@
       <c r="P23" s="132"/>
       <c r="Q23" s="9"/>
     </row>
-    <row r="24" spans="2:17" ht="16" thickBot="1">
+    <row r="24" spans="2:17" ht="17" thickBot="1">
       <c r="B24" s="58"/>
       <c r="C24" s="151" t="s">
         <v>235</v>
@@ -22090,7 +21890,7 @@
       <c r="P24" s="132"/>
       <c r="Q24" s="9"/>
     </row>
-    <row r="25" spans="2:17" ht="16" thickBot="1">
+    <row r="25" spans="2:17" ht="17" thickBot="1">
       <c r="B25" s="58"/>
       <c r="C25" s="151" t="s">
         <v>239</v>
@@ -22240,7 +22040,7 @@
       <c r="P30" s="132"/>
       <c r="Q30" s="9"/>
     </row>
-    <row r="31" spans="2:17" ht="16" thickBot="1">
+    <row r="31" spans="2:17" ht="17" thickBot="1">
       <c r="B31" s="58"/>
       <c r="C31" s="159" t="s">
         <v>236</v>
@@ -22264,7 +22064,7 @@
       <c r="P31" s="132"/>
       <c r="Q31" s="9"/>
     </row>
-    <row r="32" spans="2:17" ht="16" thickBot="1">
+    <row r="32" spans="2:17" ht="17" thickBot="1">
       <c r="B32" s="61"/>
       <c r="C32" s="159" t="s">
         <v>238</v>
@@ -22375,7 +22175,7 @@
       <c r="P36" s="132"/>
       <c r="Q36" s="9"/>
     </row>
-    <row r="37" spans="2:17" ht="16" thickBot="1">
+    <row r="37" spans="2:17" ht="17" thickBot="1">
       <c r="B37" s="61"/>
       <c r="C37" s="151" t="s">
         <v>239</v>
@@ -22399,7 +22199,7 @@
       <c r="P37" s="132"/>
       <c r="Q37" s="9"/>
     </row>
-    <row r="38" spans="2:17" ht="16" thickBot="1">
+    <row r="38" spans="2:17" ht="17" thickBot="1">
       <c r="B38" s="61"/>
       <c r="C38" s="151" t="s">
         <v>202</v>
@@ -22423,7 +22223,7 @@
       <c r="P38" s="132"/>
       <c r="Q38" s="9"/>
     </row>
-    <row r="39" spans="2:17" ht="16" thickBot="1">
+    <row r="39" spans="2:17" ht="17" thickBot="1">
       <c r="B39" s="61"/>
       <c r="C39" s="151" t="s">
         <v>219</v>
@@ -22588,7 +22388,7 @@
       <c r="P45" s="132"/>
       <c r="Q45" s="9"/>
     </row>
-    <row r="46" spans="2:17" ht="16" thickBot="1">
+    <row r="46" spans="2:17" ht="17" thickBot="1">
       <c r="B46" s="73" t="s">
         <v>287</v>
       </c>
@@ -22608,7 +22408,7 @@
       <c r="P46" s="132"/>
       <c r="Q46" s="9"/>
     </row>
-    <row r="47" spans="2:17" ht="16" thickBot="1">
+    <row r="47" spans="2:17" ht="17" thickBot="1">
       <c r="B47" s="61"/>
       <c r="C47" s="9" t="s">
         <v>288</v>
@@ -22641,7 +22441,7 @@
       </c>
       <c r="Q47" s="9"/>
     </row>
-    <row r="48" spans="2:17" ht="16" thickBot="1">
+    <row r="48" spans="2:17" ht="17" thickBot="1">
       <c r="B48" s="61"/>
       <c r="C48" s="9" t="s">
         <v>289</v>
@@ -22680,7 +22480,7 @@
       <c r="O49" s="133"/>
       <c r="P49" s="132"/>
     </row>
-    <row r="50" spans="1:16" ht="16" thickBot="1">
+    <row r="50" spans="1:16" ht="17" thickBot="1">
       <c r="B50" s="73" t="s">
         <v>429</v>
       </c>
@@ -22699,7 +22499,7 @@
       <c r="O50" s="133"/>
       <c r="P50" s="132"/>
     </row>
-    <row r="51" spans="1:16" ht="16" thickBot="1">
+    <row r="51" spans="1:16" ht="17" thickBot="1">
       <c r="B51" s="61"/>
       <c r="C51" s="9" t="s">
         <v>433</v>
@@ -22754,7 +22554,7 @@
       <c r="O52" s="133"/>
       <c r="P52" s="132"/>
     </row>
-    <row r="53" spans="1:16" ht="16" thickBot="1">
+    <row r="53" spans="1:16" ht="17" thickBot="1">
       <c r="B53" s="58"/>
       <c r="C53" s="9"/>
       <c r="D53" s="139"/>
@@ -22771,7 +22571,7 @@
       <c r="O53" s="133"/>
       <c r="P53" s="132"/>
     </row>
-    <row r="54" spans="1:16" ht="16" thickBot="1">
+    <row r="54" spans="1:16" ht="17" thickBot="1">
       <c r="B54" s="61"/>
       <c r="C54" s="9" t="s">
         <v>434</v>
@@ -22843,197 +22643,66 @@
       <c r="O56" s="133"/>
       <c r="P56" s="132"/>
     </row>
-    <row r="57" spans="1:16">
-      <c r="B57" s="73" t="s">
-        <v>468</v>
-      </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="139"/>
-      <c r="E57" s="163"/>
-      <c r="F57" s="163"/>
-      <c r="G57" s="163"/>
-      <c r="H57" s="163"/>
-      <c r="I57" s="107"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="150"/>
-      <c r="M57" s="59"/>
-      <c r="N57" s="9"/>
-      <c r="O57" s="133"/>
-      <c r="P57" s="132"/>
-    </row>
-    <row r="58" spans="1:16" ht="16" thickBot="1">
-      <c r="B58" s="61"/>
-      <c r="C58" s="9" t="s">
-        <v>469</v>
-      </c>
-      <c r="D58" s="139" t="s">
-        <v>240</v>
-      </c>
-      <c r="E58" s="161">
-        <v>0</v>
-      </c>
-      <c r="F58" s="163"/>
-      <c r="G58" s="163"/>
-      <c r="H58" s="163"/>
-      <c r="I58" s="100" t="s">
-        <v>496</v>
-      </c>
-      <c r="J58" s="9"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="150"/>
-      <c r="M58" s="59"/>
-      <c r="N58" s="9"/>
-      <c r="O58" s="133"/>
-      <c r="P58" s="335"/>
-    </row>
-    <row r="59" spans="1:16" ht="16" thickBot="1">
-      <c r="B59" s="61"/>
-      <c r="C59" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="D59" s="139" t="s">
-        <v>430</v>
-      </c>
-      <c r="E59" s="165"/>
-      <c r="F59" s="163"/>
-      <c r="G59" s="163"/>
-      <c r="H59" s="163"/>
-      <c r="I59" s="162"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="L59" s="310">
-        <f>IF(SUM(E59:E61)=1,TRUE,SUM(E59:E61))</f>
-        <v>0</v>
-      </c>
-      <c r="M59" s="59" t="str">
-        <f>IF(L59=TRUE," ","If this check is red please, make sure the percentage add up to 100%.")</f>
-        <v>If this check is red please, make sure the percentage add up to 100%.</v>
-      </c>
-      <c r="N59" s="9"/>
-      <c r="O59" s="133" t="s">
-        <v>470</v>
-      </c>
-      <c r="P59" s="335">
-        <f>L59</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" ht="16" thickBot="1">
-      <c r="B60" s="61"/>
-      <c r="C60" s="9" t="s">
-        <v>493</v>
-      </c>
-      <c r="D60" s="136" t="s">
-        <v>430</v>
-      </c>
-      <c r="E60" s="165"/>
-      <c r="I60" s="162"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="150"/>
-      <c r="M60" s="59"/>
-      <c r="N60" s="9"/>
-      <c r="O60" s="133" t="s">
-        <v>471</v>
-      </c>
-      <c r="P60" s="132"/>
-    </row>
-    <row r="61" spans="1:16" ht="16" thickBot="1">
-      <c r="A61" s="338"/>
-      <c r="B61" s="339"/>
-      <c r="C61" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="D61" s="136" t="s">
-        <v>430</v>
-      </c>
-      <c r="E61" s="165"/>
-      <c r="I61" s="162"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="150"/>
-      <c r="M61" s="59"/>
-      <c r="O61" s="133" t="s">
-        <v>472</v>
-      </c>
-      <c r="P61" s="132"/>
-    </row>
-    <row r="62" spans="1:16">
-      <c r="A62" s="338"/>
-      <c r="B62" s="339"/>
-      <c r="K62" s="15"/>
-      <c r="L62" s="340"/>
-      <c r="M62" s="59"/>
-      <c r="N62" s="9"/>
-      <c r="O62" s="133"/>
-      <c r="P62" s="335"/>
-    </row>
-    <row r="63" spans="1:16" ht="16" thickBot="1">
-      <c r="A63" s="338"/>
-      <c r="B63" s="341"/>
-      <c r="C63" s="342"/>
-      <c r="D63" s="343"/>
-      <c r="E63" s="188"/>
-      <c r="F63" s="188"/>
-      <c r="G63" s="188"/>
-      <c r="H63" s="188"/>
-      <c r="I63" s="188"/>
-      <c r="J63" s="342"/>
-      <c r="K63" s="344"/>
-      <c r="L63" s="345"/>
-      <c r="M63" s="346"/>
-      <c r="N63" s="342"/>
-      <c r="O63" s="347"/>
-      <c r="P63" s="348"/>
+    <row r="57" spans="1:16" ht="17" thickBot="1">
+      <c r="A57" s="338"/>
+      <c r="B57" s="339"/>
+      <c r="C57" s="340"/>
+      <c r="D57" s="341"/>
+      <c r="E57" s="188"/>
+      <c r="F57" s="188"/>
+      <c r="G57" s="188"/>
+      <c r="H57" s="188"/>
+      <c r="I57" s="188"/>
+      <c r="J57" s="340"/>
+      <c r="K57" s="342"/>
+      <c r="L57" s="343"/>
+      <c r="M57" s="344"/>
+      <c r="N57" s="340"/>
+      <c r="O57" s="345"/>
+      <c r="P57" s="346"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:G7"/>
   </mergeCells>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="7" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:L20">
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L59">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number Range" error="You can only enter a positive number here. " sqref="E25 E32">
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number Range" error="You can only enter a positive number here. " sqref="E25 E32" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Range" error="You can only enter a positive number here. " sqref="E38:E39">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Range" error="You can only enter a positive number here. " sqref="E38:E39" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Range" error="You can only enter a value between 0% and 100%." sqref="E47:E48">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value Range" error="You can only enter a value between 0% and 100%." sqref="E47:E48" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -23066,7 +22735,6 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -23089,7 +22757,6 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -23112,11 +22779,9 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -23127,8 +22792,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B2:BO101"/>
@@ -23140,7 +22805,7 @@
       <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="42.83203125" style="2" customWidth="1"/>
@@ -23148,7 +22813,7 @@
     <col min="68" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:67" ht="20">
+    <row r="2" spans="2:67" ht="21">
       <c r="B2" s="22" t="s">
         <v>296</v>
       </c>
@@ -23199,7 +22864,7 @@
       <c r="AC4" s="141"/>
       <c r="AD4" s="141"/>
     </row>
-    <row r="5" spans="2:67" ht="30">
+    <row r="5" spans="2:67" ht="32">
       <c r="B5" s="174" t="s">
         <v>290</v>
       </c>
@@ -23833,7 +23498,7 @@
       <c r="BN13" s="48"/>
       <c r="BO13" s="33"/>
     </row>
-    <row r="14" spans="2:67" ht="16" thickBot="1">
+    <row r="14" spans="2:67" ht="17" thickBot="1">
       <c r="B14" s="32" t="s">
         <v>53</v>
       </c>
@@ -23903,7 +23568,7 @@
       <c r="BN14" s="48"/>
       <c r="BO14" s="33"/>
     </row>
-    <row r="15" spans="2:67" ht="16" thickBot="1">
+    <row r="15" spans="2:67" ht="17" thickBot="1">
       <c r="B15" s="40" t="s">
         <v>54</v>
       </c>
@@ -24043,7 +23708,7 @@
       <c r="BN16" s="48"/>
       <c r="BO16" s="33"/>
     </row>
-    <row r="17" spans="2:67" ht="16" thickBot="1">
+    <row r="17" spans="2:67" ht="17" thickBot="1">
       <c r="B17" s="32" t="s">
         <v>56</v>
       </c>
@@ -24113,7 +23778,7 @@
       <c r="BN17" s="48"/>
       <c r="BO17" s="33"/>
     </row>
-    <row r="18" spans="2:67" ht="16" thickBot="1">
+    <row r="18" spans="2:67" ht="17" thickBot="1">
       <c r="B18" s="40" t="s">
         <v>57</v>
       </c>
@@ -25583,7 +25248,7 @@
       <c r="BN38" s="48"/>
       <c r="BO38" s="33"/>
     </row>
-    <row r="39" spans="2:67" ht="16" thickBot="1">
+    <row r="39" spans="2:67" ht="17" thickBot="1">
       <c r="B39" s="32" t="s">
         <v>78</v>
       </c>
@@ -25653,7 +25318,7 @@
       <c r="BN39" s="48"/>
       <c r="BO39" s="33"/>
     </row>
-    <row r="40" spans="2:67" ht="16" thickBot="1">
+    <row r="40" spans="2:67" ht="17" thickBot="1">
       <c r="B40" s="40" t="s">
         <v>79</v>
       </c>
@@ -26913,7 +26578,7 @@
       <c r="BN57" s="48"/>
       <c r="BO57" s="33"/>
     </row>
-    <row r="58" spans="2:67" ht="16" thickBot="1">
+    <row r="58" spans="2:67" ht="17" thickBot="1">
       <c r="B58" s="32" t="s">
         <v>88</v>
       </c>
@@ -26983,7 +26648,7 @@
       <c r="BN58" s="48"/>
       <c r="BO58" s="33"/>
     </row>
-    <row r="59" spans="2:67" ht="16" thickBot="1">
+    <row r="59" spans="2:67" ht="17" thickBot="1">
       <c r="B59" s="40" t="s">
         <v>89</v>
       </c>
@@ -27053,7 +26718,7 @@
       <c r="BN59" s="52"/>
       <c r="BO59" s="42"/>
     </row>
-    <row r="60" spans="2:67" ht="16" thickBot="1">
+    <row r="60" spans="2:67" ht="17" thickBot="1">
       <c r="B60" s="40" t="s">
         <v>46</v>
       </c>
@@ -27963,7 +27628,7 @@
       <c r="BN72" s="48"/>
       <c r="BO72" s="33"/>
     </row>
-    <row r="73" spans="2:67" ht="16" thickBot="1">
+    <row r="73" spans="2:67" ht="17" thickBot="1">
       <c r="B73" s="32" t="s">
         <v>102</v>
       </c>
@@ -28033,7 +27698,7 @@
       <c r="BN73" s="48"/>
       <c r="BO73" s="33"/>
     </row>
-    <row r="74" spans="2:67" ht="16" thickBot="1">
+    <row r="74" spans="2:67" ht="17" thickBot="1">
       <c r="B74" s="40" t="s">
         <v>103</v>
       </c>
@@ -28453,7 +28118,7 @@
       <c r="BN79" s="48"/>
       <c r="BO79" s="33"/>
     </row>
-    <row r="80" spans="2:67" ht="16" thickBot="1">
+    <row r="80" spans="2:67" ht="17" thickBot="1">
       <c r="B80" s="32" t="s">
         <v>109</v>
       </c>
@@ -28523,7 +28188,7 @@
       <c r="BN80" s="48"/>
       <c r="BO80" s="33"/>
     </row>
-    <row r="81" spans="2:67" ht="16" thickBot="1">
+    <row r="81" spans="2:67" ht="17" thickBot="1">
       <c r="B81" s="40" t="s">
         <v>110</v>
       </c>
@@ -28873,7 +28538,7 @@
       <c r="BN85" s="48"/>
       <c r="BO85" s="33"/>
     </row>
-    <row r="86" spans="2:67" ht="16" thickBot="1">
+    <row r="86" spans="2:67" ht="17" thickBot="1">
       <c r="B86" s="32" t="s">
         <v>115</v>
       </c>
@@ -28943,7 +28608,7 @@
       <c r="BN86" s="48"/>
       <c r="BO86" s="33"/>
     </row>
-    <row r="87" spans="2:67" ht="16" thickBot="1">
+    <row r="87" spans="2:67" ht="17" thickBot="1">
       <c r="B87" s="40" t="s">
         <v>116</v>
       </c>
@@ -29223,7 +28888,7 @@
       <c r="BN90" s="48"/>
       <c r="BO90" s="33"/>
     </row>
-    <row r="91" spans="2:67" ht="16" thickBot="1">
+    <row r="91" spans="2:67" ht="17" thickBot="1">
       <c r="B91" s="32" t="s">
         <v>120</v>
       </c>
@@ -29293,7 +28958,7 @@
       <c r="BN91" s="48"/>
       <c r="BO91" s="33"/>
     </row>
-    <row r="92" spans="2:67" ht="16" thickBot="1">
+    <row r="92" spans="2:67" ht="17" thickBot="1">
       <c r="B92" s="40" t="s">
         <v>121</v>
       </c>
@@ -29573,7 +29238,7 @@
       <c r="BN95" s="48"/>
       <c r="BO95" s="33"/>
     </row>
-    <row r="96" spans="2:67" ht="16" thickBot="1">
+    <row r="96" spans="2:67" ht="17" thickBot="1">
       <c r="B96" s="32" t="s">
         <v>125</v>
       </c>
@@ -29643,7 +29308,7 @@
       <c r="BN96" s="48"/>
       <c r="BO96" s="33"/>
     </row>
-    <row r="97" spans="2:67" ht="16" thickBot="1">
+    <row r="97" spans="2:67" ht="17" thickBot="1">
       <c r="B97" s="40" t="s">
         <v>126</v>
       </c>
@@ -29923,7 +29588,7 @@
       <c r="BN100" s="48"/>
       <c r="BO100" s="33"/>
     </row>
-    <row r="101" spans="2:67" ht="16" thickBot="1">
+    <row r="101" spans="2:67" ht="17" thickBot="1">
       <c r="B101" s="34" t="s">
         <v>130</v>
       </c>
@@ -30016,8 +29681,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A2:I51"/>
@@ -30026,7 +29691,7 @@
       <selection activeCell="B5" sqref="B5:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="9.6640625" style="2" customWidth="1"/>
     <col min="2" max="8" width="14" style="2" customWidth="1"/>
@@ -30034,7 +29699,7 @@
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="20">
+    <row r="2" spans="2:9" ht="21">
       <c r="B2" s="22" t="s">
         <v>255</v>
       </c>
@@ -30054,17 +29719,17 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1">
-      <c r="B5" s="363" t="s">
+      <c r="B5" s="353" t="s">
         <v>422</v>
       </c>
-      <c r="C5" s="364"/>
-      <c r="D5" s="364"/>
-      <c r="E5" s="364"/>
-      <c r="F5" s="364"/>
-      <c r="G5" s="364"/>
-      <c r="H5" s="365"/>
-    </row>
-    <row r="6" spans="2:9" ht="16" thickBot="1"/>
+      <c r="C5" s="354"/>
+      <c r="D5" s="354"/>
+      <c r="E5" s="354"/>
+      <c r="F5" s="354"/>
+      <c r="G5" s="354"/>
+      <c r="H5" s="355"/>
+    </row>
+    <row r="6" spans="2:9" ht="17" thickBot="1"/>
     <row r="7" spans="2:9">
       <c r="B7" s="55" t="s">
         <v>381</v>
@@ -30561,7 +30226,7 @@
       <c r="G50" s="290"/>
       <c r="H50" s="291"/>
     </row>
-    <row r="51" spans="2:8" ht="16" thickBot="1">
+    <row r="51" spans="2:8" ht="17" thickBot="1">
       <c r="B51" s="62"/>
       <c r="C51" s="75"/>
       <c r="D51" s="63"/>

</xml_diff>